<commit_message>
prediction process is completed
</commit_message>
<xml_diff>
--- a/data/dashboard_data/prediction_validation_logs.xlsx
+++ b/data/dashboard_data/prediction_validation_logs.xlsx
@@ -439,7 +439,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F61"/>
+  <dimension ref="A1:F121"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2287,6 +2287,1806 @@
         </is>
       </c>
     </row>
+    <row r="62">
+      <c r="A62" s="3" t="n">
+        <v>61</v>
+      </c>
+      <c r="B62" s="3" t="inlineStr">
+        <is>
+          <t>2024-09-21</t>
+        </is>
+      </c>
+      <c r="C62" s="3" t="inlineStr">
+        <is>
+          <t>wafer_07012024_041011.csv</t>
+        </is>
+      </c>
+      <c r="D62" s="3" t="inlineStr">
+        <is>
+          <t>Passed</t>
+        </is>
+      </c>
+      <c r="E62" s="3" t="inlineStr">
+        <is>
+          <t>FILE NAME VALIDATION</t>
+        </is>
+      </c>
+      <c r="F62" s="3" t="inlineStr">
+        <is>
+          <t>FILE NAME VALIDATION COMPLETED</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="3" t="n">
+        <v>62</v>
+      </c>
+      <c r="B63" s="3" t="inlineStr">
+        <is>
+          <t>2024-09-21</t>
+        </is>
+      </c>
+      <c r="C63" s="3" t="inlineStr">
+        <is>
+          <t>wafer_07012024_041011.csv</t>
+        </is>
+      </c>
+      <c r="D63" s="3" t="inlineStr">
+        <is>
+          <t>Passed</t>
+        </is>
+      </c>
+      <c r="E63" s="3" t="inlineStr">
+        <is>
+          <t>NUMBER OF COLUMNS VALIDATION</t>
+        </is>
+      </c>
+      <c r="F63" s="3" t="inlineStr">
+        <is>
+          <t>NUMBER OF COLUMNS VALIDATION COMPLETED</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="3" t="n">
+        <v>63</v>
+      </c>
+      <c r="B64" s="3" t="inlineStr">
+        <is>
+          <t>2024-09-21</t>
+        </is>
+      </c>
+      <c r="C64" s="3" t="inlineStr">
+        <is>
+          <t>wafer_07012024_041011.csv</t>
+        </is>
+      </c>
+      <c r="D64" s="3" t="inlineStr">
+        <is>
+          <t>Failed</t>
+        </is>
+      </c>
+      <c r="E64" s="3" t="inlineStr">
+        <is>
+          <t>COLUMNDATA_WHOLE_MISSING_VALIDATION</t>
+        </is>
+      </c>
+      <c r="F64" s="3" t="inlineStr">
+        <is>
+          <t>COLUMN DATA WHOLE MISSING VALIDATION FAILED, MISMATCH COLUMN LIST:[{'Sensor_Name': 'Sensor-86', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-110', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-111', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-112', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-221', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-245', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-246', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-247', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-359', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-383', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-384', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-385', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-493', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-517', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-518', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-519', 'Column_Data': [100, 0]}]</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" s="3" t="n">
+        <v>64</v>
+      </c>
+      <c r="B65" s="3" t="inlineStr">
+        <is>
+          <t>2024-09-21</t>
+        </is>
+      </c>
+      <c r="C65" s="3" t="inlineStr">
+        <is>
+          <t>wafer_13012024_090817.csv</t>
+        </is>
+      </c>
+      <c r="D65" s="3" t="inlineStr">
+        <is>
+          <t>Passed</t>
+        </is>
+      </c>
+      <c r="E65" s="3" t="inlineStr">
+        <is>
+          <t>FILE NAME VALIDATION</t>
+        </is>
+      </c>
+      <c r="F65" s="3" t="inlineStr">
+        <is>
+          <t>FILE NAME VALIDATION COMPLETED</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="3" t="n">
+        <v>65</v>
+      </c>
+      <c r="B66" s="3" t="inlineStr">
+        <is>
+          <t>2024-09-21</t>
+        </is>
+      </c>
+      <c r="C66" s="3" t="inlineStr">
+        <is>
+          <t>wafer_13012024_090817.csv</t>
+        </is>
+      </c>
+      <c r="D66" s="3" t="inlineStr">
+        <is>
+          <t>Passed</t>
+        </is>
+      </c>
+      <c r="E66" s="3" t="inlineStr">
+        <is>
+          <t>NUMBER OF COLUMNS VALIDATION</t>
+        </is>
+      </c>
+      <c r="F66" s="3" t="inlineStr">
+        <is>
+          <t>NUMBER OF COLUMNS VALIDATION COMPLETED</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" s="3" t="n">
+        <v>66</v>
+      </c>
+      <c r="B67" s="3" t="inlineStr">
+        <is>
+          <t>2024-09-21</t>
+        </is>
+      </c>
+      <c r="C67" s="3" t="inlineStr">
+        <is>
+          <t>wafer_13012024_090817.csv</t>
+        </is>
+      </c>
+      <c r="D67" s="3" t="inlineStr">
+        <is>
+          <t>Passed</t>
+        </is>
+      </c>
+      <c r="E67" s="3" t="inlineStr">
+        <is>
+          <t>COLUMNDATA_WHOLE_MISSING_VALIDATION</t>
+        </is>
+      </c>
+      <c r="F67" s="3" t="inlineStr">
+        <is>
+          <t>COLUMN DATA WHOLE MISSING VALIDATION COMPLETED</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" s="3" t="n">
+        <v>67</v>
+      </c>
+      <c r="B68" s="3" t="inlineStr">
+        <is>
+          <t>2024-09-21</t>
+        </is>
+      </c>
+      <c r="C68" s="3" t="inlineStr">
+        <is>
+          <t>wafer_13012024_090817.csv</t>
+        </is>
+      </c>
+      <c r="D68" s="3" t="inlineStr">
+        <is>
+          <t>Passed</t>
+        </is>
+      </c>
+      <c r="E68" s="3" t="inlineStr">
+        <is>
+          <t>COLUMN DATA VALIDATION</t>
+        </is>
+      </c>
+      <c r="F68" s="3" t="inlineStr">
+        <is>
+          <t>COLUMN DATA VALIDATION COMPLETED</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" s="3" t="n">
+        <v>68</v>
+      </c>
+      <c r="B69" s="3" t="inlineStr">
+        <is>
+          <t>2024-09-21</t>
+        </is>
+      </c>
+      <c r="C69" s="3" t="inlineStr">
+        <is>
+          <t>Wafer_13012024_141000.csv</t>
+        </is>
+      </c>
+      <c r="D69" s="3" t="inlineStr">
+        <is>
+          <t>Failed</t>
+        </is>
+      </c>
+      <c r="E69" s="3" t="inlineStr">
+        <is>
+          <t>FILE NAME VALIDATION</t>
+        </is>
+      </c>
+      <c r="F69" s="3" t="inlineStr">
+        <is>
+          <t>FILE NAME VALIDATION FAILED</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" s="3" t="n">
+        <v>69</v>
+      </c>
+      <c r="B70" s="3" t="inlineStr">
+        <is>
+          <t>2024-09-21</t>
+        </is>
+      </c>
+      <c r="C70" s="3" t="inlineStr">
+        <is>
+          <t>Wafer_14012024_113045.csv</t>
+        </is>
+      </c>
+      <c r="D70" s="3" t="inlineStr">
+        <is>
+          <t>Failed</t>
+        </is>
+      </c>
+      <c r="E70" s="3" t="inlineStr">
+        <is>
+          <t>FILE NAME VALIDATION</t>
+        </is>
+      </c>
+      <c r="F70" s="3" t="inlineStr">
+        <is>
+          <t>FILE NAME VALIDATION FAILED</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" s="3" t="n">
+        <v>70</v>
+      </c>
+      <c r="B71" s="3" t="inlineStr">
+        <is>
+          <t>2024-09-21</t>
+        </is>
+      </c>
+      <c r="C71" s="3" t="inlineStr">
+        <is>
+          <t>Wafer_15010_130532.csv</t>
+        </is>
+      </c>
+      <c r="D71" s="3" t="inlineStr">
+        <is>
+          <t>Failed</t>
+        </is>
+      </c>
+      <c r="E71" s="3" t="inlineStr">
+        <is>
+          <t>FILE NAME VALIDATION</t>
+        </is>
+      </c>
+      <c r="F71" s="3" t="inlineStr">
+        <is>
+          <t>FILE NAME VALIDATION FAILED</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" s="3" t="n">
+        <v>71</v>
+      </c>
+      <c r="B72" s="3" t="inlineStr">
+        <is>
+          <t>2024-09-21</t>
+        </is>
+      </c>
+      <c r="C72" s="3" t="inlineStr">
+        <is>
+          <t>wafer_16012024_051629.csv</t>
+        </is>
+      </c>
+      <c r="D72" s="3" t="inlineStr">
+        <is>
+          <t>Passed</t>
+        </is>
+      </c>
+      <c r="E72" s="3" t="inlineStr">
+        <is>
+          <t>FILE NAME VALIDATION</t>
+        </is>
+      </c>
+      <c r="F72" s="3" t="inlineStr">
+        <is>
+          <t>FILE NAME VALIDATION COMPLETED</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" s="3" t="n">
+        <v>72</v>
+      </c>
+      <c r="B73" s="3" t="inlineStr">
+        <is>
+          <t>2024-09-21</t>
+        </is>
+      </c>
+      <c r="C73" s="3" t="inlineStr">
+        <is>
+          <t>wafer_16012024_051629.csv</t>
+        </is>
+      </c>
+      <c r="D73" s="3" t="inlineStr">
+        <is>
+          <t>Passed</t>
+        </is>
+      </c>
+      <c r="E73" s="3" t="inlineStr">
+        <is>
+          <t>NUMBER OF COLUMNS VALIDATION</t>
+        </is>
+      </c>
+      <c r="F73" s="3" t="inlineStr">
+        <is>
+          <t>NUMBER OF COLUMNS VALIDATION COMPLETED</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" s="3" t="n">
+        <v>73</v>
+      </c>
+      <c r="B74" s="3" t="inlineStr">
+        <is>
+          <t>2024-09-21</t>
+        </is>
+      </c>
+      <c r="C74" s="3" t="inlineStr">
+        <is>
+          <t>wafer_16012024_051629.csv</t>
+        </is>
+      </c>
+      <c r="D74" s="3" t="inlineStr">
+        <is>
+          <t>Passed</t>
+        </is>
+      </c>
+      <c r="E74" s="3" t="inlineStr">
+        <is>
+          <t>COLUMNDATA_WHOLE_MISSING_VALIDATION</t>
+        </is>
+      </c>
+      <c r="F74" s="3" t="inlineStr">
+        <is>
+          <t>COLUMN DATA WHOLE MISSING VALIDATION COMPLETED</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" s="3" t="n">
+        <v>74</v>
+      </c>
+      <c r="B75" s="3" t="inlineStr">
+        <is>
+          <t>2024-09-21</t>
+        </is>
+      </c>
+      <c r="C75" s="3" t="inlineStr">
+        <is>
+          <t>wafer_16012024_051629.csv</t>
+        </is>
+      </c>
+      <c r="D75" s="3" t="inlineStr">
+        <is>
+          <t>Passed</t>
+        </is>
+      </c>
+      <c r="E75" s="3" t="inlineStr">
+        <is>
+          <t>COLUMN DATA VALIDATION</t>
+        </is>
+      </c>
+      <c r="F75" s="3" t="inlineStr">
+        <is>
+          <t>COLUMN DATA VALIDATION COMPLETED</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" s="3" t="n">
+        <v>75</v>
+      </c>
+      <c r="B76" s="3" t="inlineStr">
+        <is>
+          <t>2024-09-21</t>
+        </is>
+      </c>
+      <c r="C76" s="3" t="inlineStr">
+        <is>
+          <t>wafer_20012024_090819.csv</t>
+        </is>
+      </c>
+      <c r="D76" s="3" t="inlineStr">
+        <is>
+          <t>Passed</t>
+        </is>
+      </c>
+      <c r="E76" s="3" t="inlineStr">
+        <is>
+          <t>FILE NAME VALIDATION</t>
+        </is>
+      </c>
+      <c r="F76" s="3" t="inlineStr">
+        <is>
+          <t>FILE NAME VALIDATION COMPLETED</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" s="3" t="n">
+        <v>76</v>
+      </c>
+      <c r="B77" s="3" t="inlineStr">
+        <is>
+          <t>2024-09-21</t>
+        </is>
+      </c>
+      <c r="C77" s="3" t="inlineStr">
+        <is>
+          <t>wafer_20012024_090819.csv</t>
+        </is>
+      </c>
+      <c r="D77" s="3" t="inlineStr">
+        <is>
+          <t>Passed</t>
+        </is>
+      </c>
+      <c r="E77" s="3" t="inlineStr">
+        <is>
+          <t>NUMBER OF COLUMNS VALIDATION</t>
+        </is>
+      </c>
+      <c r="F77" s="3" t="inlineStr">
+        <is>
+          <t>NUMBER OF COLUMNS VALIDATION COMPLETED</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" s="3" t="n">
+        <v>77</v>
+      </c>
+      <c r="B78" s="3" t="inlineStr">
+        <is>
+          <t>2024-09-21</t>
+        </is>
+      </c>
+      <c r="C78" s="3" t="inlineStr">
+        <is>
+          <t>wafer_20012024_090819.csv</t>
+        </is>
+      </c>
+      <c r="D78" s="3" t="inlineStr">
+        <is>
+          <t>Failed</t>
+        </is>
+      </c>
+      <c r="E78" s="3" t="inlineStr">
+        <is>
+          <t>COLUMNDATA_WHOLE_MISSING_VALIDATION</t>
+        </is>
+      </c>
+      <c r="F78" s="3" t="inlineStr">
+        <is>
+          <t>COLUMN DATA WHOLE MISSING VALIDATION FAILED, MISMATCH COLUMN LIST:[{'Sensor_Name': 'Sensor-86', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-110', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-111', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-112', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-221', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-245', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-246', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-247', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-359', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-383', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-384', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-385', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-493', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-517', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-518', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-519', 'Column_Data': [100, 0]}]</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" s="3" t="n">
+        <v>78</v>
+      </c>
+      <c r="B79" s="3" t="inlineStr">
+        <is>
+          <t>2024-09-21</t>
+        </is>
+      </c>
+      <c r="C79" s="3" t="inlineStr">
+        <is>
+          <t>wafer_20022024_090716.csv</t>
+        </is>
+      </c>
+      <c r="D79" s="3" t="inlineStr">
+        <is>
+          <t>Passed</t>
+        </is>
+      </c>
+      <c r="E79" s="3" t="inlineStr">
+        <is>
+          <t>FILE NAME VALIDATION</t>
+        </is>
+      </c>
+      <c r="F79" s="3" t="inlineStr">
+        <is>
+          <t>FILE NAME VALIDATION COMPLETED</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" s="3" t="n">
+        <v>79</v>
+      </c>
+      <c r="B80" s="3" t="inlineStr">
+        <is>
+          <t>2024-09-21</t>
+        </is>
+      </c>
+      <c r="C80" s="3" t="inlineStr">
+        <is>
+          <t>wafer_20022024_090716.csv</t>
+        </is>
+      </c>
+      <c r="D80" s="3" t="inlineStr">
+        <is>
+          <t>Passed</t>
+        </is>
+      </c>
+      <c r="E80" s="3" t="inlineStr">
+        <is>
+          <t>NUMBER OF COLUMNS VALIDATION</t>
+        </is>
+      </c>
+      <c r="F80" s="3" t="inlineStr">
+        <is>
+          <t>NUMBER OF COLUMNS VALIDATION COMPLETED</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" s="3" t="n">
+        <v>80</v>
+      </c>
+      <c r="B81" s="3" t="inlineStr">
+        <is>
+          <t>2024-09-21</t>
+        </is>
+      </c>
+      <c r="C81" s="3" t="inlineStr">
+        <is>
+          <t>wafer_20022024_090716.csv</t>
+        </is>
+      </c>
+      <c r="D81" s="3" t="inlineStr">
+        <is>
+          <t>Passed</t>
+        </is>
+      </c>
+      <c r="E81" s="3" t="inlineStr">
+        <is>
+          <t>COLUMNDATA_WHOLE_MISSING_VALIDATION</t>
+        </is>
+      </c>
+      <c r="F81" s="3" t="inlineStr">
+        <is>
+          <t>COLUMN DATA WHOLE MISSING VALIDATION COMPLETED</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" s="3" t="n">
+        <v>81</v>
+      </c>
+      <c r="B82" s="3" t="inlineStr">
+        <is>
+          <t>2024-09-21</t>
+        </is>
+      </c>
+      <c r="C82" s="3" t="inlineStr">
+        <is>
+          <t>wafer_20022024_090716.csv</t>
+        </is>
+      </c>
+      <c r="D82" s="3" t="inlineStr">
+        <is>
+          <t>Passed</t>
+        </is>
+      </c>
+      <c r="E82" s="3" t="inlineStr">
+        <is>
+          <t>COLUMN DATA VALIDATION</t>
+        </is>
+      </c>
+      <c r="F82" s="3" t="inlineStr">
+        <is>
+          <t>COLUMN DATA VALIDATION COMPLETED</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" s="3" t="n">
+        <v>82</v>
+      </c>
+      <c r="B83" s="3" t="inlineStr">
+        <is>
+          <t>2024-09-21</t>
+        </is>
+      </c>
+      <c r="C83" s="3" t="inlineStr">
+        <is>
+          <t>wafer_21012024_080913.csv</t>
+        </is>
+      </c>
+      <c r="D83" s="3" t="inlineStr">
+        <is>
+          <t>Passed</t>
+        </is>
+      </c>
+      <c r="E83" s="3" t="inlineStr">
+        <is>
+          <t>FILE NAME VALIDATION</t>
+        </is>
+      </c>
+      <c r="F83" s="3" t="inlineStr">
+        <is>
+          <t>FILE NAME VALIDATION COMPLETED</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" s="3" t="n">
+        <v>83</v>
+      </c>
+      <c r="B84" s="3" t="inlineStr">
+        <is>
+          <t>2024-09-21</t>
+        </is>
+      </c>
+      <c r="C84" s="3" t="inlineStr">
+        <is>
+          <t>wafer_21012024_080913.csv</t>
+        </is>
+      </c>
+      <c r="D84" s="3" t="inlineStr">
+        <is>
+          <t>Passed</t>
+        </is>
+      </c>
+      <c r="E84" s="3" t="inlineStr">
+        <is>
+          <t>NUMBER OF COLUMNS VALIDATION</t>
+        </is>
+      </c>
+      <c r="F84" s="3" t="inlineStr">
+        <is>
+          <t>NUMBER OF COLUMNS VALIDATION COMPLETED</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" s="3" t="n">
+        <v>84</v>
+      </c>
+      <c r="B85" s="3" t="inlineStr">
+        <is>
+          <t>2024-09-21</t>
+        </is>
+      </c>
+      <c r="C85" s="3" t="inlineStr">
+        <is>
+          <t>wafer_21012024_080913.csv</t>
+        </is>
+      </c>
+      <c r="D85" s="3" t="inlineStr">
+        <is>
+          <t>Passed</t>
+        </is>
+      </c>
+      <c r="E85" s="3" t="inlineStr">
+        <is>
+          <t>COLUMNDATA_WHOLE_MISSING_VALIDATION</t>
+        </is>
+      </c>
+      <c r="F85" s="3" t="inlineStr">
+        <is>
+          <t>COLUMN DATA WHOLE MISSING VALIDATION COMPLETED</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" s="3" t="n">
+        <v>85</v>
+      </c>
+      <c r="B86" s="3" t="inlineStr">
+        <is>
+          <t>2024-09-21</t>
+        </is>
+      </c>
+      <c r="C86" s="3" t="inlineStr">
+        <is>
+          <t>wafer_21012024_080913.csv</t>
+        </is>
+      </c>
+      <c r="D86" s="3" t="inlineStr">
+        <is>
+          <t>Passed</t>
+        </is>
+      </c>
+      <c r="E86" s="3" t="inlineStr">
+        <is>
+          <t>COLUMN DATA VALIDATION</t>
+        </is>
+      </c>
+      <c r="F86" s="3" t="inlineStr">
+        <is>
+          <t>COLUMN DATA VALIDATION COMPLETED</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" s="3" t="n">
+        <v>86</v>
+      </c>
+      <c r="B87" s="3" t="inlineStr">
+        <is>
+          <t>2024-09-21</t>
+        </is>
+      </c>
+      <c r="C87" s="3" t="inlineStr">
+        <is>
+          <t>wafer_22022024_041119.csv</t>
+        </is>
+      </c>
+      <c r="D87" s="3" t="inlineStr">
+        <is>
+          <t>Passed</t>
+        </is>
+      </c>
+      <c r="E87" s="3" t="inlineStr">
+        <is>
+          <t>FILE NAME VALIDATION</t>
+        </is>
+      </c>
+      <c r="F87" s="3" t="inlineStr">
+        <is>
+          <t>FILE NAME VALIDATION COMPLETED</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" s="3" t="n">
+        <v>87</v>
+      </c>
+      <c r="B88" s="3" t="inlineStr">
+        <is>
+          <t>2024-09-21</t>
+        </is>
+      </c>
+      <c r="C88" s="3" t="inlineStr">
+        <is>
+          <t>wafer_22022024_041119.csv</t>
+        </is>
+      </c>
+      <c r="D88" s="3" t="inlineStr">
+        <is>
+          <t>Passed</t>
+        </is>
+      </c>
+      <c r="E88" s="3" t="inlineStr">
+        <is>
+          <t>NUMBER OF COLUMNS VALIDATION</t>
+        </is>
+      </c>
+      <c r="F88" s="3" t="inlineStr">
+        <is>
+          <t>NUMBER OF COLUMNS VALIDATION COMPLETED</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" s="3" t="n">
+        <v>88</v>
+      </c>
+      <c r="B89" s="3" t="inlineStr">
+        <is>
+          <t>2024-09-21</t>
+        </is>
+      </c>
+      <c r="C89" s="3" t="inlineStr">
+        <is>
+          <t>wafer_22022024_041119.csv</t>
+        </is>
+      </c>
+      <c r="D89" s="3" t="inlineStr">
+        <is>
+          <t>Failed</t>
+        </is>
+      </c>
+      <c r="E89" s="3" t="inlineStr">
+        <is>
+          <t>COLUMNDATA_WHOLE_MISSING_VALIDATION</t>
+        </is>
+      </c>
+      <c r="F89" s="3" t="inlineStr">
+        <is>
+          <t>COLUMN DATA WHOLE MISSING VALIDATION FAILED, MISMATCH COLUMN LIST:[{'Sensor_Name': 'Sensor-86', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-110', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-111', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-112', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-221', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-245', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-246', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-247', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-359', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-383', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-384', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-385', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-493', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-517', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-518', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-519', 'Column_Data': [100, 0]}]</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" s="3" t="n">
+        <v>89</v>
+      </c>
+      <c r="B90" s="3" t="inlineStr">
+        <is>
+          <t>2024-09-21</t>
+        </is>
+      </c>
+      <c r="C90" s="3" t="inlineStr">
+        <is>
+          <t>wafer_23012024_011008.csv</t>
+        </is>
+      </c>
+      <c r="D90" s="3" t="inlineStr">
+        <is>
+          <t>Passed</t>
+        </is>
+      </c>
+      <c r="E90" s="3" t="inlineStr">
+        <is>
+          <t>FILE NAME VALIDATION</t>
+        </is>
+      </c>
+      <c r="F90" s="3" t="inlineStr">
+        <is>
+          <t>FILE NAME VALIDATION COMPLETED</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" s="3" t="n">
+        <v>90</v>
+      </c>
+      <c r="B91" s="3" t="inlineStr">
+        <is>
+          <t>2024-09-21</t>
+        </is>
+      </c>
+      <c r="C91" s="3" t="inlineStr">
+        <is>
+          <t>wafer_23012024_011008.csv</t>
+        </is>
+      </c>
+      <c r="D91" s="3" t="inlineStr">
+        <is>
+          <t>Passed</t>
+        </is>
+      </c>
+      <c r="E91" s="3" t="inlineStr">
+        <is>
+          <t>NUMBER OF COLUMNS VALIDATION</t>
+        </is>
+      </c>
+      <c r="F91" s="3" t="inlineStr">
+        <is>
+          <t>NUMBER OF COLUMNS VALIDATION COMPLETED</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" s="3" t="n">
+        <v>91</v>
+      </c>
+      <c r="B92" s="3" t="inlineStr">
+        <is>
+          <t>2024-09-21</t>
+        </is>
+      </c>
+      <c r="C92" s="3" t="inlineStr">
+        <is>
+          <t>wafer_23012024_011008.csv</t>
+        </is>
+      </c>
+      <c r="D92" s="3" t="inlineStr">
+        <is>
+          <t>Failed</t>
+        </is>
+      </c>
+      <c r="E92" s="3" t="inlineStr">
+        <is>
+          <t>COLUMNDATA_WHOLE_MISSING_VALIDATION</t>
+        </is>
+      </c>
+      <c r="F92" s="3" t="inlineStr">
+        <is>
+          <t>COLUMN DATA WHOLE MISSING VALIDATION FAILED, MISMATCH COLUMN LIST:[{'Sensor_Name': 'Sensor-86', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-110', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-111', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-112', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-221', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-245', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-246', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-247', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-359', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-383', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-384', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-385', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-493', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-517', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-518', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-519', 'Column_Data': [100, 0]}]</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" s="3" t="n">
+        <v>92</v>
+      </c>
+      <c r="B93" s="3" t="inlineStr">
+        <is>
+          <t>2024-09-21</t>
+        </is>
+      </c>
+      <c r="C93" s="3" t="inlineStr">
+        <is>
+          <t>wafer_23012024_041211.csv</t>
+        </is>
+      </c>
+      <c r="D93" s="3" t="inlineStr">
+        <is>
+          <t>Passed</t>
+        </is>
+      </c>
+      <c r="E93" s="3" t="inlineStr">
+        <is>
+          <t>FILE NAME VALIDATION</t>
+        </is>
+      </c>
+      <c r="F93" s="3" t="inlineStr">
+        <is>
+          <t>FILE NAME VALIDATION COMPLETED</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" s="3" t="n">
+        <v>93</v>
+      </c>
+      <c r="B94" s="3" t="inlineStr">
+        <is>
+          <t>2024-09-21</t>
+        </is>
+      </c>
+      <c r="C94" s="3" t="inlineStr">
+        <is>
+          <t>wafer_23012024_041211.csv</t>
+        </is>
+      </c>
+      <c r="D94" s="3" t="inlineStr">
+        <is>
+          <t>Passed</t>
+        </is>
+      </c>
+      <c r="E94" s="3" t="inlineStr">
+        <is>
+          <t>NUMBER OF COLUMNS VALIDATION</t>
+        </is>
+      </c>
+      <c r="F94" s="3" t="inlineStr">
+        <is>
+          <t>NUMBER OF COLUMNS VALIDATION COMPLETED</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" s="3" t="n">
+        <v>94</v>
+      </c>
+      <c r="B95" s="3" t="inlineStr">
+        <is>
+          <t>2024-09-21</t>
+        </is>
+      </c>
+      <c r="C95" s="3" t="inlineStr">
+        <is>
+          <t>wafer_23012024_041211.csv</t>
+        </is>
+      </c>
+      <c r="D95" s="3" t="inlineStr">
+        <is>
+          <t>Passed</t>
+        </is>
+      </c>
+      <c r="E95" s="3" t="inlineStr">
+        <is>
+          <t>COLUMNDATA_WHOLE_MISSING_VALIDATION</t>
+        </is>
+      </c>
+      <c r="F95" s="3" t="inlineStr">
+        <is>
+          <t>COLUMN DATA WHOLE MISSING VALIDATION COMPLETED</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" s="3" t="n">
+        <v>95</v>
+      </c>
+      <c r="B96" s="3" t="inlineStr">
+        <is>
+          <t>2024-09-21</t>
+        </is>
+      </c>
+      <c r="C96" s="3" t="inlineStr">
+        <is>
+          <t>wafer_23012024_041211.csv</t>
+        </is>
+      </c>
+      <c r="D96" s="3" t="inlineStr">
+        <is>
+          <t>Passed</t>
+        </is>
+      </c>
+      <c r="E96" s="3" t="inlineStr">
+        <is>
+          <t>COLUMN DATA VALIDATION</t>
+        </is>
+      </c>
+      <c r="F96" s="3" t="inlineStr">
+        <is>
+          <t>COLUMN DATA VALIDATION COMPLETED</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" s="3" t="n">
+        <v>96</v>
+      </c>
+      <c r="B97" s="3" t="inlineStr">
+        <is>
+          <t>2024-09-21</t>
+        </is>
+      </c>
+      <c r="C97" s="3" t="inlineStr">
+        <is>
+          <t>wafer_27012024_080911.csv</t>
+        </is>
+      </c>
+      <c r="D97" s="3" t="inlineStr">
+        <is>
+          <t>Passed</t>
+        </is>
+      </c>
+      <c r="E97" s="3" t="inlineStr">
+        <is>
+          <t>FILE NAME VALIDATION</t>
+        </is>
+      </c>
+      <c r="F97" s="3" t="inlineStr">
+        <is>
+          <t>FILE NAME VALIDATION COMPLETED</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" s="3" t="n">
+        <v>97</v>
+      </c>
+      <c r="B98" s="3" t="inlineStr">
+        <is>
+          <t>2024-09-21</t>
+        </is>
+      </c>
+      <c r="C98" s="3" t="inlineStr">
+        <is>
+          <t>wafer_27012024_080911.csv</t>
+        </is>
+      </c>
+      <c r="D98" s="3" t="inlineStr">
+        <is>
+          <t>Passed</t>
+        </is>
+      </c>
+      <c r="E98" s="3" t="inlineStr">
+        <is>
+          <t>NUMBER OF COLUMNS VALIDATION</t>
+        </is>
+      </c>
+      <c r="F98" s="3" t="inlineStr">
+        <is>
+          <t>NUMBER OF COLUMNS VALIDATION COMPLETED</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" s="3" t="n">
+        <v>98</v>
+      </c>
+      <c r="B99" s="3" t="inlineStr">
+        <is>
+          <t>2024-09-21</t>
+        </is>
+      </c>
+      <c r="C99" s="3" t="inlineStr">
+        <is>
+          <t>wafer_27012024_080911.csv</t>
+        </is>
+      </c>
+      <c r="D99" s="3" t="inlineStr">
+        <is>
+          <t>Passed</t>
+        </is>
+      </c>
+      <c r="E99" s="3" t="inlineStr">
+        <is>
+          <t>COLUMNDATA_WHOLE_MISSING_VALIDATION</t>
+        </is>
+      </c>
+      <c r="F99" s="3" t="inlineStr">
+        <is>
+          <t>COLUMN DATA WHOLE MISSING VALIDATION COMPLETED</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" s="3" t="n">
+        <v>99</v>
+      </c>
+      <c r="B100" s="3" t="inlineStr">
+        <is>
+          <t>2024-09-21</t>
+        </is>
+      </c>
+      <c r="C100" s="3" t="inlineStr">
+        <is>
+          <t>wafer_27012024_080911.csv</t>
+        </is>
+      </c>
+      <c r="D100" s="3" t="inlineStr">
+        <is>
+          <t>Passed</t>
+        </is>
+      </c>
+      <c r="E100" s="3" t="inlineStr">
+        <is>
+          <t>COLUMN DATA VALIDATION</t>
+        </is>
+      </c>
+      <c r="F100" s="3" t="inlineStr">
+        <is>
+          <t>COLUMN DATA VALIDATION COMPLETED</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" s="3" t="n">
+        <v>100</v>
+      </c>
+      <c r="B101" s="3" t="inlineStr">
+        <is>
+          <t>2024-09-21</t>
+        </is>
+      </c>
+      <c r="C101" s="3" t="inlineStr">
+        <is>
+          <t>wafer_28012024_051011.csv</t>
+        </is>
+      </c>
+      <c r="D101" s="3" t="inlineStr">
+        <is>
+          <t>Passed</t>
+        </is>
+      </c>
+      <c r="E101" s="3" t="inlineStr">
+        <is>
+          <t>FILE NAME VALIDATION</t>
+        </is>
+      </c>
+      <c r="F101" s="3" t="inlineStr">
+        <is>
+          <t>FILE NAME VALIDATION COMPLETED</t>
+        </is>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" s="3" t="n">
+        <v>101</v>
+      </c>
+      <c r="B102" s="3" t="inlineStr">
+        <is>
+          <t>2024-09-21</t>
+        </is>
+      </c>
+      <c r="C102" s="3" t="inlineStr">
+        <is>
+          <t>wafer_28012024_051011.csv</t>
+        </is>
+      </c>
+      <c r="D102" s="3" t="inlineStr">
+        <is>
+          <t>Passed</t>
+        </is>
+      </c>
+      <c r="E102" s="3" t="inlineStr">
+        <is>
+          <t>NUMBER OF COLUMNS VALIDATION</t>
+        </is>
+      </c>
+      <c r="F102" s="3" t="inlineStr">
+        <is>
+          <t>NUMBER OF COLUMNS VALIDATION COMPLETED</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" s="3" t="n">
+        <v>102</v>
+      </c>
+      <c r="B103" s="3" t="inlineStr">
+        <is>
+          <t>2024-09-21</t>
+        </is>
+      </c>
+      <c r="C103" s="3" t="inlineStr">
+        <is>
+          <t>wafer_28012024_051011.csv</t>
+        </is>
+      </c>
+      <c r="D103" s="3" t="inlineStr">
+        <is>
+          <t>Failed</t>
+        </is>
+      </c>
+      <c r="E103" s="3" t="inlineStr">
+        <is>
+          <t>COLUMNDATA_WHOLE_MISSING_VALIDATION</t>
+        </is>
+      </c>
+      <c r="F103" s="3" t="inlineStr">
+        <is>
+          <t>COLUMN DATA WHOLE MISSING VALIDATION FAILED, MISMATCH COLUMN LIST:[{'Sensor_Name': 'Sensor-86', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-110', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-111', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-112', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-221', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-245', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-246', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-247', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-359', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-383', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-384', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-385', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-493', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-517', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-518', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-519', 'Column_Data': [100, 0]}]</t>
+        </is>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" s="3" t="n">
+        <v>103</v>
+      </c>
+      <c r="B104" s="3" t="inlineStr">
+        <is>
+          <t>2024-09-21</t>
+        </is>
+      </c>
+      <c r="C104" s="3" t="inlineStr">
+        <is>
+          <t>wafer_28012024_090817.csv</t>
+        </is>
+      </c>
+      <c r="D104" s="3" t="inlineStr">
+        <is>
+          <t>Passed</t>
+        </is>
+      </c>
+      <c r="E104" s="3" t="inlineStr">
+        <is>
+          <t>FILE NAME VALIDATION</t>
+        </is>
+      </c>
+      <c r="F104" s="3" t="inlineStr">
+        <is>
+          <t>FILE NAME VALIDATION COMPLETED</t>
+        </is>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" s="3" t="n">
+        <v>104</v>
+      </c>
+      <c r="B105" s="3" t="inlineStr">
+        <is>
+          <t>2024-09-21</t>
+        </is>
+      </c>
+      <c r="C105" s="3" t="inlineStr">
+        <is>
+          <t>wafer_28012024_090817.csv</t>
+        </is>
+      </c>
+      <c r="D105" s="3" t="inlineStr">
+        <is>
+          <t>Passed</t>
+        </is>
+      </c>
+      <c r="E105" s="3" t="inlineStr">
+        <is>
+          <t>NUMBER OF COLUMNS VALIDATION</t>
+        </is>
+      </c>
+      <c r="F105" s="3" t="inlineStr">
+        <is>
+          <t>NUMBER OF COLUMNS VALIDATION COMPLETED</t>
+        </is>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" s="3" t="n">
+        <v>105</v>
+      </c>
+      <c r="B106" s="3" t="inlineStr">
+        <is>
+          <t>2024-09-21</t>
+        </is>
+      </c>
+      <c r="C106" s="3" t="inlineStr">
+        <is>
+          <t>wafer_28012024_090817.csv</t>
+        </is>
+      </c>
+      <c r="D106" s="3" t="inlineStr">
+        <is>
+          <t>Passed</t>
+        </is>
+      </c>
+      <c r="E106" s="3" t="inlineStr">
+        <is>
+          <t>COLUMNDATA_WHOLE_MISSING_VALIDATION</t>
+        </is>
+      </c>
+      <c r="F106" s="3" t="inlineStr">
+        <is>
+          <t>COLUMN DATA WHOLE MISSING VALIDATION COMPLETED</t>
+        </is>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" s="3" t="n">
+        <v>106</v>
+      </c>
+      <c r="B107" s="3" t="inlineStr">
+        <is>
+          <t>2024-09-21</t>
+        </is>
+      </c>
+      <c r="C107" s="3" t="inlineStr">
+        <is>
+          <t>wafer_28012024_090817.csv</t>
+        </is>
+      </c>
+      <c r="D107" s="3" t="inlineStr">
+        <is>
+          <t>Passed</t>
+        </is>
+      </c>
+      <c r="E107" s="3" t="inlineStr">
+        <is>
+          <t>COLUMN DATA VALIDATION</t>
+        </is>
+      </c>
+      <c r="F107" s="3" t="inlineStr">
+        <is>
+          <t>COLUMN DATA VALIDATION COMPLETED</t>
+        </is>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" s="3" t="n">
+        <v>107</v>
+      </c>
+      <c r="B108" s="3" t="inlineStr">
+        <is>
+          <t>2024-09-21</t>
+        </is>
+      </c>
+      <c r="C108" s="3" t="inlineStr">
+        <is>
+          <t>wafer_28042024_031911.csv</t>
+        </is>
+      </c>
+      <c r="D108" s="3" t="inlineStr">
+        <is>
+          <t>Passed</t>
+        </is>
+      </c>
+      <c r="E108" s="3" t="inlineStr">
+        <is>
+          <t>FILE NAME VALIDATION</t>
+        </is>
+      </c>
+      <c r="F108" s="3" t="inlineStr">
+        <is>
+          <t>FILE NAME VALIDATION COMPLETED</t>
+        </is>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" s="3" t="n">
+        <v>108</v>
+      </c>
+      <c r="B109" s="3" t="inlineStr">
+        <is>
+          <t>2024-09-21</t>
+        </is>
+      </c>
+      <c r="C109" s="3" t="inlineStr">
+        <is>
+          <t>wafer_28042024_031911.csv</t>
+        </is>
+      </c>
+      <c r="D109" s="3" t="inlineStr">
+        <is>
+          <t>Passed</t>
+        </is>
+      </c>
+      <c r="E109" s="3" t="inlineStr">
+        <is>
+          <t>NUMBER OF COLUMNS VALIDATION</t>
+        </is>
+      </c>
+      <c r="F109" s="3" t="inlineStr">
+        <is>
+          <t>NUMBER OF COLUMNS VALIDATION COMPLETED</t>
+        </is>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" s="3" t="n">
+        <v>109</v>
+      </c>
+      <c r="B110" s="3" t="inlineStr">
+        <is>
+          <t>2024-09-21</t>
+        </is>
+      </c>
+      <c r="C110" s="3" t="inlineStr">
+        <is>
+          <t>wafer_28042024_031911.csv</t>
+        </is>
+      </c>
+      <c r="D110" s="3" t="inlineStr">
+        <is>
+          <t>Passed</t>
+        </is>
+      </c>
+      <c r="E110" s="3" t="inlineStr">
+        <is>
+          <t>COLUMNDATA_WHOLE_MISSING_VALIDATION</t>
+        </is>
+      </c>
+      <c r="F110" s="3" t="inlineStr">
+        <is>
+          <t>COLUMN DATA WHOLE MISSING VALIDATION COMPLETED</t>
+        </is>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" s="3" t="n">
+        <v>110</v>
+      </c>
+      <c r="B111" s="3" t="inlineStr">
+        <is>
+          <t>2024-09-21</t>
+        </is>
+      </c>
+      <c r="C111" s="3" t="inlineStr">
+        <is>
+          <t>wafer_28042024_031911.csv</t>
+        </is>
+      </c>
+      <c r="D111" s="3" t="inlineStr">
+        <is>
+          <t>Passed</t>
+        </is>
+      </c>
+      <c r="E111" s="3" t="inlineStr">
+        <is>
+          <t>COLUMN DATA VALIDATION</t>
+        </is>
+      </c>
+      <c r="F111" s="3" t="inlineStr">
+        <is>
+          <t>COLUMN DATA VALIDATION COMPLETED</t>
+        </is>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" s="3" t="n">
+        <v>111</v>
+      </c>
+      <c r="B112" s="3" t="inlineStr">
+        <is>
+          <t>2024-09-21</t>
+        </is>
+      </c>
+      <c r="C112" s="3" t="inlineStr">
+        <is>
+          <t>wafer_29012024_050617.csv</t>
+        </is>
+      </c>
+      <c r="D112" s="3" t="inlineStr">
+        <is>
+          <t>Passed</t>
+        </is>
+      </c>
+      <c r="E112" s="3" t="inlineStr">
+        <is>
+          <t>FILE NAME VALIDATION</t>
+        </is>
+      </c>
+      <c r="F112" s="3" t="inlineStr">
+        <is>
+          <t>FILE NAME VALIDATION COMPLETED</t>
+        </is>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" s="3" t="n">
+        <v>112</v>
+      </c>
+      <c r="B113" s="3" t="inlineStr">
+        <is>
+          <t>2024-09-21</t>
+        </is>
+      </c>
+      <c r="C113" s="3" t="inlineStr">
+        <is>
+          <t>wafer_29012024_050617.csv</t>
+        </is>
+      </c>
+      <c r="D113" s="3" t="inlineStr">
+        <is>
+          <t>Passed</t>
+        </is>
+      </c>
+      <c r="E113" s="3" t="inlineStr">
+        <is>
+          <t>NUMBER OF COLUMNS VALIDATION</t>
+        </is>
+      </c>
+      <c r="F113" s="3" t="inlineStr">
+        <is>
+          <t>NUMBER OF COLUMNS VALIDATION COMPLETED</t>
+        </is>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" s="3" t="n">
+        <v>113</v>
+      </c>
+      <c r="B114" s="3" t="inlineStr">
+        <is>
+          <t>2024-09-21</t>
+        </is>
+      </c>
+      <c r="C114" s="3" t="inlineStr">
+        <is>
+          <t>wafer_29012024_050617.csv</t>
+        </is>
+      </c>
+      <c r="D114" s="3" t="inlineStr">
+        <is>
+          <t>Passed</t>
+        </is>
+      </c>
+      <c r="E114" s="3" t="inlineStr">
+        <is>
+          <t>COLUMNDATA_WHOLE_MISSING_VALIDATION</t>
+        </is>
+      </c>
+      <c r="F114" s="3" t="inlineStr">
+        <is>
+          <t>COLUMN DATA WHOLE MISSING VALIDATION COMPLETED</t>
+        </is>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" s="3" t="n">
+        <v>114</v>
+      </c>
+      <c r="B115" s="3" t="inlineStr">
+        <is>
+          <t>2024-09-21</t>
+        </is>
+      </c>
+      <c r="C115" s="3" t="inlineStr">
+        <is>
+          <t>wafer_29012024_050617.csv</t>
+        </is>
+      </c>
+      <c r="D115" s="3" t="inlineStr">
+        <is>
+          <t>Passed</t>
+        </is>
+      </c>
+      <c r="E115" s="3" t="inlineStr">
+        <is>
+          <t>COLUMN DATA VALIDATION</t>
+        </is>
+      </c>
+      <c r="F115" s="3" t="inlineStr">
+        <is>
+          <t>COLUMN DATA VALIDATION COMPLETED</t>
+        </is>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" s="3" t="n">
+        <v>115</v>
+      </c>
+      <c r="B116" s="3" t="inlineStr">
+        <is>
+          <t>2024-09-21</t>
+        </is>
+      </c>
+      <c r="C116" s="3" t="inlineStr">
+        <is>
+          <t>wafer_29012024_060756.csv</t>
+        </is>
+      </c>
+      <c r="D116" s="3" t="inlineStr">
+        <is>
+          <t>Passed</t>
+        </is>
+      </c>
+      <c r="E116" s="3" t="inlineStr">
+        <is>
+          <t>FILE NAME VALIDATION</t>
+        </is>
+      </c>
+      <c r="F116" s="3" t="inlineStr">
+        <is>
+          <t>FILE NAME VALIDATION COMPLETED</t>
+        </is>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" s="3" t="n">
+        <v>116</v>
+      </c>
+      <c r="B117" s="3" t="inlineStr">
+        <is>
+          <t>2024-09-21</t>
+        </is>
+      </c>
+      <c r="C117" s="3" t="inlineStr">
+        <is>
+          <t>wafer_29012024_060756.csv</t>
+        </is>
+      </c>
+      <c r="D117" s="3" t="inlineStr">
+        <is>
+          <t>Passed</t>
+        </is>
+      </c>
+      <c r="E117" s="3" t="inlineStr">
+        <is>
+          <t>NUMBER OF COLUMNS VALIDATION</t>
+        </is>
+      </c>
+      <c r="F117" s="3" t="inlineStr">
+        <is>
+          <t>NUMBER OF COLUMNS VALIDATION COMPLETED</t>
+        </is>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" s="3" t="n">
+        <v>117</v>
+      </c>
+      <c r="B118" s="3" t="inlineStr">
+        <is>
+          <t>2024-09-21</t>
+        </is>
+      </c>
+      <c r="C118" s="3" t="inlineStr">
+        <is>
+          <t>wafer_29012024_060756.csv</t>
+        </is>
+      </c>
+      <c r="D118" s="3" t="inlineStr">
+        <is>
+          <t>Failed</t>
+        </is>
+      </c>
+      <c r="E118" s="3" t="inlineStr">
+        <is>
+          <t>COLUMNDATA_WHOLE_MISSING_VALIDATION</t>
+        </is>
+      </c>
+      <c r="F118" s="3" t="inlineStr">
+        <is>
+          <t>COLUMN DATA WHOLE MISSING VALIDATION FAILED, MISMATCH COLUMN LIST:[{'Sensor_Name': 'Sensor-86', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-110', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-111', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-112', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-221', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-245', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-246', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-247', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-359', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-383', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-384', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-385', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-493', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-517', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-518', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-519', 'Column_Data': [100, 0]}]</t>
+        </is>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" s="3" t="n">
+        <v>118</v>
+      </c>
+      <c r="B119" s="3" t="inlineStr">
+        <is>
+          <t>2024-09-21</t>
+        </is>
+      </c>
+      <c r="C119" s="3" t="inlineStr">
+        <is>
+          <t>wafer_31012024_090811.csv</t>
+        </is>
+      </c>
+      <c r="D119" s="3" t="inlineStr">
+        <is>
+          <t>Passed</t>
+        </is>
+      </c>
+      <c r="E119" s="3" t="inlineStr">
+        <is>
+          <t>FILE NAME VALIDATION</t>
+        </is>
+      </c>
+      <c r="F119" s="3" t="inlineStr">
+        <is>
+          <t>FILE NAME VALIDATION COMPLETED</t>
+        </is>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" s="3" t="n">
+        <v>119</v>
+      </c>
+      <c r="B120" s="3" t="inlineStr">
+        <is>
+          <t>2024-09-21</t>
+        </is>
+      </c>
+      <c r="C120" s="3" t="inlineStr">
+        <is>
+          <t>wafer_31012024_090811.csv</t>
+        </is>
+      </c>
+      <c r="D120" s="3" t="inlineStr">
+        <is>
+          <t>Passed</t>
+        </is>
+      </c>
+      <c r="E120" s="3" t="inlineStr">
+        <is>
+          <t>NUMBER OF COLUMNS VALIDATION</t>
+        </is>
+      </c>
+      <c r="F120" s="3" t="inlineStr">
+        <is>
+          <t>NUMBER OF COLUMNS VALIDATION COMPLETED</t>
+        </is>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" s="3" t="n">
+        <v>120</v>
+      </c>
+      <c r="B121" s="3" t="inlineStr">
+        <is>
+          <t>2024-09-21</t>
+        </is>
+      </c>
+      <c r="C121" s="3" t="inlineStr">
+        <is>
+          <t>wafer_31012024_090811.csv</t>
+        </is>
+      </c>
+      <c r="D121" s="3" t="inlineStr">
+        <is>
+          <t>Failed</t>
+        </is>
+      </c>
+      <c r="E121" s="3" t="inlineStr">
+        <is>
+          <t>COLUMNDATA_WHOLE_MISSING_VALIDATION</t>
+        </is>
+      </c>
+      <c r="F121" s="3" t="inlineStr">
+        <is>
+          <t>COLUMN DATA WHOLE MISSING VALIDATION FAILED, MISMATCH COLUMN LIST:[{'Sensor_Name': 'Sensor-86', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-110', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-111', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-112', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-221', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-245', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-246', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-247', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-359', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-383', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-384', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-385', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-493', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-517', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-518', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-519', 'Column_Data': [100, 0]}]</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
predicted data s3 sync added
</commit_message>
<xml_diff>
--- a/data/dashboard_data/prediction_validation_logs.xlsx
+++ b/data/dashboard_data/prediction_validation_logs.xlsx
@@ -439,7 +439,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F121"/>
+  <dimension ref="A1:F61"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2287,1806 +2287,6 @@
         </is>
       </c>
     </row>
-    <row r="62">
-      <c r="A62" s="3" t="n">
-        <v>61</v>
-      </c>
-      <c r="B62" s="3" t="inlineStr">
-        <is>
-          <t>2024-09-21</t>
-        </is>
-      </c>
-      <c r="C62" s="3" t="inlineStr">
-        <is>
-          <t>wafer_07012024_041011.csv</t>
-        </is>
-      </c>
-      <c r="D62" s="3" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
-      </c>
-      <c r="E62" s="3" t="inlineStr">
-        <is>
-          <t>FILE NAME VALIDATION</t>
-        </is>
-      </c>
-      <c r="F62" s="3" t="inlineStr">
-        <is>
-          <t>FILE NAME VALIDATION COMPLETED</t>
-        </is>
-      </c>
-    </row>
-    <row r="63">
-      <c r="A63" s="3" t="n">
-        <v>62</v>
-      </c>
-      <c r="B63" s="3" t="inlineStr">
-        <is>
-          <t>2024-09-21</t>
-        </is>
-      </c>
-      <c r="C63" s="3" t="inlineStr">
-        <is>
-          <t>wafer_07012024_041011.csv</t>
-        </is>
-      </c>
-      <c r="D63" s="3" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
-      </c>
-      <c r="E63" s="3" t="inlineStr">
-        <is>
-          <t>NUMBER OF COLUMNS VALIDATION</t>
-        </is>
-      </c>
-      <c r="F63" s="3" t="inlineStr">
-        <is>
-          <t>NUMBER OF COLUMNS VALIDATION COMPLETED</t>
-        </is>
-      </c>
-    </row>
-    <row r="64">
-      <c r="A64" s="3" t="n">
-        <v>63</v>
-      </c>
-      <c r="B64" s="3" t="inlineStr">
-        <is>
-          <t>2024-09-21</t>
-        </is>
-      </c>
-      <c r="C64" s="3" t="inlineStr">
-        <is>
-          <t>wafer_07012024_041011.csv</t>
-        </is>
-      </c>
-      <c r="D64" s="3" t="inlineStr">
-        <is>
-          <t>Failed</t>
-        </is>
-      </c>
-      <c r="E64" s="3" t="inlineStr">
-        <is>
-          <t>COLUMNDATA_WHOLE_MISSING_VALIDATION</t>
-        </is>
-      </c>
-      <c r="F64" s="3" t="inlineStr">
-        <is>
-          <t>COLUMN DATA WHOLE MISSING VALIDATION FAILED, MISMATCH COLUMN LIST:[{'Sensor_Name': 'Sensor-86', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-110', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-111', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-112', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-221', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-245', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-246', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-247', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-359', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-383', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-384', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-385', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-493', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-517', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-518', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-519', 'Column_Data': [100, 0]}]</t>
-        </is>
-      </c>
-    </row>
-    <row r="65">
-      <c r="A65" s="3" t="n">
-        <v>64</v>
-      </c>
-      <c r="B65" s="3" t="inlineStr">
-        <is>
-          <t>2024-09-21</t>
-        </is>
-      </c>
-      <c r="C65" s="3" t="inlineStr">
-        <is>
-          <t>wafer_13012024_090817.csv</t>
-        </is>
-      </c>
-      <c r="D65" s="3" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
-      </c>
-      <c r="E65" s="3" t="inlineStr">
-        <is>
-          <t>FILE NAME VALIDATION</t>
-        </is>
-      </c>
-      <c r="F65" s="3" t="inlineStr">
-        <is>
-          <t>FILE NAME VALIDATION COMPLETED</t>
-        </is>
-      </c>
-    </row>
-    <row r="66">
-      <c r="A66" s="3" t="n">
-        <v>65</v>
-      </c>
-      <c r="B66" s="3" t="inlineStr">
-        <is>
-          <t>2024-09-21</t>
-        </is>
-      </c>
-      <c r="C66" s="3" t="inlineStr">
-        <is>
-          <t>wafer_13012024_090817.csv</t>
-        </is>
-      </c>
-      <c r="D66" s="3" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
-      </c>
-      <c r="E66" s="3" t="inlineStr">
-        <is>
-          <t>NUMBER OF COLUMNS VALIDATION</t>
-        </is>
-      </c>
-      <c r="F66" s="3" t="inlineStr">
-        <is>
-          <t>NUMBER OF COLUMNS VALIDATION COMPLETED</t>
-        </is>
-      </c>
-    </row>
-    <row r="67">
-      <c r="A67" s="3" t="n">
-        <v>66</v>
-      </c>
-      <c r="B67" s="3" t="inlineStr">
-        <is>
-          <t>2024-09-21</t>
-        </is>
-      </c>
-      <c r="C67" s="3" t="inlineStr">
-        <is>
-          <t>wafer_13012024_090817.csv</t>
-        </is>
-      </c>
-      <c r="D67" s="3" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
-      </c>
-      <c r="E67" s="3" t="inlineStr">
-        <is>
-          <t>COLUMNDATA_WHOLE_MISSING_VALIDATION</t>
-        </is>
-      </c>
-      <c r="F67" s="3" t="inlineStr">
-        <is>
-          <t>COLUMN DATA WHOLE MISSING VALIDATION COMPLETED</t>
-        </is>
-      </c>
-    </row>
-    <row r="68">
-      <c r="A68" s="3" t="n">
-        <v>67</v>
-      </c>
-      <c r="B68" s="3" t="inlineStr">
-        <is>
-          <t>2024-09-21</t>
-        </is>
-      </c>
-      <c r="C68" s="3" t="inlineStr">
-        <is>
-          <t>wafer_13012024_090817.csv</t>
-        </is>
-      </c>
-      <c r="D68" s="3" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
-      </c>
-      <c r="E68" s="3" t="inlineStr">
-        <is>
-          <t>COLUMN DATA VALIDATION</t>
-        </is>
-      </c>
-      <c r="F68" s="3" t="inlineStr">
-        <is>
-          <t>COLUMN DATA VALIDATION COMPLETED</t>
-        </is>
-      </c>
-    </row>
-    <row r="69">
-      <c r="A69" s="3" t="n">
-        <v>68</v>
-      </c>
-      <c r="B69" s="3" t="inlineStr">
-        <is>
-          <t>2024-09-21</t>
-        </is>
-      </c>
-      <c r="C69" s="3" t="inlineStr">
-        <is>
-          <t>Wafer_13012024_141000.csv</t>
-        </is>
-      </c>
-      <c r="D69" s="3" t="inlineStr">
-        <is>
-          <t>Failed</t>
-        </is>
-      </c>
-      <c r="E69" s="3" t="inlineStr">
-        <is>
-          <t>FILE NAME VALIDATION</t>
-        </is>
-      </c>
-      <c r="F69" s="3" t="inlineStr">
-        <is>
-          <t>FILE NAME VALIDATION FAILED</t>
-        </is>
-      </c>
-    </row>
-    <row r="70">
-      <c r="A70" s="3" t="n">
-        <v>69</v>
-      </c>
-      <c r="B70" s="3" t="inlineStr">
-        <is>
-          <t>2024-09-21</t>
-        </is>
-      </c>
-      <c r="C70" s="3" t="inlineStr">
-        <is>
-          <t>Wafer_14012024_113045.csv</t>
-        </is>
-      </c>
-      <c r="D70" s="3" t="inlineStr">
-        <is>
-          <t>Failed</t>
-        </is>
-      </c>
-      <c r="E70" s="3" t="inlineStr">
-        <is>
-          <t>FILE NAME VALIDATION</t>
-        </is>
-      </c>
-      <c r="F70" s="3" t="inlineStr">
-        <is>
-          <t>FILE NAME VALIDATION FAILED</t>
-        </is>
-      </c>
-    </row>
-    <row r="71">
-      <c r="A71" s="3" t="n">
-        <v>70</v>
-      </c>
-      <c r="B71" s="3" t="inlineStr">
-        <is>
-          <t>2024-09-21</t>
-        </is>
-      </c>
-      <c r="C71" s="3" t="inlineStr">
-        <is>
-          <t>Wafer_15010_130532.csv</t>
-        </is>
-      </c>
-      <c r="D71" s="3" t="inlineStr">
-        <is>
-          <t>Failed</t>
-        </is>
-      </c>
-      <c r="E71" s="3" t="inlineStr">
-        <is>
-          <t>FILE NAME VALIDATION</t>
-        </is>
-      </c>
-      <c r="F71" s="3" t="inlineStr">
-        <is>
-          <t>FILE NAME VALIDATION FAILED</t>
-        </is>
-      </c>
-    </row>
-    <row r="72">
-      <c r="A72" s="3" t="n">
-        <v>71</v>
-      </c>
-      <c r="B72" s="3" t="inlineStr">
-        <is>
-          <t>2024-09-21</t>
-        </is>
-      </c>
-      <c r="C72" s="3" t="inlineStr">
-        <is>
-          <t>wafer_16012024_051629.csv</t>
-        </is>
-      </c>
-      <c r="D72" s="3" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
-      </c>
-      <c r="E72" s="3" t="inlineStr">
-        <is>
-          <t>FILE NAME VALIDATION</t>
-        </is>
-      </c>
-      <c r="F72" s="3" t="inlineStr">
-        <is>
-          <t>FILE NAME VALIDATION COMPLETED</t>
-        </is>
-      </c>
-    </row>
-    <row r="73">
-      <c r="A73" s="3" t="n">
-        <v>72</v>
-      </c>
-      <c r="B73" s="3" t="inlineStr">
-        <is>
-          <t>2024-09-21</t>
-        </is>
-      </c>
-      <c r="C73" s="3" t="inlineStr">
-        <is>
-          <t>wafer_16012024_051629.csv</t>
-        </is>
-      </c>
-      <c r="D73" s="3" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
-      </c>
-      <c r="E73" s="3" t="inlineStr">
-        <is>
-          <t>NUMBER OF COLUMNS VALIDATION</t>
-        </is>
-      </c>
-      <c r="F73" s="3" t="inlineStr">
-        <is>
-          <t>NUMBER OF COLUMNS VALIDATION COMPLETED</t>
-        </is>
-      </c>
-    </row>
-    <row r="74">
-      <c r="A74" s="3" t="n">
-        <v>73</v>
-      </c>
-      <c r="B74" s="3" t="inlineStr">
-        <is>
-          <t>2024-09-21</t>
-        </is>
-      </c>
-      <c r="C74" s="3" t="inlineStr">
-        <is>
-          <t>wafer_16012024_051629.csv</t>
-        </is>
-      </c>
-      <c r="D74" s="3" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
-      </c>
-      <c r="E74" s="3" t="inlineStr">
-        <is>
-          <t>COLUMNDATA_WHOLE_MISSING_VALIDATION</t>
-        </is>
-      </c>
-      <c r="F74" s="3" t="inlineStr">
-        <is>
-          <t>COLUMN DATA WHOLE MISSING VALIDATION COMPLETED</t>
-        </is>
-      </c>
-    </row>
-    <row r="75">
-      <c r="A75" s="3" t="n">
-        <v>74</v>
-      </c>
-      <c r="B75" s="3" t="inlineStr">
-        <is>
-          <t>2024-09-21</t>
-        </is>
-      </c>
-      <c r="C75" s="3" t="inlineStr">
-        <is>
-          <t>wafer_16012024_051629.csv</t>
-        </is>
-      </c>
-      <c r="D75" s="3" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
-      </c>
-      <c r="E75" s="3" t="inlineStr">
-        <is>
-          <t>COLUMN DATA VALIDATION</t>
-        </is>
-      </c>
-      <c r="F75" s="3" t="inlineStr">
-        <is>
-          <t>COLUMN DATA VALIDATION COMPLETED</t>
-        </is>
-      </c>
-    </row>
-    <row r="76">
-      <c r="A76" s="3" t="n">
-        <v>75</v>
-      </c>
-      <c r="B76" s="3" t="inlineStr">
-        <is>
-          <t>2024-09-21</t>
-        </is>
-      </c>
-      <c r="C76" s="3" t="inlineStr">
-        <is>
-          <t>wafer_20012024_090819.csv</t>
-        </is>
-      </c>
-      <c r="D76" s="3" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
-      </c>
-      <c r="E76" s="3" t="inlineStr">
-        <is>
-          <t>FILE NAME VALIDATION</t>
-        </is>
-      </c>
-      <c r="F76" s="3" t="inlineStr">
-        <is>
-          <t>FILE NAME VALIDATION COMPLETED</t>
-        </is>
-      </c>
-    </row>
-    <row r="77">
-      <c r="A77" s="3" t="n">
-        <v>76</v>
-      </c>
-      <c r="B77" s="3" t="inlineStr">
-        <is>
-          <t>2024-09-21</t>
-        </is>
-      </c>
-      <c r="C77" s="3" t="inlineStr">
-        <is>
-          <t>wafer_20012024_090819.csv</t>
-        </is>
-      </c>
-      <c r="D77" s="3" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
-      </c>
-      <c r="E77" s="3" t="inlineStr">
-        <is>
-          <t>NUMBER OF COLUMNS VALIDATION</t>
-        </is>
-      </c>
-      <c r="F77" s="3" t="inlineStr">
-        <is>
-          <t>NUMBER OF COLUMNS VALIDATION COMPLETED</t>
-        </is>
-      </c>
-    </row>
-    <row r="78">
-      <c r="A78" s="3" t="n">
-        <v>77</v>
-      </c>
-      <c r="B78" s="3" t="inlineStr">
-        <is>
-          <t>2024-09-21</t>
-        </is>
-      </c>
-      <c r="C78" s="3" t="inlineStr">
-        <is>
-          <t>wafer_20012024_090819.csv</t>
-        </is>
-      </c>
-      <c r="D78" s="3" t="inlineStr">
-        <is>
-          <t>Failed</t>
-        </is>
-      </c>
-      <c r="E78" s="3" t="inlineStr">
-        <is>
-          <t>COLUMNDATA_WHOLE_MISSING_VALIDATION</t>
-        </is>
-      </c>
-      <c r="F78" s="3" t="inlineStr">
-        <is>
-          <t>COLUMN DATA WHOLE MISSING VALIDATION FAILED, MISMATCH COLUMN LIST:[{'Sensor_Name': 'Sensor-86', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-110', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-111', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-112', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-221', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-245', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-246', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-247', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-359', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-383', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-384', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-385', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-493', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-517', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-518', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-519', 'Column_Data': [100, 0]}]</t>
-        </is>
-      </c>
-    </row>
-    <row r="79">
-      <c r="A79" s="3" t="n">
-        <v>78</v>
-      </c>
-      <c r="B79" s="3" t="inlineStr">
-        <is>
-          <t>2024-09-21</t>
-        </is>
-      </c>
-      <c r="C79" s="3" t="inlineStr">
-        <is>
-          <t>wafer_20022024_090716.csv</t>
-        </is>
-      </c>
-      <c r="D79" s="3" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
-      </c>
-      <c r="E79" s="3" t="inlineStr">
-        <is>
-          <t>FILE NAME VALIDATION</t>
-        </is>
-      </c>
-      <c r="F79" s="3" t="inlineStr">
-        <is>
-          <t>FILE NAME VALIDATION COMPLETED</t>
-        </is>
-      </c>
-    </row>
-    <row r="80">
-      <c r="A80" s="3" t="n">
-        <v>79</v>
-      </c>
-      <c r="B80" s="3" t="inlineStr">
-        <is>
-          <t>2024-09-21</t>
-        </is>
-      </c>
-      <c r="C80" s="3" t="inlineStr">
-        <is>
-          <t>wafer_20022024_090716.csv</t>
-        </is>
-      </c>
-      <c r="D80" s="3" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
-      </c>
-      <c r="E80" s="3" t="inlineStr">
-        <is>
-          <t>NUMBER OF COLUMNS VALIDATION</t>
-        </is>
-      </c>
-      <c r="F80" s="3" t="inlineStr">
-        <is>
-          <t>NUMBER OF COLUMNS VALIDATION COMPLETED</t>
-        </is>
-      </c>
-    </row>
-    <row r="81">
-      <c r="A81" s="3" t="n">
-        <v>80</v>
-      </c>
-      <c r="B81" s="3" t="inlineStr">
-        <is>
-          <t>2024-09-21</t>
-        </is>
-      </c>
-      <c r="C81" s="3" t="inlineStr">
-        <is>
-          <t>wafer_20022024_090716.csv</t>
-        </is>
-      </c>
-      <c r="D81" s="3" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
-      </c>
-      <c r="E81" s="3" t="inlineStr">
-        <is>
-          <t>COLUMNDATA_WHOLE_MISSING_VALIDATION</t>
-        </is>
-      </c>
-      <c r="F81" s="3" t="inlineStr">
-        <is>
-          <t>COLUMN DATA WHOLE MISSING VALIDATION COMPLETED</t>
-        </is>
-      </c>
-    </row>
-    <row r="82">
-      <c r="A82" s="3" t="n">
-        <v>81</v>
-      </c>
-      <c r="B82" s="3" t="inlineStr">
-        <is>
-          <t>2024-09-21</t>
-        </is>
-      </c>
-      <c r="C82" s="3" t="inlineStr">
-        <is>
-          <t>wafer_20022024_090716.csv</t>
-        </is>
-      </c>
-      <c r="D82" s="3" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
-      </c>
-      <c r="E82" s="3" t="inlineStr">
-        <is>
-          <t>COLUMN DATA VALIDATION</t>
-        </is>
-      </c>
-      <c r="F82" s="3" t="inlineStr">
-        <is>
-          <t>COLUMN DATA VALIDATION COMPLETED</t>
-        </is>
-      </c>
-    </row>
-    <row r="83">
-      <c r="A83" s="3" t="n">
-        <v>82</v>
-      </c>
-      <c r="B83" s="3" t="inlineStr">
-        <is>
-          <t>2024-09-21</t>
-        </is>
-      </c>
-      <c r="C83" s="3" t="inlineStr">
-        <is>
-          <t>wafer_21012024_080913.csv</t>
-        </is>
-      </c>
-      <c r="D83" s="3" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
-      </c>
-      <c r="E83" s="3" t="inlineStr">
-        <is>
-          <t>FILE NAME VALIDATION</t>
-        </is>
-      </c>
-      <c r="F83" s="3" t="inlineStr">
-        <is>
-          <t>FILE NAME VALIDATION COMPLETED</t>
-        </is>
-      </c>
-    </row>
-    <row r="84">
-      <c r="A84" s="3" t="n">
-        <v>83</v>
-      </c>
-      <c r="B84" s="3" t="inlineStr">
-        <is>
-          <t>2024-09-21</t>
-        </is>
-      </c>
-      <c r="C84" s="3" t="inlineStr">
-        <is>
-          <t>wafer_21012024_080913.csv</t>
-        </is>
-      </c>
-      <c r="D84" s="3" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
-      </c>
-      <c r="E84" s="3" t="inlineStr">
-        <is>
-          <t>NUMBER OF COLUMNS VALIDATION</t>
-        </is>
-      </c>
-      <c r="F84" s="3" t="inlineStr">
-        <is>
-          <t>NUMBER OF COLUMNS VALIDATION COMPLETED</t>
-        </is>
-      </c>
-    </row>
-    <row r="85">
-      <c r="A85" s="3" t="n">
-        <v>84</v>
-      </c>
-      <c r="B85" s="3" t="inlineStr">
-        <is>
-          <t>2024-09-21</t>
-        </is>
-      </c>
-      <c r="C85" s="3" t="inlineStr">
-        <is>
-          <t>wafer_21012024_080913.csv</t>
-        </is>
-      </c>
-      <c r="D85" s="3" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
-      </c>
-      <c r="E85" s="3" t="inlineStr">
-        <is>
-          <t>COLUMNDATA_WHOLE_MISSING_VALIDATION</t>
-        </is>
-      </c>
-      <c r="F85" s="3" t="inlineStr">
-        <is>
-          <t>COLUMN DATA WHOLE MISSING VALIDATION COMPLETED</t>
-        </is>
-      </c>
-    </row>
-    <row r="86">
-      <c r="A86" s="3" t="n">
-        <v>85</v>
-      </c>
-      <c r="B86" s="3" t="inlineStr">
-        <is>
-          <t>2024-09-21</t>
-        </is>
-      </c>
-      <c r="C86" s="3" t="inlineStr">
-        <is>
-          <t>wafer_21012024_080913.csv</t>
-        </is>
-      </c>
-      <c r="D86" s="3" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
-      </c>
-      <c r="E86" s="3" t="inlineStr">
-        <is>
-          <t>COLUMN DATA VALIDATION</t>
-        </is>
-      </c>
-      <c r="F86" s="3" t="inlineStr">
-        <is>
-          <t>COLUMN DATA VALIDATION COMPLETED</t>
-        </is>
-      </c>
-    </row>
-    <row r="87">
-      <c r="A87" s="3" t="n">
-        <v>86</v>
-      </c>
-      <c r="B87" s="3" t="inlineStr">
-        <is>
-          <t>2024-09-21</t>
-        </is>
-      </c>
-      <c r="C87" s="3" t="inlineStr">
-        <is>
-          <t>wafer_22022024_041119.csv</t>
-        </is>
-      </c>
-      <c r="D87" s="3" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
-      </c>
-      <c r="E87" s="3" t="inlineStr">
-        <is>
-          <t>FILE NAME VALIDATION</t>
-        </is>
-      </c>
-      <c r="F87" s="3" t="inlineStr">
-        <is>
-          <t>FILE NAME VALIDATION COMPLETED</t>
-        </is>
-      </c>
-    </row>
-    <row r="88">
-      <c r="A88" s="3" t="n">
-        <v>87</v>
-      </c>
-      <c r="B88" s="3" t="inlineStr">
-        <is>
-          <t>2024-09-21</t>
-        </is>
-      </c>
-      <c r="C88" s="3" t="inlineStr">
-        <is>
-          <t>wafer_22022024_041119.csv</t>
-        </is>
-      </c>
-      <c r="D88" s="3" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
-      </c>
-      <c r="E88" s="3" t="inlineStr">
-        <is>
-          <t>NUMBER OF COLUMNS VALIDATION</t>
-        </is>
-      </c>
-      <c r="F88" s="3" t="inlineStr">
-        <is>
-          <t>NUMBER OF COLUMNS VALIDATION COMPLETED</t>
-        </is>
-      </c>
-    </row>
-    <row r="89">
-      <c r="A89" s="3" t="n">
-        <v>88</v>
-      </c>
-      <c r="B89" s="3" t="inlineStr">
-        <is>
-          <t>2024-09-21</t>
-        </is>
-      </c>
-      <c r="C89" s="3" t="inlineStr">
-        <is>
-          <t>wafer_22022024_041119.csv</t>
-        </is>
-      </c>
-      <c r="D89" s="3" t="inlineStr">
-        <is>
-          <t>Failed</t>
-        </is>
-      </c>
-      <c r="E89" s="3" t="inlineStr">
-        <is>
-          <t>COLUMNDATA_WHOLE_MISSING_VALIDATION</t>
-        </is>
-      </c>
-      <c r="F89" s="3" t="inlineStr">
-        <is>
-          <t>COLUMN DATA WHOLE MISSING VALIDATION FAILED, MISMATCH COLUMN LIST:[{'Sensor_Name': 'Sensor-86', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-110', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-111', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-112', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-221', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-245', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-246', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-247', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-359', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-383', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-384', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-385', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-493', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-517', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-518', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-519', 'Column_Data': [100, 0]}]</t>
-        </is>
-      </c>
-    </row>
-    <row r="90">
-      <c r="A90" s="3" t="n">
-        <v>89</v>
-      </c>
-      <c r="B90" s="3" t="inlineStr">
-        <is>
-          <t>2024-09-21</t>
-        </is>
-      </c>
-      <c r="C90" s="3" t="inlineStr">
-        <is>
-          <t>wafer_23012024_011008.csv</t>
-        </is>
-      </c>
-      <c r="D90" s="3" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
-      </c>
-      <c r="E90" s="3" t="inlineStr">
-        <is>
-          <t>FILE NAME VALIDATION</t>
-        </is>
-      </c>
-      <c r="F90" s="3" t="inlineStr">
-        <is>
-          <t>FILE NAME VALIDATION COMPLETED</t>
-        </is>
-      </c>
-    </row>
-    <row r="91">
-      <c r="A91" s="3" t="n">
-        <v>90</v>
-      </c>
-      <c r="B91" s="3" t="inlineStr">
-        <is>
-          <t>2024-09-21</t>
-        </is>
-      </c>
-      <c r="C91" s="3" t="inlineStr">
-        <is>
-          <t>wafer_23012024_011008.csv</t>
-        </is>
-      </c>
-      <c r="D91" s="3" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
-      </c>
-      <c r="E91" s="3" t="inlineStr">
-        <is>
-          <t>NUMBER OF COLUMNS VALIDATION</t>
-        </is>
-      </c>
-      <c r="F91" s="3" t="inlineStr">
-        <is>
-          <t>NUMBER OF COLUMNS VALIDATION COMPLETED</t>
-        </is>
-      </c>
-    </row>
-    <row r="92">
-      <c r="A92" s="3" t="n">
-        <v>91</v>
-      </c>
-      <c r="B92" s="3" t="inlineStr">
-        <is>
-          <t>2024-09-21</t>
-        </is>
-      </c>
-      <c r="C92" s="3" t="inlineStr">
-        <is>
-          <t>wafer_23012024_011008.csv</t>
-        </is>
-      </c>
-      <c r="D92" s="3" t="inlineStr">
-        <is>
-          <t>Failed</t>
-        </is>
-      </c>
-      <c r="E92" s="3" t="inlineStr">
-        <is>
-          <t>COLUMNDATA_WHOLE_MISSING_VALIDATION</t>
-        </is>
-      </c>
-      <c r="F92" s="3" t="inlineStr">
-        <is>
-          <t>COLUMN DATA WHOLE MISSING VALIDATION FAILED, MISMATCH COLUMN LIST:[{'Sensor_Name': 'Sensor-86', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-110', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-111', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-112', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-221', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-245', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-246', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-247', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-359', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-383', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-384', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-385', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-493', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-517', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-518', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-519', 'Column_Data': [100, 0]}]</t>
-        </is>
-      </c>
-    </row>
-    <row r="93">
-      <c r="A93" s="3" t="n">
-        <v>92</v>
-      </c>
-      <c r="B93" s="3" t="inlineStr">
-        <is>
-          <t>2024-09-21</t>
-        </is>
-      </c>
-      <c r="C93" s="3" t="inlineStr">
-        <is>
-          <t>wafer_23012024_041211.csv</t>
-        </is>
-      </c>
-      <c r="D93" s="3" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
-      </c>
-      <c r="E93" s="3" t="inlineStr">
-        <is>
-          <t>FILE NAME VALIDATION</t>
-        </is>
-      </c>
-      <c r="F93" s="3" t="inlineStr">
-        <is>
-          <t>FILE NAME VALIDATION COMPLETED</t>
-        </is>
-      </c>
-    </row>
-    <row r="94">
-      <c r="A94" s="3" t="n">
-        <v>93</v>
-      </c>
-      <c r="B94" s="3" t="inlineStr">
-        <is>
-          <t>2024-09-21</t>
-        </is>
-      </c>
-      <c r="C94" s="3" t="inlineStr">
-        <is>
-          <t>wafer_23012024_041211.csv</t>
-        </is>
-      </c>
-      <c r="D94" s="3" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
-      </c>
-      <c r="E94" s="3" t="inlineStr">
-        <is>
-          <t>NUMBER OF COLUMNS VALIDATION</t>
-        </is>
-      </c>
-      <c r="F94" s="3" t="inlineStr">
-        <is>
-          <t>NUMBER OF COLUMNS VALIDATION COMPLETED</t>
-        </is>
-      </c>
-    </row>
-    <row r="95">
-      <c r="A95" s="3" t="n">
-        <v>94</v>
-      </c>
-      <c r="B95" s="3" t="inlineStr">
-        <is>
-          <t>2024-09-21</t>
-        </is>
-      </c>
-      <c r="C95" s="3" t="inlineStr">
-        <is>
-          <t>wafer_23012024_041211.csv</t>
-        </is>
-      </c>
-      <c r="D95" s="3" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
-      </c>
-      <c r="E95" s="3" t="inlineStr">
-        <is>
-          <t>COLUMNDATA_WHOLE_MISSING_VALIDATION</t>
-        </is>
-      </c>
-      <c r="F95" s="3" t="inlineStr">
-        <is>
-          <t>COLUMN DATA WHOLE MISSING VALIDATION COMPLETED</t>
-        </is>
-      </c>
-    </row>
-    <row r="96">
-      <c r="A96" s="3" t="n">
-        <v>95</v>
-      </c>
-      <c r="B96" s="3" t="inlineStr">
-        <is>
-          <t>2024-09-21</t>
-        </is>
-      </c>
-      <c r="C96" s="3" t="inlineStr">
-        <is>
-          <t>wafer_23012024_041211.csv</t>
-        </is>
-      </c>
-      <c r="D96" s="3" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
-      </c>
-      <c r="E96" s="3" t="inlineStr">
-        <is>
-          <t>COLUMN DATA VALIDATION</t>
-        </is>
-      </c>
-      <c r="F96" s="3" t="inlineStr">
-        <is>
-          <t>COLUMN DATA VALIDATION COMPLETED</t>
-        </is>
-      </c>
-    </row>
-    <row r="97">
-      <c r="A97" s="3" t="n">
-        <v>96</v>
-      </c>
-      <c r="B97" s="3" t="inlineStr">
-        <is>
-          <t>2024-09-21</t>
-        </is>
-      </c>
-      <c r="C97" s="3" t="inlineStr">
-        <is>
-          <t>wafer_27012024_080911.csv</t>
-        </is>
-      </c>
-      <c r="D97" s="3" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
-      </c>
-      <c r="E97" s="3" t="inlineStr">
-        <is>
-          <t>FILE NAME VALIDATION</t>
-        </is>
-      </c>
-      <c r="F97" s="3" t="inlineStr">
-        <is>
-          <t>FILE NAME VALIDATION COMPLETED</t>
-        </is>
-      </c>
-    </row>
-    <row r="98">
-      <c r="A98" s="3" t="n">
-        <v>97</v>
-      </c>
-      <c r="B98" s="3" t="inlineStr">
-        <is>
-          <t>2024-09-21</t>
-        </is>
-      </c>
-      <c r="C98" s="3" t="inlineStr">
-        <is>
-          <t>wafer_27012024_080911.csv</t>
-        </is>
-      </c>
-      <c r="D98" s="3" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
-      </c>
-      <c r="E98" s="3" t="inlineStr">
-        <is>
-          <t>NUMBER OF COLUMNS VALIDATION</t>
-        </is>
-      </c>
-      <c r="F98" s="3" t="inlineStr">
-        <is>
-          <t>NUMBER OF COLUMNS VALIDATION COMPLETED</t>
-        </is>
-      </c>
-    </row>
-    <row r="99">
-      <c r="A99" s="3" t="n">
-        <v>98</v>
-      </c>
-      <c r="B99" s="3" t="inlineStr">
-        <is>
-          <t>2024-09-21</t>
-        </is>
-      </c>
-      <c r="C99" s="3" t="inlineStr">
-        <is>
-          <t>wafer_27012024_080911.csv</t>
-        </is>
-      </c>
-      <c r="D99" s="3" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
-      </c>
-      <c r="E99" s="3" t="inlineStr">
-        <is>
-          <t>COLUMNDATA_WHOLE_MISSING_VALIDATION</t>
-        </is>
-      </c>
-      <c r="F99" s="3" t="inlineStr">
-        <is>
-          <t>COLUMN DATA WHOLE MISSING VALIDATION COMPLETED</t>
-        </is>
-      </c>
-    </row>
-    <row r="100">
-      <c r="A100" s="3" t="n">
-        <v>99</v>
-      </c>
-      <c r="B100" s="3" t="inlineStr">
-        <is>
-          <t>2024-09-21</t>
-        </is>
-      </c>
-      <c r="C100" s="3" t="inlineStr">
-        <is>
-          <t>wafer_27012024_080911.csv</t>
-        </is>
-      </c>
-      <c r="D100" s="3" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
-      </c>
-      <c r="E100" s="3" t="inlineStr">
-        <is>
-          <t>COLUMN DATA VALIDATION</t>
-        </is>
-      </c>
-      <c r="F100" s="3" t="inlineStr">
-        <is>
-          <t>COLUMN DATA VALIDATION COMPLETED</t>
-        </is>
-      </c>
-    </row>
-    <row r="101">
-      <c r="A101" s="3" t="n">
-        <v>100</v>
-      </c>
-      <c r="B101" s="3" t="inlineStr">
-        <is>
-          <t>2024-09-21</t>
-        </is>
-      </c>
-      <c r="C101" s="3" t="inlineStr">
-        <is>
-          <t>wafer_28012024_051011.csv</t>
-        </is>
-      </c>
-      <c r="D101" s="3" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
-      </c>
-      <c r="E101" s="3" t="inlineStr">
-        <is>
-          <t>FILE NAME VALIDATION</t>
-        </is>
-      </c>
-      <c r="F101" s="3" t="inlineStr">
-        <is>
-          <t>FILE NAME VALIDATION COMPLETED</t>
-        </is>
-      </c>
-    </row>
-    <row r="102">
-      <c r="A102" s="3" t="n">
-        <v>101</v>
-      </c>
-      <c r="B102" s="3" t="inlineStr">
-        <is>
-          <t>2024-09-21</t>
-        </is>
-      </c>
-      <c r="C102" s="3" t="inlineStr">
-        <is>
-          <t>wafer_28012024_051011.csv</t>
-        </is>
-      </c>
-      <c r="D102" s="3" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
-      </c>
-      <c r="E102" s="3" t="inlineStr">
-        <is>
-          <t>NUMBER OF COLUMNS VALIDATION</t>
-        </is>
-      </c>
-      <c r="F102" s="3" t="inlineStr">
-        <is>
-          <t>NUMBER OF COLUMNS VALIDATION COMPLETED</t>
-        </is>
-      </c>
-    </row>
-    <row r="103">
-      <c r="A103" s="3" t="n">
-        <v>102</v>
-      </c>
-      <c r="B103" s="3" t="inlineStr">
-        <is>
-          <t>2024-09-21</t>
-        </is>
-      </c>
-      <c r="C103" s="3" t="inlineStr">
-        <is>
-          <t>wafer_28012024_051011.csv</t>
-        </is>
-      </c>
-      <c r="D103" s="3" t="inlineStr">
-        <is>
-          <t>Failed</t>
-        </is>
-      </c>
-      <c r="E103" s="3" t="inlineStr">
-        <is>
-          <t>COLUMNDATA_WHOLE_MISSING_VALIDATION</t>
-        </is>
-      </c>
-      <c r="F103" s="3" t="inlineStr">
-        <is>
-          <t>COLUMN DATA WHOLE MISSING VALIDATION FAILED, MISMATCH COLUMN LIST:[{'Sensor_Name': 'Sensor-86', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-110', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-111', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-112', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-221', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-245', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-246', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-247', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-359', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-383', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-384', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-385', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-493', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-517', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-518', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-519', 'Column_Data': [100, 0]}]</t>
-        </is>
-      </c>
-    </row>
-    <row r="104">
-      <c r="A104" s="3" t="n">
-        <v>103</v>
-      </c>
-      <c r="B104" s="3" t="inlineStr">
-        <is>
-          <t>2024-09-21</t>
-        </is>
-      </c>
-      <c r="C104" s="3" t="inlineStr">
-        <is>
-          <t>wafer_28012024_090817.csv</t>
-        </is>
-      </c>
-      <c r="D104" s="3" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
-      </c>
-      <c r="E104" s="3" t="inlineStr">
-        <is>
-          <t>FILE NAME VALIDATION</t>
-        </is>
-      </c>
-      <c r="F104" s="3" t="inlineStr">
-        <is>
-          <t>FILE NAME VALIDATION COMPLETED</t>
-        </is>
-      </c>
-    </row>
-    <row r="105">
-      <c r="A105" s="3" t="n">
-        <v>104</v>
-      </c>
-      <c r="B105" s="3" t="inlineStr">
-        <is>
-          <t>2024-09-21</t>
-        </is>
-      </c>
-      <c r="C105" s="3" t="inlineStr">
-        <is>
-          <t>wafer_28012024_090817.csv</t>
-        </is>
-      </c>
-      <c r="D105" s="3" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
-      </c>
-      <c r="E105" s="3" t="inlineStr">
-        <is>
-          <t>NUMBER OF COLUMNS VALIDATION</t>
-        </is>
-      </c>
-      <c r="F105" s="3" t="inlineStr">
-        <is>
-          <t>NUMBER OF COLUMNS VALIDATION COMPLETED</t>
-        </is>
-      </c>
-    </row>
-    <row r="106">
-      <c r="A106" s="3" t="n">
-        <v>105</v>
-      </c>
-      <c r="B106" s="3" t="inlineStr">
-        <is>
-          <t>2024-09-21</t>
-        </is>
-      </c>
-      <c r="C106" s="3" t="inlineStr">
-        <is>
-          <t>wafer_28012024_090817.csv</t>
-        </is>
-      </c>
-      <c r="D106" s="3" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
-      </c>
-      <c r="E106" s="3" t="inlineStr">
-        <is>
-          <t>COLUMNDATA_WHOLE_MISSING_VALIDATION</t>
-        </is>
-      </c>
-      <c r="F106" s="3" t="inlineStr">
-        <is>
-          <t>COLUMN DATA WHOLE MISSING VALIDATION COMPLETED</t>
-        </is>
-      </c>
-    </row>
-    <row r="107">
-      <c r="A107" s="3" t="n">
-        <v>106</v>
-      </c>
-      <c r="B107" s="3" t="inlineStr">
-        <is>
-          <t>2024-09-21</t>
-        </is>
-      </c>
-      <c r="C107" s="3" t="inlineStr">
-        <is>
-          <t>wafer_28012024_090817.csv</t>
-        </is>
-      </c>
-      <c r="D107" s="3" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
-      </c>
-      <c r="E107" s="3" t="inlineStr">
-        <is>
-          <t>COLUMN DATA VALIDATION</t>
-        </is>
-      </c>
-      <c r="F107" s="3" t="inlineStr">
-        <is>
-          <t>COLUMN DATA VALIDATION COMPLETED</t>
-        </is>
-      </c>
-    </row>
-    <row r="108">
-      <c r="A108" s="3" t="n">
-        <v>107</v>
-      </c>
-      <c r="B108" s="3" t="inlineStr">
-        <is>
-          <t>2024-09-21</t>
-        </is>
-      </c>
-      <c r="C108" s="3" t="inlineStr">
-        <is>
-          <t>wafer_28042024_031911.csv</t>
-        </is>
-      </c>
-      <c r="D108" s="3" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
-      </c>
-      <c r="E108" s="3" t="inlineStr">
-        <is>
-          <t>FILE NAME VALIDATION</t>
-        </is>
-      </c>
-      <c r="F108" s="3" t="inlineStr">
-        <is>
-          <t>FILE NAME VALIDATION COMPLETED</t>
-        </is>
-      </c>
-    </row>
-    <row r="109">
-      <c r="A109" s="3" t="n">
-        <v>108</v>
-      </c>
-      <c r="B109" s="3" t="inlineStr">
-        <is>
-          <t>2024-09-21</t>
-        </is>
-      </c>
-      <c r="C109" s="3" t="inlineStr">
-        <is>
-          <t>wafer_28042024_031911.csv</t>
-        </is>
-      </c>
-      <c r="D109" s="3" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
-      </c>
-      <c r="E109" s="3" t="inlineStr">
-        <is>
-          <t>NUMBER OF COLUMNS VALIDATION</t>
-        </is>
-      </c>
-      <c r="F109" s="3" t="inlineStr">
-        <is>
-          <t>NUMBER OF COLUMNS VALIDATION COMPLETED</t>
-        </is>
-      </c>
-    </row>
-    <row r="110">
-      <c r="A110" s="3" t="n">
-        <v>109</v>
-      </c>
-      <c r="B110" s="3" t="inlineStr">
-        <is>
-          <t>2024-09-21</t>
-        </is>
-      </c>
-      <c r="C110" s="3" t="inlineStr">
-        <is>
-          <t>wafer_28042024_031911.csv</t>
-        </is>
-      </c>
-      <c r="D110" s="3" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
-      </c>
-      <c r="E110" s="3" t="inlineStr">
-        <is>
-          <t>COLUMNDATA_WHOLE_MISSING_VALIDATION</t>
-        </is>
-      </c>
-      <c r="F110" s="3" t="inlineStr">
-        <is>
-          <t>COLUMN DATA WHOLE MISSING VALIDATION COMPLETED</t>
-        </is>
-      </c>
-    </row>
-    <row r="111">
-      <c r="A111" s="3" t="n">
-        <v>110</v>
-      </c>
-      <c r="B111" s="3" t="inlineStr">
-        <is>
-          <t>2024-09-21</t>
-        </is>
-      </c>
-      <c r="C111" s="3" t="inlineStr">
-        <is>
-          <t>wafer_28042024_031911.csv</t>
-        </is>
-      </c>
-      <c r="D111" s="3" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
-      </c>
-      <c r="E111" s="3" t="inlineStr">
-        <is>
-          <t>COLUMN DATA VALIDATION</t>
-        </is>
-      </c>
-      <c r="F111" s="3" t="inlineStr">
-        <is>
-          <t>COLUMN DATA VALIDATION COMPLETED</t>
-        </is>
-      </c>
-    </row>
-    <row r="112">
-      <c r="A112" s="3" t="n">
-        <v>111</v>
-      </c>
-      <c r="B112" s="3" t="inlineStr">
-        <is>
-          <t>2024-09-21</t>
-        </is>
-      </c>
-      <c r="C112" s="3" t="inlineStr">
-        <is>
-          <t>wafer_29012024_050617.csv</t>
-        </is>
-      </c>
-      <c r="D112" s="3" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
-      </c>
-      <c r="E112" s="3" t="inlineStr">
-        <is>
-          <t>FILE NAME VALIDATION</t>
-        </is>
-      </c>
-      <c r="F112" s="3" t="inlineStr">
-        <is>
-          <t>FILE NAME VALIDATION COMPLETED</t>
-        </is>
-      </c>
-    </row>
-    <row r="113">
-      <c r="A113" s="3" t="n">
-        <v>112</v>
-      </c>
-      <c r="B113" s="3" t="inlineStr">
-        <is>
-          <t>2024-09-21</t>
-        </is>
-      </c>
-      <c r="C113" s="3" t="inlineStr">
-        <is>
-          <t>wafer_29012024_050617.csv</t>
-        </is>
-      </c>
-      <c r="D113" s="3" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
-      </c>
-      <c r="E113" s="3" t="inlineStr">
-        <is>
-          <t>NUMBER OF COLUMNS VALIDATION</t>
-        </is>
-      </c>
-      <c r="F113" s="3" t="inlineStr">
-        <is>
-          <t>NUMBER OF COLUMNS VALIDATION COMPLETED</t>
-        </is>
-      </c>
-    </row>
-    <row r="114">
-      <c r="A114" s="3" t="n">
-        <v>113</v>
-      </c>
-      <c r="B114" s="3" t="inlineStr">
-        <is>
-          <t>2024-09-21</t>
-        </is>
-      </c>
-      <c r="C114" s="3" t="inlineStr">
-        <is>
-          <t>wafer_29012024_050617.csv</t>
-        </is>
-      </c>
-      <c r="D114" s="3" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
-      </c>
-      <c r="E114" s="3" t="inlineStr">
-        <is>
-          <t>COLUMNDATA_WHOLE_MISSING_VALIDATION</t>
-        </is>
-      </c>
-      <c r="F114" s="3" t="inlineStr">
-        <is>
-          <t>COLUMN DATA WHOLE MISSING VALIDATION COMPLETED</t>
-        </is>
-      </c>
-    </row>
-    <row r="115">
-      <c r="A115" s="3" t="n">
-        <v>114</v>
-      </c>
-      <c r="B115" s="3" t="inlineStr">
-        <is>
-          <t>2024-09-21</t>
-        </is>
-      </c>
-      <c r="C115" s="3" t="inlineStr">
-        <is>
-          <t>wafer_29012024_050617.csv</t>
-        </is>
-      </c>
-      <c r="D115" s="3" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
-      </c>
-      <c r="E115" s="3" t="inlineStr">
-        <is>
-          <t>COLUMN DATA VALIDATION</t>
-        </is>
-      </c>
-      <c r="F115" s="3" t="inlineStr">
-        <is>
-          <t>COLUMN DATA VALIDATION COMPLETED</t>
-        </is>
-      </c>
-    </row>
-    <row r="116">
-      <c r="A116" s="3" t="n">
-        <v>115</v>
-      </c>
-      <c r="B116" s="3" t="inlineStr">
-        <is>
-          <t>2024-09-21</t>
-        </is>
-      </c>
-      <c r="C116" s="3" t="inlineStr">
-        <is>
-          <t>wafer_29012024_060756.csv</t>
-        </is>
-      </c>
-      <c r="D116" s="3" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
-      </c>
-      <c r="E116" s="3" t="inlineStr">
-        <is>
-          <t>FILE NAME VALIDATION</t>
-        </is>
-      </c>
-      <c r="F116" s="3" t="inlineStr">
-        <is>
-          <t>FILE NAME VALIDATION COMPLETED</t>
-        </is>
-      </c>
-    </row>
-    <row r="117">
-      <c r="A117" s="3" t="n">
-        <v>116</v>
-      </c>
-      <c r="B117" s="3" t="inlineStr">
-        <is>
-          <t>2024-09-21</t>
-        </is>
-      </c>
-      <c r="C117" s="3" t="inlineStr">
-        <is>
-          <t>wafer_29012024_060756.csv</t>
-        </is>
-      </c>
-      <c r="D117" s="3" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
-      </c>
-      <c r="E117" s="3" t="inlineStr">
-        <is>
-          <t>NUMBER OF COLUMNS VALIDATION</t>
-        </is>
-      </c>
-      <c r="F117" s="3" t="inlineStr">
-        <is>
-          <t>NUMBER OF COLUMNS VALIDATION COMPLETED</t>
-        </is>
-      </c>
-    </row>
-    <row r="118">
-      <c r="A118" s="3" t="n">
-        <v>117</v>
-      </c>
-      <c r="B118" s="3" t="inlineStr">
-        <is>
-          <t>2024-09-21</t>
-        </is>
-      </c>
-      <c r="C118" s="3" t="inlineStr">
-        <is>
-          <t>wafer_29012024_060756.csv</t>
-        </is>
-      </c>
-      <c r="D118" s="3" t="inlineStr">
-        <is>
-          <t>Failed</t>
-        </is>
-      </c>
-      <c r="E118" s="3" t="inlineStr">
-        <is>
-          <t>COLUMNDATA_WHOLE_MISSING_VALIDATION</t>
-        </is>
-      </c>
-      <c r="F118" s="3" t="inlineStr">
-        <is>
-          <t>COLUMN DATA WHOLE MISSING VALIDATION FAILED, MISMATCH COLUMN LIST:[{'Sensor_Name': 'Sensor-86', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-110', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-111', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-112', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-221', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-245', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-246', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-247', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-359', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-383', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-384', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-385', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-493', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-517', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-518', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-519', 'Column_Data': [100, 0]}]</t>
-        </is>
-      </c>
-    </row>
-    <row r="119">
-      <c r="A119" s="3" t="n">
-        <v>118</v>
-      </c>
-      <c r="B119" s="3" t="inlineStr">
-        <is>
-          <t>2024-09-21</t>
-        </is>
-      </c>
-      <c r="C119" s="3" t="inlineStr">
-        <is>
-          <t>wafer_31012024_090811.csv</t>
-        </is>
-      </c>
-      <c r="D119" s="3" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
-      </c>
-      <c r="E119" s="3" t="inlineStr">
-        <is>
-          <t>FILE NAME VALIDATION</t>
-        </is>
-      </c>
-      <c r="F119" s="3" t="inlineStr">
-        <is>
-          <t>FILE NAME VALIDATION COMPLETED</t>
-        </is>
-      </c>
-    </row>
-    <row r="120">
-      <c r="A120" s="3" t="n">
-        <v>119</v>
-      </c>
-      <c r="B120" s="3" t="inlineStr">
-        <is>
-          <t>2024-09-21</t>
-        </is>
-      </c>
-      <c r="C120" s="3" t="inlineStr">
-        <is>
-          <t>wafer_31012024_090811.csv</t>
-        </is>
-      </c>
-      <c r="D120" s="3" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
-      </c>
-      <c r="E120" s="3" t="inlineStr">
-        <is>
-          <t>NUMBER OF COLUMNS VALIDATION</t>
-        </is>
-      </c>
-      <c r="F120" s="3" t="inlineStr">
-        <is>
-          <t>NUMBER OF COLUMNS VALIDATION COMPLETED</t>
-        </is>
-      </c>
-    </row>
-    <row r="121">
-      <c r="A121" s="3" t="n">
-        <v>120</v>
-      </c>
-      <c r="B121" s="3" t="inlineStr">
-        <is>
-          <t>2024-09-21</t>
-        </is>
-      </c>
-      <c r="C121" s="3" t="inlineStr">
-        <is>
-          <t>wafer_31012024_090811.csv</t>
-        </is>
-      </c>
-      <c r="D121" s="3" t="inlineStr">
-        <is>
-          <t>Failed</t>
-        </is>
-      </c>
-      <c r="E121" s="3" t="inlineStr">
-        <is>
-          <t>COLUMNDATA_WHOLE_MISSING_VALIDATION</t>
-        </is>
-      </c>
-      <c r="F121" s="3" t="inlineStr">
-        <is>
-          <t>COLUMN DATA WHOLE MISSING VALIDATION FAILED, MISMATCH COLUMN LIST:[{'Sensor_Name': 'Sensor-86', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-110', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-111', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-112', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-221', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-245', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-246', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-247', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-359', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-383', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-384', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-385', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-493', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-517', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-518', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-519', 'Column_Data': [100, 0]}]</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
training and prediction process rechecked
</commit_message>
<xml_diff>
--- a/data/dashboard_data/prediction_validation_logs.xlsx
+++ b/data/dashboard_data/prediction_validation_logs.xlsx
@@ -493,7 +493,7 @@
       </c>
       <c r="B2" s="3" t="inlineStr">
         <is>
-          <t>2024-09-21</t>
+          <t>2024-09-26</t>
         </is>
       </c>
       <c r="C2" s="3" t="inlineStr">
@@ -523,7 +523,7 @@
       </c>
       <c r="B3" s="3" t="inlineStr">
         <is>
-          <t>2024-09-21</t>
+          <t>2024-09-26</t>
         </is>
       </c>
       <c r="C3" s="3" t="inlineStr">
@@ -553,7 +553,7 @@
       </c>
       <c r="B4" s="3" t="inlineStr">
         <is>
-          <t>2024-09-21</t>
+          <t>2024-09-26</t>
         </is>
       </c>
       <c r="C4" s="3" t="inlineStr">
@@ -583,7 +583,7 @@
       </c>
       <c r="B5" s="3" t="inlineStr">
         <is>
-          <t>2024-09-21</t>
+          <t>2024-09-26</t>
         </is>
       </c>
       <c r="C5" s="3" t="inlineStr">
@@ -613,7 +613,7 @@
       </c>
       <c r="B6" s="3" t="inlineStr">
         <is>
-          <t>2024-09-21</t>
+          <t>2024-09-26</t>
         </is>
       </c>
       <c r="C6" s="3" t="inlineStr">
@@ -643,7 +643,7 @@
       </c>
       <c r="B7" s="3" t="inlineStr">
         <is>
-          <t>2024-09-21</t>
+          <t>2024-09-26</t>
         </is>
       </c>
       <c r="C7" s="3" t="inlineStr">
@@ -673,7 +673,7 @@
       </c>
       <c r="B8" s="3" t="inlineStr">
         <is>
-          <t>2024-09-21</t>
+          <t>2024-09-26</t>
         </is>
       </c>
       <c r="C8" s="3" t="inlineStr">
@@ -703,7 +703,7 @@
       </c>
       <c r="B9" s="3" t="inlineStr">
         <is>
-          <t>2024-09-21</t>
+          <t>2024-09-26</t>
         </is>
       </c>
       <c r="C9" s="3" t="inlineStr">
@@ -733,7 +733,7 @@
       </c>
       <c r="B10" s="3" t="inlineStr">
         <is>
-          <t>2024-09-21</t>
+          <t>2024-09-26</t>
         </is>
       </c>
       <c r="C10" s="3" t="inlineStr">
@@ -763,7 +763,7 @@
       </c>
       <c r="B11" s="3" t="inlineStr">
         <is>
-          <t>2024-09-21</t>
+          <t>2024-09-26</t>
         </is>
       </c>
       <c r="C11" s="3" t="inlineStr">
@@ -793,7 +793,7 @@
       </c>
       <c r="B12" s="3" t="inlineStr">
         <is>
-          <t>2024-09-21</t>
+          <t>2024-09-26</t>
         </is>
       </c>
       <c r="C12" s="3" t="inlineStr">
@@ -823,7 +823,7 @@
       </c>
       <c r="B13" s="3" t="inlineStr">
         <is>
-          <t>2024-09-21</t>
+          <t>2024-09-26</t>
         </is>
       </c>
       <c r="C13" s="3" t="inlineStr">
@@ -853,7 +853,7 @@
       </c>
       <c r="B14" s="3" t="inlineStr">
         <is>
-          <t>2024-09-21</t>
+          <t>2024-09-26</t>
         </is>
       </c>
       <c r="C14" s="3" t="inlineStr">
@@ -883,7 +883,7 @@
       </c>
       <c r="B15" s="3" t="inlineStr">
         <is>
-          <t>2024-09-21</t>
+          <t>2024-09-26</t>
         </is>
       </c>
       <c r="C15" s="3" t="inlineStr">
@@ -913,7 +913,7 @@
       </c>
       <c r="B16" s="3" t="inlineStr">
         <is>
-          <t>2024-09-21</t>
+          <t>2024-09-26</t>
         </is>
       </c>
       <c r="C16" s="3" t="inlineStr">
@@ -943,7 +943,7 @@
       </c>
       <c r="B17" s="3" t="inlineStr">
         <is>
-          <t>2024-09-21</t>
+          <t>2024-09-26</t>
         </is>
       </c>
       <c r="C17" s="3" t="inlineStr">
@@ -973,7 +973,7 @@
       </c>
       <c r="B18" s="3" t="inlineStr">
         <is>
-          <t>2024-09-21</t>
+          <t>2024-09-26</t>
         </is>
       </c>
       <c r="C18" s="3" t="inlineStr">
@@ -1003,7 +1003,7 @@
       </c>
       <c r="B19" s="3" t="inlineStr">
         <is>
-          <t>2024-09-21</t>
+          <t>2024-09-26</t>
         </is>
       </c>
       <c r="C19" s="3" t="inlineStr">
@@ -1033,7 +1033,7 @@
       </c>
       <c r="B20" s="3" t="inlineStr">
         <is>
-          <t>2024-09-21</t>
+          <t>2024-09-26</t>
         </is>
       </c>
       <c r="C20" s="3" t="inlineStr">
@@ -1063,7 +1063,7 @@
       </c>
       <c r="B21" s="3" t="inlineStr">
         <is>
-          <t>2024-09-21</t>
+          <t>2024-09-26</t>
         </is>
       </c>
       <c r="C21" s="3" t="inlineStr">
@@ -1093,7 +1093,7 @@
       </c>
       <c r="B22" s="3" t="inlineStr">
         <is>
-          <t>2024-09-21</t>
+          <t>2024-09-26</t>
         </is>
       </c>
       <c r="C22" s="3" t="inlineStr">
@@ -1123,7 +1123,7 @@
       </c>
       <c r="B23" s="3" t="inlineStr">
         <is>
-          <t>2024-09-21</t>
+          <t>2024-09-26</t>
         </is>
       </c>
       <c r="C23" s="3" t="inlineStr">
@@ -1153,7 +1153,7 @@
       </c>
       <c r="B24" s="3" t="inlineStr">
         <is>
-          <t>2024-09-21</t>
+          <t>2024-09-26</t>
         </is>
       </c>
       <c r="C24" s="3" t="inlineStr">
@@ -1183,7 +1183,7 @@
       </c>
       <c r="B25" s="3" t="inlineStr">
         <is>
-          <t>2024-09-21</t>
+          <t>2024-09-26</t>
         </is>
       </c>
       <c r="C25" s="3" t="inlineStr">
@@ -1213,7 +1213,7 @@
       </c>
       <c r="B26" s="3" t="inlineStr">
         <is>
-          <t>2024-09-21</t>
+          <t>2024-09-26</t>
         </is>
       </c>
       <c r="C26" s="3" t="inlineStr">
@@ -1243,7 +1243,7 @@
       </c>
       <c r="B27" s="3" t="inlineStr">
         <is>
-          <t>2024-09-21</t>
+          <t>2024-09-26</t>
         </is>
       </c>
       <c r="C27" s="3" t="inlineStr">
@@ -1273,7 +1273,7 @@
       </c>
       <c r="B28" s="3" t="inlineStr">
         <is>
-          <t>2024-09-21</t>
+          <t>2024-09-26</t>
         </is>
       </c>
       <c r="C28" s="3" t="inlineStr">
@@ -1303,7 +1303,7 @@
       </c>
       <c r="B29" s="3" t="inlineStr">
         <is>
-          <t>2024-09-21</t>
+          <t>2024-09-26</t>
         </is>
       </c>
       <c r="C29" s="3" t="inlineStr">
@@ -1333,7 +1333,7 @@
       </c>
       <c r="B30" s="3" t="inlineStr">
         <is>
-          <t>2024-09-21</t>
+          <t>2024-09-26</t>
         </is>
       </c>
       <c r="C30" s="3" t="inlineStr">
@@ -1363,7 +1363,7 @@
       </c>
       <c r="B31" s="3" t="inlineStr">
         <is>
-          <t>2024-09-21</t>
+          <t>2024-09-26</t>
         </is>
       </c>
       <c r="C31" s="3" t="inlineStr">
@@ -1393,7 +1393,7 @@
       </c>
       <c r="B32" s="3" t="inlineStr">
         <is>
-          <t>2024-09-21</t>
+          <t>2024-09-26</t>
         </is>
       </c>
       <c r="C32" s="3" t="inlineStr">
@@ -1423,7 +1423,7 @@
       </c>
       <c r="B33" s="3" t="inlineStr">
         <is>
-          <t>2024-09-21</t>
+          <t>2024-09-26</t>
         </is>
       </c>
       <c r="C33" s="3" t="inlineStr">
@@ -1453,7 +1453,7 @@
       </c>
       <c r="B34" s="3" t="inlineStr">
         <is>
-          <t>2024-09-21</t>
+          <t>2024-09-26</t>
         </is>
       </c>
       <c r="C34" s="3" t="inlineStr">
@@ -1483,7 +1483,7 @@
       </c>
       <c r="B35" s="3" t="inlineStr">
         <is>
-          <t>2024-09-21</t>
+          <t>2024-09-26</t>
         </is>
       </c>
       <c r="C35" s="3" t="inlineStr">
@@ -1513,7 +1513,7 @@
       </c>
       <c r="B36" s="3" t="inlineStr">
         <is>
-          <t>2024-09-21</t>
+          <t>2024-09-26</t>
         </is>
       </c>
       <c r="C36" s="3" t="inlineStr">
@@ -1543,7 +1543,7 @@
       </c>
       <c r="B37" s="3" t="inlineStr">
         <is>
-          <t>2024-09-21</t>
+          <t>2024-09-26</t>
         </is>
       </c>
       <c r="C37" s="3" t="inlineStr">
@@ -1573,7 +1573,7 @@
       </c>
       <c r="B38" s="3" t="inlineStr">
         <is>
-          <t>2024-09-21</t>
+          <t>2024-09-26</t>
         </is>
       </c>
       <c r="C38" s="3" t="inlineStr">
@@ -1603,7 +1603,7 @@
       </c>
       <c r="B39" s="3" t="inlineStr">
         <is>
-          <t>2024-09-21</t>
+          <t>2024-09-26</t>
         </is>
       </c>
       <c r="C39" s="3" t="inlineStr">
@@ -1633,7 +1633,7 @@
       </c>
       <c r="B40" s="3" t="inlineStr">
         <is>
-          <t>2024-09-21</t>
+          <t>2024-09-26</t>
         </is>
       </c>
       <c r="C40" s="3" t="inlineStr">
@@ -1663,7 +1663,7 @@
       </c>
       <c r="B41" s="3" t="inlineStr">
         <is>
-          <t>2024-09-21</t>
+          <t>2024-09-26</t>
         </is>
       </c>
       <c r="C41" s="3" t="inlineStr">
@@ -1693,7 +1693,7 @@
       </c>
       <c r="B42" s="3" t="inlineStr">
         <is>
-          <t>2024-09-21</t>
+          <t>2024-09-26</t>
         </is>
       </c>
       <c r="C42" s="3" t="inlineStr">
@@ -1723,7 +1723,7 @@
       </c>
       <c r="B43" s="3" t="inlineStr">
         <is>
-          <t>2024-09-21</t>
+          <t>2024-09-26</t>
         </is>
       </c>
       <c r="C43" s="3" t="inlineStr">
@@ -1753,7 +1753,7 @@
       </c>
       <c r="B44" s="3" t="inlineStr">
         <is>
-          <t>2024-09-21</t>
+          <t>2024-09-26</t>
         </is>
       </c>
       <c r="C44" s="3" t="inlineStr">
@@ -1783,7 +1783,7 @@
       </c>
       <c r="B45" s="3" t="inlineStr">
         <is>
-          <t>2024-09-21</t>
+          <t>2024-09-26</t>
         </is>
       </c>
       <c r="C45" s="3" t="inlineStr">
@@ -1813,7 +1813,7 @@
       </c>
       <c r="B46" s="3" t="inlineStr">
         <is>
-          <t>2024-09-21</t>
+          <t>2024-09-26</t>
         </is>
       </c>
       <c r="C46" s="3" t="inlineStr">
@@ -1843,7 +1843,7 @@
       </c>
       <c r="B47" s="3" t="inlineStr">
         <is>
-          <t>2024-09-21</t>
+          <t>2024-09-26</t>
         </is>
       </c>
       <c r="C47" s="3" t="inlineStr">
@@ -1873,7 +1873,7 @@
       </c>
       <c r="B48" s="3" t="inlineStr">
         <is>
-          <t>2024-09-21</t>
+          <t>2024-09-26</t>
         </is>
       </c>
       <c r="C48" s="3" t="inlineStr">
@@ -1903,7 +1903,7 @@
       </c>
       <c r="B49" s="3" t="inlineStr">
         <is>
-          <t>2024-09-21</t>
+          <t>2024-09-26</t>
         </is>
       </c>
       <c r="C49" s="3" t="inlineStr">
@@ -1933,7 +1933,7 @@
       </c>
       <c r="B50" s="3" t="inlineStr">
         <is>
-          <t>2024-09-21</t>
+          <t>2024-09-26</t>
         </is>
       </c>
       <c r="C50" s="3" t="inlineStr">
@@ -1963,7 +1963,7 @@
       </c>
       <c r="B51" s="3" t="inlineStr">
         <is>
-          <t>2024-09-21</t>
+          <t>2024-09-26</t>
         </is>
       </c>
       <c r="C51" s="3" t="inlineStr">
@@ -1993,7 +1993,7 @@
       </c>
       <c r="B52" s="3" t="inlineStr">
         <is>
-          <t>2024-09-21</t>
+          <t>2024-09-26</t>
         </is>
       </c>
       <c r="C52" s="3" t="inlineStr">
@@ -2023,7 +2023,7 @@
       </c>
       <c r="B53" s="3" t="inlineStr">
         <is>
-          <t>2024-09-21</t>
+          <t>2024-09-26</t>
         </is>
       </c>
       <c r="C53" s="3" t="inlineStr">
@@ -2053,7 +2053,7 @@
       </c>
       <c r="B54" s="3" t="inlineStr">
         <is>
-          <t>2024-09-21</t>
+          <t>2024-09-26</t>
         </is>
       </c>
       <c r="C54" s="3" t="inlineStr">
@@ -2083,7 +2083,7 @@
       </c>
       <c r="B55" s="3" t="inlineStr">
         <is>
-          <t>2024-09-21</t>
+          <t>2024-09-26</t>
         </is>
       </c>
       <c r="C55" s="3" t="inlineStr">
@@ -2113,7 +2113,7 @@
       </c>
       <c r="B56" s="3" t="inlineStr">
         <is>
-          <t>2024-09-21</t>
+          <t>2024-09-26</t>
         </is>
       </c>
       <c r="C56" s="3" t="inlineStr">
@@ -2143,7 +2143,7 @@
       </c>
       <c r="B57" s="3" t="inlineStr">
         <is>
-          <t>2024-09-21</t>
+          <t>2024-09-26</t>
         </is>
       </c>
       <c r="C57" s="3" t="inlineStr">
@@ -2173,7 +2173,7 @@
       </c>
       <c r="B58" s="3" t="inlineStr">
         <is>
-          <t>2024-09-21</t>
+          <t>2024-09-26</t>
         </is>
       </c>
       <c r="C58" s="3" t="inlineStr">
@@ -2203,7 +2203,7 @@
       </c>
       <c r="B59" s="3" t="inlineStr">
         <is>
-          <t>2024-09-21</t>
+          <t>2024-09-26</t>
         </is>
       </c>
       <c r="C59" s="3" t="inlineStr">
@@ -2233,7 +2233,7 @@
       </c>
       <c r="B60" s="3" t="inlineStr">
         <is>
-          <t>2024-09-21</t>
+          <t>2024-09-26</t>
         </is>
       </c>
       <c r="C60" s="3" t="inlineStr">
@@ -2263,7 +2263,7 @@
       </c>
       <c r="B61" s="3" t="inlineStr">
         <is>
-          <t>2024-09-21</t>
+          <t>2024-09-26</t>
         </is>
       </c>
       <c r="C61" s="3" t="inlineStr">

</xml_diff>

<commit_message>
2nd rechecked training and prediction process
</commit_message>
<xml_diff>
--- a/data/dashboard_data/prediction_validation_logs.xlsx
+++ b/data/dashboard_data/prediction_validation_logs.xlsx
@@ -493,7 +493,7 @@
       </c>
       <c r="B2" s="3" t="inlineStr">
         <is>
-          <t>2024-09-26</t>
+          <t>2024-10-01</t>
         </is>
       </c>
       <c r="C2" s="3" t="inlineStr">
@@ -523,7 +523,7 @@
       </c>
       <c r="B3" s="3" t="inlineStr">
         <is>
-          <t>2024-09-26</t>
+          <t>2024-10-01</t>
         </is>
       </c>
       <c r="C3" s="3" t="inlineStr">
@@ -553,7 +553,7 @@
       </c>
       <c r="B4" s="3" t="inlineStr">
         <is>
-          <t>2024-09-26</t>
+          <t>2024-10-01</t>
         </is>
       </c>
       <c r="C4" s="3" t="inlineStr">
@@ -583,7 +583,7 @@
       </c>
       <c r="B5" s="3" t="inlineStr">
         <is>
-          <t>2024-09-26</t>
+          <t>2024-10-01</t>
         </is>
       </c>
       <c r="C5" s="3" t="inlineStr">
@@ -613,7 +613,7 @@
       </c>
       <c r="B6" s="3" t="inlineStr">
         <is>
-          <t>2024-09-26</t>
+          <t>2024-10-01</t>
         </is>
       </c>
       <c r="C6" s="3" t="inlineStr">
@@ -643,7 +643,7 @@
       </c>
       <c r="B7" s="3" t="inlineStr">
         <is>
-          <t>2024-09-26</t>
+          <t>2024-10-01</t>
         </is>
       </c>
       <c r="C7" s="3" t="inlineStr">
@@ -673,7 +673,7 @@
       </c>
       <c r="B8" s="3" t="inlineStr">
         <is>
-          <t>2024-09-26</t>
+          <t>2024-10-01</t>
         </is>
       </c>
       <c r="C8" s="3" t="inlineStr">
@@ -703,7 +703,7 @@
       </c>
       <c r="B9" s="3" t="inlineStr">
         <is>
-          <t>2024-09-26</t>
+          <t>2024-10-01</t>
         </is>
       </c>
       <c r="C9" s="3" t="inlineStr">
@@ -733,7 +733,7 @@
       </c>
       <c r="B10" s="3" t="inlineStr">
         <is>
-          <t>2024-09-26</t>
+          <t>2024-10-01</t>
         </is>
       </c>
       <c r="C10" s="3" t="inlineStr">
@@ -763,7 +763,7 @@
       </c>
       <c r="B11" s="3" t="inlineStr">
         <is>
-          <t>2024-09-26</t>
+          <t>2024-10-01</t>
         </is>
       </c>
       <c r="C11" s="3" t="inlineStr">
@@ -793,7 +793,7 @@
       </c>
       <c r="B12" s="3" t="inlineStr">
         <is>
-          <t>2024-09-26</t>
+          <t>2024-10-01</t>
         </is>
       </c>
       <c r="C12" s="3" t="inlineStr">
@@ -823,7 +823,7 @@
       </c>
       <c r="B13" s="3" t="inlineStr">
         <is>
-          <t>2024-09-26</t>
+          <t>2024-10-01</t>
         </is>
       </c>
       <c r="C13" s="3" t="inlineStr">
@@ -853,7 +853,7 @@
       </c>
       <c r="B14" s="3" t="inlineStr">
         <is>
-          <t>2024-09-26</t>
+          <t>2024-10-01</t>
         </is>
       </c>
       <c r="C14" s="3" t="inlineStr">
@@ -883,7 +883,7 @@
       </c>
       <c r="B15" s="3" t="inlineStr">
         <is>
-          <t>2024-09-26</t>
+          <t>2024-10-01</t>
         </is>
       </c>
       <c r="C15" s="3" t="inlineStr">
@@ -913,7 +913,7 @@
       </c>
       <c r="B16" s="3" t="inlineStr">
         <is>
-          <t>2024-09-26</t>
+          <t>2024-10-01</t>
         </is>
       </c>
       <c r="C16" s="3" t="inlineStr">
@@ -943,7 +943,7 @@
       </c>
       <c r="B17" s="3" t="inlineStr">
         <is>
-          <t>2024-09-26</t>
+          <t>2024-10-01</t>
         </is>
       </c>
       <c r="C17" s="3" t="inlineStr">
@@ -973,7 +973,7 @@
       </c>
       <c r="B18" s="3" t="inlineStr">
         <is>
-          <t>2024-09-26</t>
+          <t>2024-10-01</t>
         </is>
       </c>
       <c r="C18" s="3" t="inlineStr">
@@ -1003,7 +1003,7 @@
       </c>
       <c r="B19" s="3" t="inlineStr">
         <is>
-          <t>2024-09-26</t>
+          <t>2024-10-01</t>
         </is>
       </c>
       <c r="C19" s="3" t="inlineStr">
@@ -1033,7 +1033,7 @@
       </c>
       <c r="B20" s="3" t="inlineStr">
         <is>
-          <t>2024-09-26</t>
+          <t>2024-10-01</t>
         </is>
       </c>
       <c r="C20" s="3" t="inlineStr">
@@ -1063,7 +1063,7 @@
       </c>
       <c r="B21" s="3" t="inlineStr">
         <is>
-          <t>2024-09-26</t>
+          <t>2024-10-01</t>
         </is>
       </c>
       <c r="C21" s="3" t="inlineStr">
@@ -1093,7 +1093,7 @@
       </c>
       <c r="B22" s="3" t="inlineStr">
         <is>
-          <t>2024-09-26</t>
+          <t>2024-10-01</t>
         </is>
       </c>
       <c r="C22" s="3" t="inlineStr">
@@ -1123,7 +1123,7 @@
       </c>
       <c r="B23" s="3" t="inlineStr">
         <is>
-          <t>2024-09-26</t>
+          <t>2024-10-01</t>
         </is>
       </c>
       <c r="C23" s="3" t="inlineStr">
@@ -1153,7 +1153,7 @@
       </c>
       <c r="B24" s="3" t="inlineStr">
         <is>
-          <t>2024-09-26</t>
+          <t>2024-10-01</t>
         </is>
       </c>
       <c r="C24" s="3" t="inlineStr">
@@ -1183,7 +1183,7 @@
       </c>
       <c r="B25" s="3" t="inlineStr">
         <is>
-          <t>2024-09-26</t>
+          <t>2024-10-01</t>
         </is>
       </c>
       <c r="C25" s="3" t="inlineStr">
@@ -1213,7 +1213,7 @@
       </c>
       <c r="B26" s="3" t="inlineStr">
         <is>
-          <t>2024-09-26</t>
+          <t>2024-10-01</t>
         </is>
       </c>
       <c r="C26" s="3" t="inlineStr">
@@ -1243,7 +1243,7 @@
       </c>
       <c r="B27" s="3" t="inlineStr">
         <is>
-          <t>2024-09-26</t>
+          <t>2024-10-01</t>
         </is>
       </c>
       <c r="C27" s="3" t="inlineStr">
@@ -1273,7 +1273,7 @@
       </c>
       <c r="B28" s="3" t="inlineStr">
         <is>
-          <t>2024-09-26</t>
+          <t>2024-10-01</t>
         </is>
       </c>
       <c r="C28" s="3" t="inlineStr">
@@ -1303,7 +1303,7 @@
       </c>
       <c r="B29" s="3" t="inlineStr">
         <is>
-          <t>2024-09-26</t>
+          <t>2024-10-01</t>
         </is>
       </c>
       <c r="C29" s="3" t="inlineStr">
@@ -1333,7 +1333,7 @@
       </c>
       <c r="B30" s="3" t="inlineStr">
         <is>
-          <t>2024-09-26</t>
+          <t>2024-10-01</t>
         </is>
       </c>
       <c r="C30" s="3" t="inlineStr">
@@ -1363,7 +1363,7 @@
       </c>
       <c r="B31" s="3" t="inlineStr">
         <is>
-          <t>2024-09-26</t>
+          <t>2024-10-01</t>
         </is>
       </c>
       <c r="C31" s="3" t="inlineStr">
@@ -1393,7 +1393,7 @@
       </c>
       <c r="B32" s="3" t="inlineStr">
         <is>
-          <t>2024-09-26</t>
+          <t>2024-10-01</t>
         </is>
       </c>
       <c r="C32" s="3" t="inlineStr">
@@ -1423,7 +1423,7 @@
       </c>
       <c r="B33" s="3" t="inlineStr">
         <is>
-          <t>2024-09-26</t>
+          <t>2024-10-01</t>
         </is>
       </c>
       <c r="C33" s="3" t="inlineStr">
@@ -1453,7 +1453,7 @@
       </c>
       <c r="B34" s="3" t="inlineStr">
         <is>
-          <t>2024-09-26</t>
+          <t>2024-10-01</t>
         </is>
       </c>
       <c r="C34" s="3" t="inlineStr">
@@ -1483,7 +1483,7 @@
       </c>
       <c r="B35" s="3" t="inlineStr">
         <is>
-          <t>2024-09-26</t>
+          <t>2024-10-01</t>
         </is>
       </c>
       <c r="C35" s="3" t="inlineStr">
@@ -1513,7 +1513,7 @@
       </c>
       <c r="B36" s="3" t="inlineStr">
         <is>
-          <t>2024-09-26</t>
+          <t>2024-10-01</t>
         </is>
       </c>
       <c r="C36" s="3" t="inlineStr">
@@ -1543,7 +1543,7 @@
       </c>
       <c r="B37" s="3" t="inlineStr">
         <is>
-          <t>2024-09-26</t>
+          <t>2024-10-01</t>
         </is>
       </c>
       <c r="C37" s="3" t="inlineStr">
@@ -1573,7 +1573,7 @@
       </c>
       <c r="B38" s="3" t="inlineStr">
         <is>
-          <t>2024-09-26</t>
+          <t>2024-10-01</t>
         </is>
       </c>
       <c r="C38" s="3" t="inlineStr">
@@ -1603,7 +1603,7 @@
       </c>
       <c r="B39" s="3" t="inlineStr">
         <is>
-          <t>2024-09-26</t>
+          <t>2024-10-01</t>
         </is>
       </c>
       <c r="C39" s="3" t="inlineStr">
@@ -1633,7 +1633,7 @@
       </c>
       <c r="B40" s="3" t="inlineStr">
         <is>
-          <t>2024-09-26</t>
+          <t>2024-10-01</t>
         </is>
       </c>
       <c r="C40" s="3" t="inlineStr">
@@ -1663,7 +1663,7 @@
       </c>
       <c r="B41" s="3" t="inlineStr">
         <is>
-          <t>2024-09-26</t>
+          <t>2024-10-01</t>
         </is>
       </c>
       <c r="C41" s="3" t="inlineStr">
@@ -1693,7 +1693,7 @@
       </c>
       <c r="B42" s="3" t="inlineStr">
         <is>
-          <t>2024-09-26</t>
+          <t>2024-10-01</t>
         </is>
       </c>
       <c r="C42" s="3" t="inlineStr">
@@ -1723,7 +1723,7 @@
       </c>
       <c r="B43" s="3" t="inlineStr">
         <is>
-          <t>2024-09-26</t>
+          <t>2024-10-01</t>
         </is>
       </c>
       <c r="C43" s="3" t="inlineStr">
@@ -1753,7 +1753,7 @@
       </c>
       <c r="B44" s="3" t="inlineStr">
         <is>
-          <t>2024-09-26</t>
+          <t>2024-10-01</t>
         </is>
       </c>
       <c r="C44" s="3" t="inlineStr">
@@ -1783,7 +1783,7 @@
       </c>
       <c r="B45" s="3" t="inlineStr">
         <is>
-          <t>2024-09-26</t>
+          <t>2024-10-01</t>
         </is>
       </c>
       <c r="C45" s="3" t="inlineStr">
@@ -1813,7 +1813,7 @@
       </c>
       <c r="B46" s="3" t="inlineStr">
         <is>
-          <t>2024-09-26</t>
+          <t>2024-10-01</t>
         </is>
       </c>
       <c r="C46" s="3" t="inlineStr">
@@ -1843,7 +1843,7 @@
       </c>
       <c r="B47" s="3" t="inlineStr">
         <is>
-          <t>2024-09-26</t>
+          <t>2024-10-01</t>
         </is>
       </c>
       <c r="C47" s="3" t="inlineStr">
@@ -1873,7 +1873,7 @@
       </c>
       <c r="B48" s="3" t="inlineStr">
         <is>
-          <t>2024-09-26</t>
+          <t>2024-10-01</t>
         </is>
       </c>
       <c r="C48" s="3" t="inlineStr">
@@ -1903,7 +1903,7 @@
       </c>
       <c r="B49" s="3" t="inlineStr">
         <is>
-          <t>2024-09-26</t>
+          <t>2024-10-01</t>
         </is>
       </c>
       <c r="C49" s="3" t="inlineStr">
@@ -1933,7 +1933,7 @@
       </c>
       <c r="B50" s="3" t="inlineStr">
         <is>
-          <t>2024-09-26</t>
+          <t>2024-10-01</t>
         </is>
       </c>
       <c r="C50" s="3" t="inlineStr">
@@ -1963,7 +1963,7 @@
       </c>
       <c r="B51" s="3" t="inlineStr">
         <is>
-          <t>2024-09-26</t>
+          <t>2024-10-01</t>
         </is>
       </c>
       <c r="C51" s="3" t="inlineStr">
@@ -1993,7 +1993,7 @@
       </c>
       <c r="B52" s="3" t="inlineStr">
         <is>
-          <t>2024-09-26</t>
+          <t>2024-10-01</t>
         </is>
       </c>
       <c r="C52" s="3" t="inlineStr">
@@ -2023,7 +2023,7 @@
       </c>
       <c r="B53" s="3" t="inlineStr">
         <is>
-          <t>2024-09-26</t>
+          <t>2024-10-01</t>
         </is>
       </c>
       <c r="C53" s="3" t="inlineStr">
@@ -2053,7 +2053,7 @@
       </c>
       <c r="B54" s="3" t="inlineStr">
         <is>
-          <t>2024-09-26</t>
+          <t>2024-10-01</t>
         </is>
       </c>
       <c r="C54" s="3" t="inlineStr">
@@ -2083,7 +2083,7 @@
       </c>
       <c r="B55" s="3" t="inlineStr">
         <is>
-          <t>2024-09-26</t>
+          <t>2024-10-01</t>
         </is>
       </c>
       <c r="C55" s="3" t="inlineStr">
@@ -2113,7 +2113,7 @@
       </c>
       <c r="B56" s="3" t="inlineStr">
         <is>
-          <t>2024-09-26</t>
+          <t>2024-10-01</t>
         </is>
       </c>
       <c r="C56" s="3" t="inlineStr">
@@ -2143,7 +2143,7 @@
       </c>
       <c r="B57" s="3" t="inlineStr">
         <is>
-          <t>2024-09-26</t>
+          <t>2024-10-01</t>
         </is>
       </c>
       <c r="C57" s="3" t="inlineStr">
@@ -2173,7 +2173,7 @@
       </c>
       <c r="B58" s="3" t="inlineStr">
         <is>
-          <t>2024-09-26</t>
+          <t>2024-10-01</t>
         </is>
       </c>
       <c r="C58" s="3" t="inlineStr">
@@ -2203,7 +2203,7 @@
       </c>
       <c r="B59" s="3" t="inlineStr">
         <is>
-          <t>2024-09-26</t>
+          <t>2024-10-01</t>
         </is>
       </c>
       <c r="C59" s="3" t="inlineStr">
@@ -2233,7 +2233,7 @@
       </c>
       <c r="B60" s="3" t="inlineStr">
         <is>
-          <t>2024-09-26</t>
+          <t>2024-10-01</t>
         </is>
       </c>
       <c r="C60" s="3" t="inlineStr">
@@ -2263,7 +2263,7 @@
       </c>
       <c r="B61" s="3" t="inlineStr">
         <is>
-          <t>2024-09-26</t>
+          <t>2024-10-01</t>
         </is>
       </c>
       <c r="C61" s="3" t="inlineStr">

</xml_diff>

<commit_message>
prediction and training process completed
</commit_message>
<xml_diff>
--- a/data/dashboard_data/prediction_validation_logs.xlsx
+++ b/data/dashboard_data/prediction_validation_logs.xlsx
@@ -439,7 +439,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F61"/>
+  <dimension ref="A1:F43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -449,10 +449,10 @@
   <cols>
     <col width="6" customWidth="1" min="1" max="1"/>
     <col width="12" customWidth="1" min="2" max="2"/>
-    <col width="27" customWidth="1" min="3" max="3"/>
+    <col width="28" customWidth="1" min="3" max="3"/>
     <col width="8" customWidth="1" min="4" max="4"/>
     <col width="37" customWidth="1" min="5" max="5"/>
-    <col width="963" customWidth="1" min="6" max="6"/>
+    <col width="14427" customWidth="1" min="6" max="6"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -493,17 +493,17 @@
       </c>
       <c r="B2" s="3" t="inlineStr">
         <is>
-          <t>2024-10-01</t>
+          <t>2024-10-10</t>
         </is>
       </c>
       <c r="C2" s="3" t="inlineStr">
         <is>
-          <t>wafer_07012024_041011.csv</t>
+          <t>wafer_150102023_122518.csv</t>
         </is>
       </c>
       <c r="D2" s="3" t="inlineStr">
         <is>
-          <t>Passed</t>
+          <t>Failed</t>
         </is>
       </c>
       <c r="E2" s="3" t="inlineStr">
@@ -513,7 +513,7 @@
       </c>
       <c r="F2" s="3" t="inlineStr">
         <is>
-          <t>FILE NAME VALIDATION COMPLETED</t>
+          <t>FILE NAME VALIDATION FAILED</t>
         </is>
       </c>
     </row>
@@ -523,27 +523,27 @@
       </c>
       <c r="B3" s="3" t="inlineStr">
         <is>
-          <t>2024-10-01</t>
+          <t>2024-10-10</t>
         </is>
       </c>
       <c r="C3" s="3" t="inlineStr">
         <is>
-          <t>wafer_07012024_041011.csv</t>
+          <t>wafer_150112023_122518.csv</t>
         </is>
       </c>
       <c r="D3" s="3" t="inlineStr">
         <is>
-          <t>Passed</t>
+          <t>Failed</t>
         </is>
       </c>
       <c r="E3" s="3" t="inlineStr">
         <is>
-          <t>NUMBER OF COLUMNS VALIDATION</t>
+          <t>FILE NAME VALIDATION</t>
         </is>
       </c>
       <c r="F3" s="3" t="inlineStr">
         <is>
-          <t>NUMBER OF COLUMNS VALIDATION COMPLETED</t>
+          <t>FILE NAME VALIDATION FAILED</t>
         </is>
       </c>
     </row>
@@ -553,27 +553,27 @@
       </c>
       <c r="B4" s="3" t="inlineStr">
         <is>
-          <t>2024-10-01</t>
+          <t>2024-10-10</t>
         </is>
       </c>
       <c r="C4" s="3" t="inlineStr">
         <is>
-          <t>wafer_07012024_041011.csv</t>
+          <t>wafer_15012023_122518.csv</t>
         </is>
       </c>
       <c r="D4" s="3" t="inlineStr">
         <is>
-          <t>Failed</t>
+          <t>Passed</t>
         </is>
       </c>
       <c r="E4" s="3" t="inlineStr">
         <is>
-          <t>COLUMNDATA_WHOLE_MISSING_VALIDATION</t>
+          <t>FILE NAME VALIDATION</t>
         </is>
       </c>
       <c r="F4" s="3" t="inlineStr">
         <is>
-          <t>COLUMN DATA WHOLE MISSING VALIDATION FAILED, MISMATCH COLUMN LIST:[{'Sensor_Name': 'Sensor-86', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-110', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-111', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-112', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-221', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-245', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-246', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-247', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-359', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-383', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-384', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-385', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-493', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-517', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-518', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-519', 'Column_Data': [100, 0]}]</t>
+          <t>FILE NAME VALIDATION COMPLETED</t>
         </is>
       </c>
     </row>
@@ -583,12 +583,12 @@
       </c>
       <c r="B5" s="3" t="inlineStr">
         <is>
-          <t>2024-10-01</t>
+          <t>2024-10-10</t>
         </is>
       </c>
       <c r="C5" s="3" t="inlineStr">
         <is>
-          <t>wafer_13012024_090817.csv</t>
+          <t>wafer_15012023_122518.csv</t>
         </is>
       </c>
       <c r="D5" s="3" t="inlineStr">
@@ -598,12 +598,12 @@
       </c>
       <c r="E5" s="3" t="inlineStr">
         <is>
-          <t>FILE NAME VALIDATION</t>
+          <t>NUMBER OF COLUMNS VALIDATION</t>
         </is>
       </c>
       <c r="F5" s="3" t="inlineStr">
         <is>
-          <t>FILE NAME VALIDATION COMPLETED</t>
+          <t>NUMBER OF COLUMNS VALIDATION COMPLETED</t>
         </is>
       </c>
     </row>
@@ -613,12 +613,12 @@
       </c>
       <c r="B6" s="3" t="inlineStr">
         <is>
-          <t>2024-10-01</t>
+          <t>2024-10-10</t>
         </is>
       </c>
       <c r="C6" s="3" t="inlineStr">
         <is>
-          <t>wafer_13012024_090817.csv</t>
+          <t>wafer_15012023_122518.csv</t>
         </is>
       </c>
       <c r="D6" s="3" t="inlineStr">
@@ -628,12 +628,12 @@
       </c>
       <c r="E6" s="3" t="inlineStr">
         <is>
-          <t>NUMBER OF COLUMNS VALIDATION</t>
+          <t>COLUMNDATA_WHOLE_MISSING_VALIDATION</t>
         </is>
       </c>
       <c r="F6" s="3" t="inlineStr">
         <is>
-          <t>NUMBER OF COLUMNS VALIDATION COMPLETED</t>
+          <t>COLUMN DATA WHOLE MISSING VALIDATION COMPLETED</t>
         </is>
       </c>
     </row>
@@ -643,12 +643,12 @@
       </c>
       <c r="B7" s="3" t="inlineStr">
         <is>
-          <t>2024-10-01</t>
+          <t>2024-10-10</t>
         </is>
       </c>
       <c r="C7" s="3" t="inlineStr">
         <is>
-          <t>wafer_13012024_090817.csv</t>
+          <t>wafer_15012023_122518.csv</t>
         </is>
       </c>
       <c r="D7" s="3" t="inlineStr">
@@ -658,12 +658,12 @@
       </c>
       <c r="E7" s="3" t="inlineStr">
         <is>
-          <t>COLUMNDATA_WHOLE_MISSING_VALIDATION</t>
+          <t>COLUMN DATA VALIDATION</t>
         </is>
       </c>
       <c r="F7" s="3" t="inlineStr">
         <is>
-          <t>COLUMN DATA WHOLE MISSING VALIDATION COMPLETED</t>
+          <t>COLUMN DATA VALIDATION COMPLETED</t>
         </is>
       </c>
     </row>
@@ -673,27 +673,27 @@
       </c>
       <c r="B8" s="3" t="inlineStr">
         <is>
-          <t>2024-10-01</t>
+          <t>2024-10-10</t>
         </is>
       </c>
       <c r="C8" s="3" t="inlineStr">
         <is>
-          <t>wafer_13012024_090817.csv</t>
+          <t>wafer_150122023_122518.csv</t>
         </is>
       </c>
       <c r="D8" s="3" t="inlineStr">
         <is>
-          <t>Passed</t>
+          <t>Failed</t>
         </is>
       </c>
       <c r="E8" s="3" t="inlineStr">
         <is>
-          <t>COLUMN DATA VALIDATION</t>
+          <t>FILE NAME VALIDATION</t>
         </is>
       </c>
       <c r="F8" s="3" t="inlineStr">
         <is>
-          <t>COLUMN DATA VALIDATION COMPLETED</t>
+          <t>FILE NAME VALIDATION FAILED</t>
         </is>
       </c>
     </row>
@@ -703,12 +703,12 @@
       </c>
       <c r="B9" s="3" t="inlineStr">
         <is>
-          <t>2024-10-01</t>
+          <t>2024-10-10</t>
         </is>
       </c>
       <c r="C9" s="3" t="inlineStr">
         <is>
-          <t>Wafer_13012024_141000.csv</t>
+          <t>wafer_150132023_122518.csv</t>
         </is>
       </c>
       <c r="D9" s="3" t="inlineStr">
@@ -733,12 +733,12 @@
       </c>
       <c r="B10" s="3" t="inlineStr">
         <is>
-          <t>2024-10-01</t>
+          <t>2024-10-10</t>
         </is>
       </c>
       <c r="C10" s="3" t="inlineStr">
         <is>
-          <t>Wafer_14012024_113045.csv</t>
+          <t>wafer_150142023_122518.csv</t>
         </is>
       </c>
       <c r="D10" s="3" t="inlineStr">
@@ -763,12 +763,12 @@
       </c>
       <c r="B11" s="3" t="inlineStr">
         <is>
-          <t>2024-10-01</t>
+          <t>2024-10-10</t>
         </is>
       </c>
       <c r="C11" s="3" t="inlineStr">
         <is>
-          <t>Wafer_15010_130532.csv</t>
+          <t>wafer_150152023_122518.csv</t>
         </is>
       </c>
       <c r="D11" s="3" t="inlineStr">
@@ -793,17 +793,17 @@
       </c>
       <c r="B12" s="3" t="inlineStr">
         <is>
-          <t>2024-10-01</t>
+          <t>2024-10-10</t>
         </is>
       </c>
       <c r="C12" s="3" t="inlineStr">
         <is>
-          <t>wafer_16012024_051629.csv</t>
+          <t>wafer_150162023_122518.csv</t>
         </is>
       </c>
       <c r="D12" s="3" t="inlineStr">
         <is>
-          <t>Passed</t>
+          <t>Failed</t>
         </is>
       </c>
       <c r="E12" s="3" t="inlineStr">
@@ -813,7 +813,7 @@
       </c>
       <c r="F12" s="3" t="inlineStr">
         <is>
-          <t>FILE NAME VALIDATION COMPLETED</t>
+          <t>FILE NAME VALIDATION FAILED</t>
         </is>
       </c>
     </row>
@@ -823,27 +823,27 @@
       </c>
       <c r="B13" s="3" t="inlineStr">
         <is>
-          <t>2024-10-01</t>
+          <t>2024-10-10</t>
         </is>
       </c>
       <c r="C13" s="3" t="inlineStr">
         <is>
-          <t>wafer_16012024_051629.csv</t>
+          <t>wafer_150172023_122518.csv</t>
         </is>
       </c>
       <c r="D13" s="3" t="inlineStr">
         <is>
-          <t>Passed</t>
+          <t>Failed</t>
         </is>
       </c>
       <c r="E13" s="3" t="inlineStr">
         <is>
-          <t>NUMBER OF COLUMNS VALIDATION</t>
+          <t>FILE NAME VALIDATION</t>
         </is>
       </c>
       <c r="F13" s="3" t="inlineStr">
         <is>
-          <t>NUMBER OF COLUMNS VALIDATION COMPLETED</t>
+          <t>FILE NAME VALIDATION FAILED</t>
         </is>
       </c>
     </row>
@@ -853,12 +853,12 @@
       </c>
       <c r="B14" s="3" t="inlineStr">
         <is>
-          <t>2024-10-01</t>
+          <t>2024-10-10</t>
         </is>
       </c>
       <c r="C14" s="3" t="inlineStr">
         <is>
-          <t>wafer_16012024_051629.csv</t>
+          <t>wafer_15022023_122518.csv</t>
         </is>
       </c>
       <c r="D14" s="3" t="inlineStr">
@@ -868,12 +868,12 @@
       </c>
       <c r="E14" s="3" t="inlineStr">
         <is>
-          <t>COLUMNDATA_WHOLE_MISSING_VALIDATION</t>
+          <t>FILE NAME VALIDATION</t>
         </is>
       </c>
       <c r="F14" s="3" t="inlineStr">
         <is>
-          <t>COLUMN DATA WHOLE MISSING VALIDATION COMPLETED</t>
+          <t>FILE NAME VALIDATION COMPLETED</t>
         </is>
       </c>
     </row>
@@ -883,12 +883,12 @@
       </c>
       <c r="B15" s="3" t="inlineStr">
         <is>
-          <t>2024-10-01</t>
+          <t>2024-10-10</t>
         </is>
       </c>
       <c r="C15" s="3" t="inlineStr">
         <is>
-          <t>wafer_16012024_051629.csv</t>
+          <t>wafer_15022023_122518.csv</t>
         </is>
       </c>
       <c r="D15" s="3" t="inlineStr">
@@ -898,12 +898,12 @@
       </c>
       <c r="E15" s="3" t="inlineStr">
         <is>
-          <t>COLUMN DATA VALIDATION</t>
+          <t>NUMBER OF COLUMNS VALIDATION</t>
         </is>
       </c>
       <c r="F15" s="3" t="inlineStr">
         <is>
-          <t>COLUMN DATA VALIDATION COMPLETED</t>
+          <t>NUMBER OF COLUMNS VALIDATION COMPLETED</t>
         </is>
       </c>
     </row>
@@ -913,12 +913,12 @@
       </c>
       <c r="B16" s="3" t="inlineStr">
         <is>
-          <t>2024-10-01</t>
+          <t>2024-10-10</t>
         </is>
       </c>
       <c r="C16" s="3" t="inlineStr">
         <is>
-          <t>wafer_20012024_090819.csv</t>
+          <t>wafer_15022023_122518.csv</t>
         </is>
       </c>
       <c r="D16" s="3" t="inlineStr">
@@ -928,12 +928,12 @@
       </c>
       <c r="E16" s="3" t="inlineStr">
         <is>
-          <t>FILE NAME VALIDATION</t>
+          <t>COLUMNDATA_WHOLE_MISSING_VALIDATION</t>
         </is>
       </c>
       <c r="F16" s="3" t="inlineStr">
         <is>
-          <t>FILE NAME VALIDATION COMPLETED</t>
+          <t>COLUMN DATA WHOLE MISSING VALIDATION COMPLETED</t>
         </is>
       </c>
     </row>
@@ -943,12 +943,12 @@
       </c>
       <c r="B17" s="3" t="inlineStr">
         <is>
-          <t>2024-10-01</t>
+          <t>2024-10-10</t>
         </is>
       </c>
       <c r="C17" s="3" t="inlineStr">
         <is>
-          <t>wafer_20012024_090819.csv</t>
+          <t>wafer_15022023_122518.csv</t>
         </is>
       </c>
       <c r="D17" s="3" t="inlineStr">
@@ -958,12 +958,12 @@
       </c>
       <c r="E17" s="3" t="inlineStr">
         <is>
-          <t>NUMBER OF COLUMNS VALIDATION</t>
+          <t>COLUMN DATA VALIDATION</t>
         </is>
       </c>
       <c r="F17" s="3" t="inlineStr">
         <is>
-          <t>NUMBER OF COLUMNS VALIDATION COMPLETED</t>
+          <t>COLUMN DATA VALIDATION COMPLETED</t>
         </is>
       </c>
     </row>
@@ -973,27 +973,27 @@
       </c>
       <c r="B18" s="3" t="inlineStr">
         <is>
-          <t>2024-10-01</t>
+          <t>2024-10-10</t>
         </is>
       </c>
       <c r="C18" s="3" t="inlineStr">
         <is>
-          <t>wafer_20012024_090819.csv</t>
+          <t>wafer_15032023_122518.csv</t>
         </is>
       </c>
       <c r="D18" s="3" t="inlineStr">
         <is>
-          <t>Failed</t>
+          <t>Passed</t>
         </is>
       </c>
       <c r="E18" s="3" t="inlineStr">
         <is>
-          <t>COLUMNDATA_WHOLE_MISSING_VALIDATION</t>
+          <t>FILE NAME VALIDATION</t>
         </is>
       </c>
       <c r="F18" s="3" t="inlineStr">
         <is>
-          <t>COLUMN DATA WHOLE MISSING VALIDATION FAILED, MISMATCH COLUMN LIST:[{'Sensor_Name': 'Sensor-86', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-110', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-111', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-112', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-221', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-245', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-246', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-247', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-359', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-383', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-384', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-385', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-493', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-517', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-518', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-519', 'Column_Data': [100, 0]}]</t>
+          <t>FILE NAME VALIDATION COMPLETED</t>
         </is>
       </c>
     </row>
@@ -1003,27 +1003,27 @@
       </c>
       <c r="B19" s="3" t="inlineStr">
         <is>
-          <t>2024-10-01</t>
+          <t>2024-10-10</t>
         </is>
       </c>
       <c r="C19" s="3" t="inlineStr">
         <is>
-          <t>wafer_20022024_090716.csv</t>
+          <t>wafer_15032023_122518.csv</t>
         </is>
       </c>
       <c r="D19" s="3" t="inlineStr">
         <is>
-          <t>Passed</t>
+          <t>Failed</t>
         </is>
       </c>
       <c r="E19" s="3" t="inlineStr">
         <is>
-          <t>FILE NAME VALIDATION</t>
+          <t>NUMBER OF COLUMNS VALIDATION</t>
         </is>
       </c>
       <c r="F19" s="3" t="inlineStr">
         <is>
-          <t>FILE NAME VALIDATION COMPLETED</t>
+          <t>COLUMN_DIFF BETWEEN DSA FILE AND PREDICTION FILE:-2</t>
         </is>
       </c>
     </row>
@@ -1033,12 +1033,12 @@
       </c>
       <c r="B20" s="3" t="inlineStr">
         <is>
-          <t>2024-10-01</t>
+          <t>2024-10-10</t>
         </is>
       </c>
       <c r="C20" s="3" t="inlineStr">
         <is>
-          <t>wafer_20022024_090716.csv</t>
+          <t>wafer_15042023_122518.csv</t>
         </is>
       </c>
       <c r="D20" s="3" t="inlineStr">
@@ -1048,12 +1048,12 @@
       </c>
       <c r="E20" s="3" t="inlineStr">
         <is>
-          <t>NUMBER OF COLUMNS VALIDATION</t>
+          <t>FILE NAME VALIDATION</t>
         </is>
       </c>
       <c r="F20" s="3" t="inlineStr">
         <is>
-          <t>NUMBER OF COLUMNS VALIDATION COMPLETED</t>
+          <t>FILE NAME VALIDATION COMPLETED</t>
         </is>
       </c>
     </row>
@@ -1063,12 +1063,12 @@
       </c>
       <c r="B21" s="3" t="inlineStr">
         <is>
-          <t>2024-10-01</t>
+          <t>2024-10-10</t>
         </is>
       </c>
       <c r="C21" s="3" t="inlineStr">
         <is>
-          <t>wafer_20022024_090716.csv</t>
+          <t>wafer_15042023_122518.csv</t>
         </is>
       </c>
       <c r="D21" s="3" t="inlineStr">
@@ -1078,12 +1078,12 @@
       </c>
       <c r="E21" s="3" t="inlineStr">
         <is>
-          <t>COLUMNDATA_WHOLE_MISSING_VALIDATION</t>
+          <t>NUMBER OF COLUMNS VALIDATION</t>
         </is>
       </c>
       <c r="F21" s="3" t="inlineStr">
         <is>
-          <t>COLUMN DATA WHOLE MISSING VALIDATION COMPLETED</t>
+          <t>NUMBER OF COLUMNS VALIDATION COMPLETED</t>
         </is>
       </c>
     </row>
@@ -1093,12 +1093,12 @@
       </c>
       <c r="B22" s="3" t="inlineStr">
         <is>
-          <t>2024-10-01</t>
+          <t>2024-10-10</t>
         </is>
       </c>
       <c r="C22" s="3" t="inlineStr">
         <is>
-          <t>wafer_20022024_090716.csv</t>
+          <t>wafer_15042023_122518.csv</t>
         </is>
       </c>
       <c r="D22" s="3" t="inlineStr">
@@ -1108,12 +1108,12 @@
       </c>
       <c r="E22" s="3" t="inlineStr">
         <is>
-          <t>COLUMN DATA VALIDATION</t>
+          <t>COLUMNDATA_WHOLE_MISSING_VALIDATION</t>
         </is>
       </c>
       <c r="F22" s="3" t="inlineStr">
         <is>
-          <t>COLUMN DATA VALIDATION COMPLETED</t>
+          <t>COLUMN DATA WHOLE MISSING VALIDATION COMPLETED</t>
         </is>
       </c>
     </row>
@@ -1123,12 +1123,12 @@
       </c>
       <c r="B23" s="3" t="inlineStr">
         <is>
-          <t>2024-10-01</t>
+          <t>2024-10-10</t>
         </is>
       </c>
       <c r="C23" s="3" t="inlineStr">
         <is>
-          <t>wafer_21012024_080913.csv</t>
+          <t>wafer_15042023_122518.csv</t>
         </is>
       </c>
       <c r="D23" s="3" t="inlineStr">
@@ -1138,12 +1138,12 @@
       </c>
       <c r="E23" s="3" t="inlineStr">
         <is>
-          <t>FILE NAME VALIDATION</t>
+          <t>COLUMN DATA VALIDATION</t>
         </is>
       </c>
       <c r="F23" s="3" t="inlineStr">
         <is>
-          <t>FILE NAME VALIDATION COMPLETED</t>
+          <t>COLUMN DATA VALIDATION COMPLETED</t>
         </is>
       </c>
     </row>
@@ -1153,12 +1153,12 @@
       </c>
       <c r="B24" s="3" t="inlineStr">
         <is>
-          <t>2024-10-01</t>
+          <t>2024-10-10</t>
         </is>
       </c>
       <c r="C24" s="3" t="inlineStr">
         <is>
-          <t>wafer_21012024_080913.csv</t>
+          <t>wafer_15052023_122518.csv</t>
         </is>
       </c>
       <c r="D24" s="3" t="inlineStr">
@@ -1168,12 +1168,12 @@
       </c>
       <c r="E24" s="3" t="inlineStr">
         <is>
-          <t>NUMBER OF COLUMNS VALIDATION</t>
+          <t>FILE NAME VALIDATION</t>
         </is>
       </c>
       <c r="F24" s="3" t="inlineStr">
         <is>
-          <t>NUMBER OF COLUMNS VALIDATION COMPLETED</t>
+          <t>FILE NAME VALIDATION COMPLETED</t>
         </is>
       </c>
     </row>
@@ -1183,12 +1183,12 @@
       </c>
       <c r="B25" s="3" t="inlineStr">
         <is>
-          <t>2024-10-01</t>
+          <t>2024-10-10</t>
         </is>
       </c>
       <c r="C25" s="3" t="inlineStr">
         <is>
-          <t>wafer_21012024_080913.csv</t>
+          <t>wafer_15052023_122518.csv</t>
         </is>
       </c>
       <c r="D25" s="3" t="inlineStr">
@@ -1198,12 +1198,12 @@
       </c>
       <c r="E25" s="3" t="inlineStr">
         <is>
-          <t>COLUMNDATA_WHOLE_MISSING_VALIDATION</t>
+          <t>NUMBER OF COLUMNS VALIDATION</t>
         </is>
       </c>
       <c r="F25" s="3" t="inlineStr">
         <is>
-          <t>COLUMN DATA WHOLE MISSING VALIDATION COMPLETED</t>
+          <t>NUMBER OF COLUMNS VALIDATION COMPLETED</t>
         </is>
       </c>
     </row>
@@ -1213,12 +1213,12 @@
       </c>
       <c r="B26" s="3" t="inlineStr">
         <is>
-          <t>2024-10-01</t>
+          <t>2024-10-10</t>
         </is>
       </c>
       <c r="C26" s="3" t="inlineStr">
         <is>
-          <t>wafer_21012024_080913.csv</t>
+          <t>wafer_15052023_122518.csv</t>
         </is>
       </c>
       <c r="D26" s="3" t="inlineStr">
@@ -1228,12 +1228,12 @@
       </c>
       <c r="E26" s="3" t="inlineStr">
         <is>
-          <t>COLUMN DATA VALIDATION</t>
+          <t>COLUMNDATA_WHOLE_MISSING_VALIDATION</t>
         </is>
       </c>
       <c r="F26" s="3" t="inlineStr">
         <is>
-          <t>COLUMN DATA VALIDATION COMPLETED</t>
+          <t>COLUMN DATA WHOLE MISSING VALIDATION COMPLETED</t>
         </is>
       </c>
     </row>
@@ -1243,12 +1243,12 @@
       </c>
       <c r="B27" s="3" t="inlineStr">
         <is>
-          <t>2024-10-01</t>
+          <t>2024-10-10</t>
         </is>
       </c>
       <c r="C27" s="3" t="inlineStr">
         <is>
-          <t>wafer_22022024_041119.csv</t>
+          <t>wafer_15052023_122518.csv</t>
         </is>
       </c>
       <c r="D27" s="3" t="inlineStr">
@@ -1258,12 +1258,12 @@
       </c>
       <c r="E27" s="3" t="inlineStr">
         <is>
-          <t>FILE NAME VALIDATION</t>
+          <t>COLUMN DATA VALIDATION</t>
         </is>
       </c>
       <c r="F27" s="3" t="inlineStr">
         <is>
-          <t>FILE NAME VALIDATION COMPLETED</t>
+          <t>COLUMN DATA VALIDATION COMPLETED</t>
         </is>
       </c>
     </row>
@@ -1273,12 +1273,12 @@
       </c>
       <c r="B28" s="3" t="inlineStr">
         <is>
-          <t>2024-10-01</t>
+          <t>2024-10-10</t>
         </is>
       </c>
       <c r="C28" s="3" t="inlineStr">
         <is>
-          <t>wafer_22022024_041119.csv</t>
+          <t>wafer_15062023_122518.csv</t>
         </is>
       </c>
       <c r="D28" s="3" t="inlineStr">
@@ -1288,12 +1288,12 @@
       </c>
       <c r="E28" s="3" t="inlineStr">
         <is>
-          <t>NUMBER OF COLUMNS VALIDATION</t>
+          <t>FILE NAME VALIDATION</t>
         </is>
       </c>
       <c r="F28" s="3" t="inlineStr">
         <is>
-          <t>NUMBER OF COLUMNS VALIDATION COMPLETED</t>
+          <t>FILE NAME VALIDATION COMPLETED</t>
         </is>
       </c>
     </row>
@@ -1303,27 +1303,27 @@
       </c>
       <c r="B29" s="3" t="inlineStr">
         <is>
-          <t>2024-10-01</t>
+          <t>2024-10-10</t>
         </is>
       </c>
       <c r="C29" s="3" t="inlineStr">
         <is>
-          <t>wafer_22022024_041119.csv</t>
+          <t>wafer_15062023_122518.csv</t>
         </is>
       </c>
       <c r="D29" s="3" t="inlineStr">
         <is>
-          <t>Failed</t>
+          <t>Passed</t>
         </is>
       </c>
       <c r="E29" s="3" t="inlineStr">
         <is>
-          <t>COLUMNDATA_WHOLE_MISSING_VALIDATION</t>
+          <t>NUMBER OF COLUMNS VALIDATION</t>
         </is>
       </c>
       <c r="F29" s="3" t="inlineStr">
         <is>
-          <t>COLUMN DATA WHOLE MISSING VALIDATION FAILED, MISMATCH COLUMN LIST:[{'Sensor_Name': 'Sensor-86', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-110', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-111', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-112', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-221', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-245', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-246', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-247', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-359', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-383', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-384', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-385', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-493', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-517', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-518', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-519', 'Column_Data': [100, 0]}]</t>
+          <t>NUMBER OF COLUMNS VALIDATION COMPLETED</t>
         </is>
       </c>
     </row>
@@ -1333,12 +1333,12 @@
       </c>
       <c r="B30" s="3" t="inlineStr">
         <is>
-          <t>2024-10-01</t>
+          <t>2024-10-10</t>
         </is>
       </c>
       <c r="C30" s="3" t="inlineStr">
         <is>
-          <t>wafer_23012024_011008.csv</t>
+          <t>wafer_15062023_122518.csv</t>
         </is>
       </c>
       <c r="D30" s="3" t="inlineStr">
@@ -1348,12 +1348,12 @@
       </c>
       <c r="E30" s="3" t="inlineStr">
         <is>
-          <t>FILE NAME VALIDATION</t>
+          <t>COLUMNDATA_WHOLE_MISSING_VALIDATION</t>
         </is>
       </c>
       <c r="F30" s="3" t="inlineStr">
         <is>
-          <t>FILE NAME VALIDATION COMPLETED</t>
+          <t>COLUMN DATA WHOLE MISSING VALIDATION COMPLETED</t>
         </is>
       </c>
     </row>
@@ -1363,27 +1363,27 @@
       </c>
       <c r="B31" s="3" t="inlineStr">
         <is>
-          <t>2024-10-01</t>
+          <t>2024-10-10</t>
         </is>
       </c>
       <c r="C31" s="3" t="inlineStr">
         <is>
-          <t>wafer_23012024_011008.csv</t>
+          <t>wafer_15062023_122518.csv</t>
         </is>
       </c>
       <c r="D31" s="3" t="inlineStr">
         <is>
-          <t>Passed</t>
+          <t>Failed</t>
         </is>
       </c>
       <c r="E31" s="3" t="inlineStr">
         <is>
-          <t>NUMBER OF COLUMNS VALIDATION</t>
+          <t>COLUMN DATA VALIDATION</t>
         </is>
       </c>
       <c r="F31" s="3" t="inlineStr">
         <is>
-          <t>NUMBER OF COLUMNS VALIDATION COMPLETED</t>
+          <t>COLUMN DATA VALIDATION FAILED, MISMATCH COLUMN LIST:[{'schema_file': 'Column_name:Sensor-6, Column_dtype:float64', 'raw_file': 'Column_name:Sensor-6, Column_dtype:int64'}, {'schema_file': 'Column_name:Sensor-11, Column_dtype:float64', 'raw_file': 'Column_name:Sensor-11, Column_dtype:int64'}, {'schema_file': 'Column_name:Sensor-14, Column_dtype:float64', 'raw_file': 'Column_name:Sensor-14, Column_dtype:int64'}, {'schema_file': 'Column_name:Sensor-43, Column_dtype:float64', 'raw_file': 'Column_name:Sensor-43, Column_dtype:int64'}, {'schema_file': 'Column_name:Sensor-50, Column_dtype:float64', 'raw_file': 'Column_name:Sensor-50, Column_dtype:int64'}, {'schema_file': 'Column_name:Sensor-53, Column_dtype:float64', 'raw_file': 'Column_name:Sensor-53, Column_dtype:int64'}, {'schema_file': 'Column_name:Sensor-70, Column_dtype:float64', 'raw_file': 'Column_name:Sensor-70, Column_dtype:int64'}, {'schema_file': 'Column_name:Sensor-98, Column_dtype:float64', 'raw_file': 'Column_name:Sensor-98, Column_dtype:int64'}, {'schema_file': 'Column_name:Sensor-142, Column_dtype:float64', 'raw_file': 'Column_name:Sensor-142, Column_dtype:int64'}, {'schema_file': 'Column_name:Sensor-150, Column_dtype:float64', 'raw_file': 'Column_name:Sensor-150, Column_dtype:int64'}, {'schema_file': 'Column_name:Sensor-179, Column_dtype:float64', 'raw_file': 'Column_name:Sensor-179, Column_dtype:int64'}, {'schema_file': 'Column_name:Sensor-180, Column_dtype:float64', 'raw_file': 'Column_name:Sensor-180, Column_dtype:int64'}, {'schema_file': 'Column_name:Sensor-187, Column_dtype:float64', 'raw_file': 'Column_name:Sensor-187, Column_dtype:int64'}, {'schema_file': 'Column_name:Sensor-190, Column_dtype:float64', 'raw_file': 'Column_name:Sensor-190, Column_dtype:int64'}, {'schema_file': 'Column_name:Sensor-191, Column_dtype:float64', 'raw_file': 'Column_name:Sensor-191, Column_dtype:int64'}, {'schema_file': 'Column_name:Sensor-192, Column_dtype:float64', 'raw_file': 'Column_name:Sensor-192, Column_dtype:int64'}, {'schema_file': 'Column_name:Sensor-193, Column_dtype:float64', 'raw_file': 'Column_name:Sensor-193, Column_dtype:int64'}, {'schema_file': 'Column_name:Sensor-194, Column_dtype:float64', 'raw_file': 'Column_name:Sensor-194, Column_dtype:int64'}, {'schema_file': 'Column_name:Sensor-195, Column_dtype:float64', 'raw_file': 'Column_name:Sensor-195, Column_dtype:int64'}, {'schema_file': 'Column_name:Sensor-227, Column_dtype:float64', 'raw_file': 'Column_name:Sensor-227, Column_dtype:int64'}, {'schema_file': 'Column_name:Sensor-230, Column_dtype:float64', 'raw_file': 'Column_name:Sensor-230, Column_dtype:int64'}, {'schema_file': 'Column_name:Sensor-231, Column_dtype:float64', 'raw_file': 'Column_name:Sensor-231, Column_dtype:int64'}, {'schema_file': 'Column_name:Sensor-232, Column_dtype:float64', 'raw_file': 'Column_name:Sensor-232, Column_dtype:int64'}, {'schema_file': 'Column_name:Sensor-233, Column_dtype:float64', 'raw_file': 'Column_name:Sensor-233, Column_dtype:int64'}, {'schema_file': 'Column_name:Sensor-234, Column_dtype:float64', 'raw_file': 'Column_name:Sensor-234, Column_dtype:int64'}, {'schema_file': 'Column_name:Sensor-235, Column_dtype:float64', 'raw_file': 'Column_name:Sensor-235, Column_dtype:int64'}, {'schema_file': 'Column_name:Sensor-236, Column_dtype:float64', 'raw_file': 'Column_name:Sensor-236, Column_dtype:int64'}, {'schema_file': 'Column_name:Sensor-237, Column_dtype:float64', 'raw_file': 'Column_name:Sensor-237, Column_dtype:int64'}, {'schema_file': 'Column_name:Sensor-238, Column_dtype:float64', 'raw_file': 'Column_name:Sensor-238, Column_dtype:int64'}, {'schema_file': 'Column_name:Sensor-241, Column_dtype:float64', 'raw_file': 'Column_name:Sensor-241, Column_dtype:int64'}, {'schema_file': 'Column_name:Sensor-242, Column_dtype:float64', 'raw_file': 'Column_name:Sensor-242, Column_dtype:int64'}, {'schema_file': 'Column_name:Sensor-243, Column_dtype:float64', 'raw_file': 'Column_name:Sensor-243, Column_dtype:int64'}, {'schema_file': 'Column_name:Sensor-244, Column_dtype:float64', 'raw_file': 'Column_name:Sensor-244, Column_dtype:int64'}, {'schema_file': 'Column_name:Sensor-257, Column_dtype:float64', 'raw_file': 'Column_name:Sensor-257, Column_dtype:int64'}, {'schema_file': 'Column_name:Sensor-258, Column_dtype:float64', 'raw_file': 'Column_name:Sensor-258, Column_dtype:int64'}, {'schema_file': 'Column_name:Sensor-259, Column_dtype:float64', 'raw_file': 'Column_name:Sensor-259, Column_dtype:int64'}, {'schema_file': 'Column_name:Sensor-260, Column_dtype:float64', 'raw_file': 'Column_name:Sensor-260, Column_dtype:int64'}, {'schema_file': 'Column_name:Sensor-261, Column_dtype:float64', 'raw_file': 'Column_name:Sensor-261, Column_dtype:int64'}, {'schema_file': 'Column_name:Sensor-262, Column_dtype:float64', 'raw_file': 'Column_name:Sensor-262, Column_dtype:int64'}, {'schema_file': 'Column_name:Sensor-263, Column_dtype:float64', 'raw_file': 'Column_name:Sensor-263, Column_dtype:int64'}, {'schema_file': 'Column_name:Sensor-264, Column_dtype:float64', 'raw_file': 'Column_name:Sensor-264, Column_dtype:int64'}, {'schema_file': 'Column_name:Sensor-265, Column_dtype:float64', 'raw_file': 'Column_name:Sensor-265, Column_dtype:int64'}, {'schema_file': 'Column_name:Sensor-266, Column_dtype:float64', 'raw_file': 'Column_name:Sensor-266, Column_dtype:int64'}, {'schema_file': 'Column_name:Sensor-267, Column_dtype:float64', 'raw_file': 'Column_name:Sensor-267, Column_dtype:int64'}, {'schema_file': 'Column_name:Sensor-277, Column_dtype:float64', 'raw_file': 'Column_name:Sensor-277, Column_dtype:int64'}, {'schema_file': 'Column_name:Sensor-285, Column_dtype:float64', 'raw_file': 'Column_name:Sensor-285, Column_dtype:int64'}, {'schema_file': 'Column_name:Sensor-314, Column_dtype:float64', 'raw_file': 'Column_name:Sensor-314, Column_dtype:int64'}, {'schema_file': 'Column_name:Sensor-315, Column_dtype:float64', 'raw_file': 'Column_name:Sensor-315, Column_dtype:int64'}, {'schema_file': 'Column_name:Sensor-316, Column_dtype:float64', 'raw_file': 'Column_name:Sensor-316, Column_dtype:int64'}, {'schema_file': 'Column_name:Sensor-323, Column_dtype:float64', 'raw_file': 'Column_name:Sensor-323, Column_dtype:int64'}, {'schema_file': 'Column_name:Sensor-326, Column_dtype:float64', 'raw_file': 'Column_name:Sensor-326, Column_dtype:int64'}, {'schema_file': 'Column_name:Sensor-327, Column_dtype:float64', 'raw_file': 'Column_name:Sensor-327, Column_dtype:int64'}, {'schema_file': 'Column_name:Sensor-328, Column_dtype:float64', 'raw_file': 'Column_name:Sensor-328, Column_dtype:int64'}, {'schema_file': 'Column_name:Sensor-329, Column_dtype:float64', 'raw_file': 'Column_name:Sensor-329, Column_dtype:int64'}, {'schema_file': 'Column_name:Sensor-330, Column_dtype:float64', 'raw_file': 'Column_name:Sensor-330, Column_dtype:int64'}, {'schema_file': 'Column_name:Sensor-331, Column_dtype:float64', 'raw_file': 'Column_name:Sensor-331, Column_dtype:int64'}, {'schema_file': 'Column_name:Sensor-365, Column_dtype:float64', 'raw_file': 'Column_name:Sensor-365, Column_dtype:int64'}, {'schema_file': 'Column_name:Sensor-370, Column_dtype:float64', 'raw_file': 'Column_name:Sensor-370, Column_dtype:int64'}, {'schema_file': 'Column_name:Sensor-371, Column_dtype:float64', 'raw_file': 'Column_name:Sensor-371, Column_dtype:int64'}, {'schema_file': 'Column_name:Sensor-372, Column_dtype:float64', 'raw_file': 'Column_name:Sensor-372, Column_dtype:int64'}, {'schema_file': 'Column_name:Sensor-373, Column_dtype:float64', 'raw_file': 'Column_name:Sensor-373, Column_dtype:int64'}, {'schema_file': 'Column_name:Sensor-374, Column_dtype:float64', 'raw_file': 'Column_name:Sensor-374, Column_dtype:int64'}, {'schema_file': 'Column_name:Sensor-375, Column_dtype:float64', 'raw_file': 'Column_name:Sensor-375, Column_dtype:int64'}, {'schema_file': 'Column_name:Sensor-376, Column_dtype:float64', 'raw_file': 'Column_name:Sensor-376, Column_dtype:int64'}, {'schema_file': 'Column_name:Sensor-379, Column_dtype:float64', 'raw_file': 'Column_name:Sensor-379, Column_dtype:int64'}, {'schema_file': 'Column_name:Sensor-380, Column_dtype:float64', 'raw_file': 'Column_name:Sensor-380, Column_dtype:int64'}, {'schema_file': 'Column_name:Sensor-381, Column_dtype:float64', 'raw_file': 'Column_name:Sensor-381, Column_dtype:int64'}, {'schema_file': 'Column_name:Sensor-382, Column_dtype:float64', 'raw_file': 'Column_name:Sensor-382, Column_dtype:int64'}, {'schema_file': 'Column_name:Sensor-395, Column_dtype:float64', 'raw_file': 'Column_name:Sensor-395, Column_dtype:int64'}, {'schema_file': 'Column_name:Sensor-396, Column_dtype:float64', 'raw_file': 'Column_name:Sensor-396, Column_dtype:int64'}, {'schema_file': 'Column_name:Sensor-397, Column_dtype:float64', 'raw_file': 'Column_name:Sensor-397, Column_dtype:int64'}, {'schema_file': 'Column_name:Sensor-398, Column_dtype:float64', 'raw_file': 'Column_name:Sensor-398, Column_dtype:int64'}, {'schema_file': 'Column_name:Sensor-399, Column_dtype:float64', 'raw_file': 'Column_name:Sensor-399, Column_dtype:int64'}, {'schema_file': 'Column_name:Sensor-400, Column_dtype:float64', 'raw_file': 'Column_name:Sensor-400, Column_dtype:int64'}, {'schema_file': 'Column_name:Sensor-401, Column_dtype:float64', 'raw_file': 'Column_name:Sensor-401, Column_dtype:int64'}, {'schema_file': 'Column_name:Sensor-402, Column_dtype:float64', 'raw_file': 'Column_name:Sensor-402, Column_dtype:int64'}, {'schema_file': 'Column_name:Sensor-403, Column_dtype:float64', 'raw_file': 'Column_name:Sensor-403, Column_dtype:int64'}, {'schema_file': 'Column_name:Sensor-404, Column_dtype:float64', 'raw_file': 'Column_name:Sensor-404, Column_dtype:int64'}, {'schema_file': 'Column_name:Sensor-405, Column_dtype:float64', 'raw_file': 'Column_name:Sensor-405, Column_dtype:int64'}, {'schema_file': 'Column_name:Sensor-415, Column_dtype:float64', 'raw_file': 'Column_name:Sensor-415, Column_dtype:int64'}, {'schema_file': 'Column_name:Sensor-423, Column_dtype:float64', 'raw_file': 'Column_name:Sensor-423, Column_dtype:int64'}, {'schema_file': 'Column_name:Sensor-450, Column_dtype:float64', 'raw_file': 'Column_name:Sensor-450, Column_dtype:int64'}, {'schema_file': 'Column_name:Sensor-451, Column_dtype:float64', 'raw_file': 'Column_name:Sensor-451, Column_dtype:int64'}, {'schema_file': 'Column_name:Sensor-452, Column_dtype:float64', 'raw_file': 'Column_name:Sensor-452, Column_dtype:int64'}, {'schema_file': 'Column_name:Sensor-459, Column_dtype:float64', 'raw_file': 'Column_name:Sensor-459, Column_dtype:int64'}, {'schema_file': 'Column_name:Sensor-462, Column_dtype:float64', 'raw_file': 'Column_name:Sensor-462, Column_dtype:int64'}, {'schema_file': 'Column_name:Sensor-463, Column_dtype:float64', 'raw_file': 'Column_name:Sensor-463, Column_dtype:int64'}, {'schema_file': 'Column_name:Sensor-464, Column_dtype:float64', 'raw_file': 'Column_name:Sensor-464, Column_dtype:int64'}, {'schema_file': 'Column_name:Sensor-465, Column_dtype:float64', 'raw_file': 'Column_name:Sensor-465, Column_dtype:int64'}, {'schema_file': 'Column_name:Sensor-466, Column_dtype:float64', 'raw_file': 'Column_name:Sensor-466, Column_dtype:int64'}, {'schema_file': 'Column_name:Sensor-467, Column_dtype:float64', 'raw_file': 'Column_name:Sensor-467, Column_dtype:int64'}, {'schema_file': 'Column_name:Sensor-482, Column_dtype:float64', 'raw_file': 'Column_name:Sensor-482, Column_dtype:int64'}, {'schema_file': 'Column_name:Sensor-499, Column_dtype:float64', 'raw_file': 'Column_name:Sensor-499, Column_dtype:int64'}, {'schema_file': 'Column_name:Sensor-502, Column_dtype:float64', 'raw_file': 'Column_name:Sensor-502, Column_dtype:int64'}, {'schema_file': 'Column_name:Sensor-503, Column_dtype:float64', 'raw_file': 'Column_name:Sensor-503, Column_dtype:int64'}, {'schema_file': 'Column_name:Sensor-504, Column_dtype:float64', 'raw_file': 'Column_name:Sensor-504, Column_dtype:int64'}, {'schema_file': 'Column_name:Sensor-505, Column_dtype:float64', 'raw_file': 'Column_name:Sensor-505, Column_dtype:int64'}, {'schema_file': 'Column_name:Sensor-506, Column_dtype:float64', 'raw_file': 'Column_name:Sensor-506, Column_dtype:int64'}, {'schema_file': 'Column_name:Sensor-507, Column_dtype:float64', 'raw_file': 'Column_name:Sensor-507, Column_dtype:int64'}, {'schema_file': 'Column_name:Sensor-508, Column_dtype:float64', 'raw_file': 'Column_name:Sensor-508, Column_dtype:int64'}, {'schema_file': 'Column_name:Sensor-509, Column_dtype:float64', 'raw_file': 'Column_name:Sensor-509, Column_dtype:int64'}, {'schema_file': 'Column_name:Sensor-510, Column_dtype:float64', 'raw_file': 'Column_name:Sensor-510, Column_dtype:int64'}, {'schema_file': 'Column_name:Sensor-513, Column_dtype:float64', 'raw_file': 'Column_name:Sensor-513, Column_dtype:int64'}, {'schema_file': 'Column_name:Sensor-514, Column_dtype:float64', 'raw_file': 'Column_name:Sensor-514, Column_dtype:int64'}, {'schema_file': 'Column_name:Sensor-515, Column_dtype:float64', 'raw_file': 'Column_name:Sensor-515, Column_dtype:int64'}, {'schema_file': 'Column_name:Sensor-516, Column_dtype:float64', 'raw_file': 'Column_name:Sensor-516, Column_dtype:int64'}, {'schema_file': 'Column_name:Sensor-529, Column_dtype:float64', 'raw_file': 'Column_name:Sensor-529, Column_dtype:int64'}, {'schema_file': 'Column_name:Sensor-530, Column_dtype:float64', 'raw_file': 'Column_name:Sensor-530, Column_dtype:int64'}, {'schema_file': 'Column_name:Sensor-531, Column_dtype:float64', 'raw_file': 'Column_name:Sensor-531, Column_dtype:int64'}, {'schema_file': 'Column_name:Sensor-532, Column_dtype:float64', 'raw_file': 'Column_name:Sensor-532, Column_dtype:int64'}, {'schema_file': 'Column_name:Sensor-533, Column_dtype:float64', 'raw_file': 'Column_name:Sensor-533, Column_dtype:int64'}, {'schema_file': 'Column_name:Sensor-534, Column_dtype:float64', 'raw_file': 'Column_name:Sensor-534, Column_dtype:int64'}, {'schema_file': 'Column_name:Sensor-535, Column_dtype:float64', 'raw_file': 'Column_name:Sensor-535, Column_dtype:int64'}, {'schema_file': 'Column_name:Sensor-536, Column_dtype:float64', 'raw_file': 'Column_name:Sensor-536, Column_dtype:int64'}, {'schema_file': 'Column_name:Sensor-537, Column_dtype:float64', 'raw_file': 'Column_name:Sensor-537, Column_dtype:int64'}, {'schema_file': 'Column_name:Sensor-538, Column_dtype:float64', 'raw_file': 'Column_name:Sensor-538, Column_dtype:int64'}, {'schema_file': 'Column_name:Sensor-539, Column_dtype:float64', 'raw_file': 'Column_name:Sensor-539, Column_dtype:int64'}]</t>
         </is>
       </c>
     </row>
@@ -1393,27 +1393,27 @@
       </c>
       <c r="B32" s="3" t="inlineStr">
         <is>
-          <t>2024-10-01</t>
+          <t>2024-10-10</t>
         </is>
       </c>
       <c r="C32" s="3" t="inlineStr">
         <is>
-          <t>wafer_23012024_011008.csv</t>
+          <t>wafer_15072023_122518.csv</t>
         </is>
       </c>
       <c r="D32" s="3" t="inlineStr">
         <is>
-          <t>Failed</t>
+          <t>Passed</t>
         </is>
       </c>
       <c r="E32" s="3" t="inlineStr">
         <is>
-          <t>COLUMNDATA_WHOLE_MISSING_VALIDATION</t>
+          <t>FILE NAME VALIDATION</t>
         </is>
       </c>
       <c r="F32" s="3" t="inlineStr">
         <is>
-          <t>COLUMN DATA WHOLE MISSING VALIDATION FAILED, MISMATCH COLUMN LIST:[{'Sensor_Name': 'Sensor-86', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-110', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-111', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-112', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-221', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-245', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-246', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-247', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-359', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-383', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-384', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-385', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-493', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-517', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-518', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-519', 'Column_Data': [100, 0]}]</t>
+          <t>FILE NAME VALIDATION COMPLETED</t>
         </is>
       </c>
     </row>
@@ -1423,12 +1423,12 @@
       </c>
       <c r="B33" s="3" t="inlineStr">
         <is>
-          <t>2024-10-01</t>
+          <t>2024-10-10</t>
         </is>
       </c>
       <c r="C33" s="3" t="inlineStr">
         <is>
-          <t>wafer_23012024_041211.csv</t>
+          <t>wafer_15072023_122518.csv</t>
         </is>
       </c>
       <c r="D33" s="3" t="inlineStr">
@@ -1438,12 +1438,12 @@
       </c>
       <c r="E33" s="3" t="inlineStr">
         <is>
-          <t>FILE NAME VALIDATION</t>
+          <t>NUMBER OF COLUMNS VALIDATION</t>
         </is>
       </c>
       <c r="F33" s="3" t="inlineStr">
         <is>
-          <t>FILE NAME VALIDATION COMPLETED</t>
+          <t>NUMBER OF COLUMNS VALIDATION COMPLETED</t>
         </is>
       </c>
     </row>
@@ -1453,12 +1453,12 @@
       </c>
       <c r="B34" s="3" t="inlineStr">
         <is>
-          <t>2024-10-01</t>
+          <t>2024-10-10</t>
         </is>
       </c>
       <c r="C34" s="3" t="inlineStr">
         <is>
-          <t>wafer_23012024_041211.csv</t>
+          <t>wafer_15072023_122518.csv</t>
         </is>
       </c>
       <c r="D34" s="3" t="inlineStr">
@@ -1468,12 +1468,12 @@
       </c>
       <c r="E34" s="3" t="inlineStr">
         <is>
-          <t>NUMBER OF COLUMNS VALIDATION</t>
+          <t>COLUMNDATA_WHOLE_MISSING_VALIDATION</t>
         </is>
       </c>
       <c r="F34" s="3" t="inlineStr">
         <is>
-          <t>NUMBER OF COLUMNS VALIDATION COMPLETED</t>
+          <t>COLUMN DATA WHOLE MISSING VALIDATION COMPLETED</t>
         </is>
       </c>
     </row>
@@ -1483,12 +1483,12 @@
       </c>
       <c r="B35" s="3" t="inlineStr">
         <is>
-          <t>2024-10-01</t>
+          <t>2024-10-10</t>
         </is>
       </c>
       <c r="C35" s="3" t="inlineStr">
         <is>
-          <t>wafer_23012024_041211.csv</t>
+          <t>wafer_15072023_122518.csv</t>
         </is>
       </c>
       <c r="D35" s="3" t="inlineStr">
@@ -1498,12 +1498,12 @@
       </c>
       <c r="E35" s="3" t="inlineStr">
         <is>
-          <t>COLUMNDATA_WHOLE_MISSING_VALIDATION</t>
+          <t>COLUMN DATA VALIDATION</t>
         </is>
       </c>
       <c r="F35" s="3" t="inlineStr">
         <is>
-          <t>COLUMN DATA WHOLE MISSING VALIDATION COMPLETED</t>
+          <t>COLUMN DATA VALIDATION COMPLETED</t>
         </is>
       </c>
     </row>
@@ -1513,12 +1513,12 @@
       </c>
       <c r="B36" s="3" t="inlineStr">
         <is>
-          <t>2024-10-01</t>
+          <t>2024-10-10</t>
         </is>
       </c>
       <c r="C36" s="3" t="inlineStr">
         <is>
-          <t>wafer_23012024_041211.csv</t>
+          <t>wafer_15082023_122518.csv</t>
         </is>
       </c>
       <c r="D36" s="3" t="inlineStr">
@@ -1528,12 +1528,12 @@
       </c>
       <c r="E36" s="3" t="inlineStr">
         <is>
-          <t>COLUMN DATA VALIDATION</t>
+          <t>FILE NAME VALIDATION</t>
         </is>
       </c>
       <c r="F36" s="3" t="inlineStr">
         <is>
-          <t>COLUMN DATA VALIDATION COMPLETED</t>
+          <t>FILE NAME VALIDATION COMPLETED</t>
         </is>
       </c>
     </row>
@@ -1543,12 +1543,12 @@
       </c>
       <c r="B37" s="3" t="inlineStr">
         <is>
-          <t>2024-10-01</t>
+          <t>2024-10-10</t>
         </is>
       </c>
       <c r="C37" s="3" t="inlineStr">
         <is>
-          <t>wafer_27012024_080911.csv</t>
+          <t>wafer_15082023_122518.csv</t>
         </is>
       </c>
       <c r="D37" s="3" t="inlineStr">
@@ -1558,12 +1558,12 @@
       </c>
       <c r="E37" s="3" t="inlineStr">
         <is>
-          <t>FILE NAME VALIDATION</t>
+          <t>NUMBER OF COLUMNS VALIDATION</t>
         </is>
       </c>
       <c r="F37" s="3" t="inlineStr">
         <is>
-          <t>FILE NAME VALIDATION COMPLETED</t>
+          <t>NUMBER OF COLUMNS VALIDATION COMPLETED</t>
         </is>
       </c>
     </row>
@@ -1573,12 +1573,12 @@
       </c>
       <c r="B38" s="3" t="inlineStr">
         <is>
-          <t>2024-10-01</t>
+          <t>2024-10-10</t>
         </is>
       </c>
       <c r="C38" s="3" t="inlineStr">
         <is>
-          <t>wafer_27012024_080911.csv</t>
+          <t>wafer_15082023_122518.csv</t>
         </is>
       </c>
       <c r="D38" s="3" t="inlineStr">
@@ -1588,12 +1588,12 @@
       </c>
       <c r="E38" s="3" t="inlineStr">
         <is>
-          <t>NUMBER OF COLUMNS VALIDATION</t>
+          <t>COLUMNDATA_WHOLE_MISSING_VALIDATION</t>
         </is>
       </c>
       <c r="F38" s="3" t="inlineStr">
         <is>
-          <t>NUMBER OF COLUMNS VALIDATION COMPLETED</t>
+          <t>COLUMN DATA WHOLE MISSING VALIDATION COMPLETED</t>
         </is>
       </c>
     </row>
@@ -1603,12 +1603,12 @@
       </c>
       <c r="B39" s="3" t="inlineStr">
         <is>
-          <t>2024-10-01</t>
+          <t>2024-10-10</t>
         </is>
       </c>
       <c r="C39" s="3" t="inlineStr">
         <is>
-          <t>wafer_27012024_080911.csv</t>
+          <t>wafer_15082023_122518.csv</t>
         </is>
       </c>
       <c r="D39" s="3" t="inlineStr">
@@ -1618,12 +1618,12 @@
       </c>
       <c r="E39" s="3" t="inlineStr">
         <is>
-          <t>COLUMNDATA_WHOLE_MISSING_VALIDATION</t>
+          <t>COLUMN DATA VALIDATION</t>
         </is>
       </c>
       <c r="F39" s="3" t="inlineStr">
         <is>
-          <t>COLUMN DATA WHOLE MISSING VALIDATION COMPLETED</t>
+          <t>COLUMN DATA VALIDATION COMPLETED</t>
         </is>
       </c>
     </row>
@@ -1633,12 +1633,12 @@
       </c>
       <c r="B40" s="3" t="inlineStr">
         <is>
-          <t>2024-10-01</t>
+          <t>2024-10-10</t>
         </is>
       </c>
       <c r="C40" s="3" t="inlineStr">
         <is>
-          <t>wafer_27012024_080911.csv</t>
+          <t>wafer_15092023_122518.csv</t>
         </is>
       </c>
       <c r="D40" s="3" t="inlineStr">
@@ -1648,12 +1648,12 @@
       </c>
       <c r="E40" s="3" t="inlineStr">
         <is>
-          <t>COLUMN DATA VALIDATION</t>
+          <t>FILE NAME VALIDATION</t>
         </is>
       </c>
       <c r="F40" s="3" t="inlineStr">
         <is>
-          <t>COLUMN DATA VALIDATION COMPLETED</t>
+          <t>FILE NAME VALIDATION COMPLETED</t>
         </is>
       </c>
     </row>
@@ -1663,12 +1663,12 @@
       </c>
       <c r="B41" s="3" t="inlineStr">
         <is>
-          <t>2024-10-01</t>
+          <t>2024-10-10</t>
         </is>
       </c>
       <c r="C41" s="3" t="inlineStr">
         <is>
-          <t>wafer_28012024_051011.csv</t>
+          <t>wafer_15092023_122518.csv</t>
         </is>
       </c>
       <c r="D41" s="3" t="inlineStr">
@@ -1678,12 +1678,12 @@
       </c>
       <c r="E41" s="3" t="inlineStr">
         <is>
-          <t>FILE NAME VALIDATION</t>
+          <t>NUMBER OF COLUMNS VALIDATION</t>
         </is>
       </c>
       <c r="F41" s="3" t="inlineStr">
         <is>
-          <t>FILE NAME VALIDATION COMPLETED</t>
+          <t>NUMBER OF COLUMNS VALIDATION COMPLETED</t>
         </is>
       </c>
     </row>
@@ -1693,12 +1693,12 @@
       </c>
       <c r="B42" s="3" t="inlineStr">
         <is>
-          <t>2024-10-01</t>
+          <t>2024-10-10</t>
         </is>
       </c>
       <c r="C42" s="3" t="inlineStr">
         <is>
-          <t>wafer_28012024_051011.csv</t>
+          <t>wafer_15092023_122518.csv</t>
         </is>
       </c>
       <c r="D42" s="3" t="inlineStr">
@@ -1708,12 +1708,12 @@
       </c>
       <c r="E42" s="3" t="inlineStr">
         <is>
-          <t>NUMBER OF COLUMNS VALIDATION</t>
+          <t>COLUMNDATA_WHOLE_MISSING_VALIDATION</t>
         </is>
       </c>
       <c r="F42" s="3" t="inlineStr">
         <is>
-          <t>NUMBER OF COLUMNS VALIDATION COMPLETED</t>
+          <t>COLUMN DATA WHOLE MISSING VALIDATION COMPLETED</t>
         </is>
       </c>
     </row>
@@ -1723,567 +1723,27 @@
       </c>
       <c r="B43" s="3" t="inlineStr">
         <is>
-          <t>2024-10-01</t>
+          <t>2024-10-10</t>
         </is>
       </c>
       <c r="C43" s="3" t="inlineStr">
         <is>
-          <t>wafer_28012024_051011.csv</t>
+          <t>wafer_15092023_122518.csv</t>
         </is>
       </c>
       <c r="D43" s="3" t="inlineStr">
         <is>
-          <t>Failed</t>
+          <t>Passed</t>
         </is>
       </c>
       <c r="E43" s="3" t="inlineStr">
         <is>
-          <t>COLUMNDATA_WHOLE_MISSING_VALIDATION</t>
+          <t>COLUMN DATA VALIDATION</t>
         </is>
       </c>
       <c r="F43" s="3" t="inlineStr">
         <is>
-          <t>COLUMN DATA WHOLE MISSING VALIDATION FAILED, MISMATCH COLUMN LIST:[{'Sensor_Name': 'Sensor-86', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-110', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-111', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-112', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-221', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-245', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-246', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-247', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-359', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-383', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-384', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-385', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-493', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-517', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-518', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-519', 'Column_Data': [100, 0]}]</t>
-        </is>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44" s="3" t="n">
-        <v>43</v>
-      </c>
-      <c r="B44" s="3" t="inlineStr">
-        <is>
-          <t>2024-10-01</t>
-        </is>
-      </c>
-      <c r="C44" s="3" t="inlineStr">
-        <is>
-          <t>wafer_28012024_090817.csv</t>
-        </is>
-      </c>
-      <c r="D44" s="3" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
-      </c>
-      <c r="E44" s="3" t="inlineStr">
-        <is>
-          <t>FILE NAME VALIDATION</t>
-        </is>
-      </c>
-      <c r="F44" s="3" t="inlineStr">
-        <is>
-          <t>FILE NAME VALIDATION COMPLETED</t>
-        </is>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" s="3" t="n">
-        <v>44</v>
-      </c>
-      <c r="B45" s="3" t="inlineStr">
-        <is>
-          <t>2024-10-01</t>
-        </is>
-      </c>
-      <c r="C45" s="3" t="inlineStr">
-        <is>
-          <t>wafer_28012024_090817.csv</t>
-        </is>
-      </c>
-      <c r="D45" s="3" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
-      </c>
-      <c r="E45" s="3" t="inlineStr">
-        <is>
-          <t>NUMBER OF COLUMNS VALIDATION</t>
-        </is>
-      </c>
-      <c r="F45" s="3" t="inlineStr">
-        <is>
-          <t>NUMBER OF COLUMNS VALIDATION COMPLETED</t>
-        </is>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46" s="3" t="n">
-        <v>45</v>
-      </c>
-      <c r="B46" s="3" t="inlineStr">
-        <is>
-          <t>2024-10-01</t>
-        </is>
-      </c>
-      <c r="C46" s="3" t="inlineStr">
-        <is>
-          <t>wafer_28012024_090817.csv</t>
-        </is>
-      </c>
-      <c r="D46" s="3" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
-      </c>
-      <c r="E46" s="3" t="inlineStr">
-        <is>
-          <t>COLUMNDATA_WHOLE_MISSING_VALIDATION</t>
-        </is>
-      </c>
-      <c r="F46" s="3" t="inlineStr">
-        <is>
-          <t>COLUMN DATA WHOLE MISSING VALIDATION COMPLETED</t>
-        </is>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47" s="3" t="n">
-        <v>46</v>
-      </c>
-      <c r="B47" s="3" t="inlineStr">
-        <is>
-          <t>2024-10-01</t>
-        </is>
-      </c>
-      <c r="C47" s="3" t="inlineStr">
-        <is>
-          <t>wafer_28012024_090817.csv</t>
-        </is>
-      </c>
-      <c r="D47" s="3" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
-      </c>
-      <c r="E47" s="3" t="inlineStr">
-        <is>
-          <t>COLUMN DATA VALIDATION</t>
-        </is>
-      </c>
-      <c r="F47" s="3" t="inlineStr">
-        <is>
           <t>COLUMN DATA VALIDATION COMPLETED</t>
-        </is>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48" s="3" t="n">
-        <v>47</v>
-      </c>
-      <c r="B48" s="3" t="inlineStr">
-        <is>
-          <t>2024-10-01</t>
-        </is>
-      </c>
-      <c r="C48" s="3" t="inlineStr">
-        <is>
-          <t>wafer_28042024_031911.csv</t>
-        </is>
-      </c>
-      <c r="D48" s="3" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
-      </c>
-      <c r="E48" s="3" t="inlineStr">
-        <is>
-          <t>FILE NAME VALIDATION</t>
-        </is>
-      </c>
-      <c r="F48" s="3" t="inlineStr">
-        <is>
-          <t>FILE NAME VALIDATION COMPLETED</t>
-        </is>
-      </c>
-    </row>
-    <row r="49">
-      <c r="A49" s="3" t="n">
-        <v>48</v>
-      </c>
-      <c r="B49" s="3" t="inlineStr">
-        <is>
-          <t>2024-10-01</t>
-        </is>
-      </c>
-      <c r="C49" s="3" t="inlineStr">
-        <is>
-          <t>wafer_28042024_031911.csv</t>
-        </is>
-      </c>
-      <c r="D49" s="3" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
-      </c>
-      <c r="E49" s="3" t="inlineStr">
-        <is>
-          <t>NUMBER OF COLUMNS VALIDATION</t>
-        </is>
-      </c>
-      <c r="F49" s="3" t="inlineStr">
-        <is>
-          <t>NUMBER OF COLUMNS VALIDATION COMPLETED</t>
-        </is>
-      </c>
-    </row>
-    <row r="50">
-      <c r="A50" s="3" t="n">
-        <v>49</v>
-      </c>
-      <c r="B50" s="3" t="inlineStr">
-        <is>
-          <t>2024-10-01</t>
-        </is>
-      </c>
-      <c r="C50" s="3" t="inlineStr">
-        <is>
-          <t>wafer_28042024_031911.csv</t>
-        </is>
-      </c>
-      <c r="D50" s="3" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
-      </c>
-      <c r="E50" s="3" t="inlineStr">
-        <is>
-          <t>COLUMNDATA_WHOLE_MISSING_VALIDATION</t>
-        </is>
-      </c>
-      <c r="F50" s="3" t="inlineStr">
-        <is>
-          <t>COLUMN DATA WHOLE MISSING VALIDATION COMPLETED</t>
-        </is>
-      </c>
-    </row>
-    <row r="51">
-      <c r="A51" s="3" t="n">
-        <v>50</v>
-      </c>
-      <c r="B51" s="3" t="inlineStr">
-        <is>
-          <t>2024-10-01</t>
-        </is>
-      </c>
-      <c r="C51" s="3" t="inlineStr">
-        <is>
-          <t>wafer_28042024_031911.csv</t>
-        </is>
-      </c>
-      <c r="D51" s="3" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
-      </c>
-      <c r="E51" s="3" t="inlineStr">
-        <is>
-          <t>COLUMN DATA VALIDATION</t>
-        </is>
-      </c>
-      <c r="F51" s="3" t="inlineStr">
-        <is>
-          <t>COLUMN DATA VALIDATION COMPLETED</t>
-        </is>
-      </c>
-    </row>
-    <row r="52">
-      <c r="A52" s="3" t="n">
-        <v>51</v>
-      </c>
-      <c r="B52" s="3" t="inlineStr">
-        <is>
-          <t>2024-10-01</t>
-        </is>
-      </c>
-      <c r="C52" s="3" t="inlineStr">
-        <is>
-          <t>wafer_29012024_050617.csv</t>
-        </is>
-      </c>
-      <c r="D52" s="3" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
-      </c>
-      <c r="E52" s="3" t="inlineStr">
-        <is>
-          <t>FILE NAME VALIDATION</t>
-        </is>
-      </c>
-      <c r="F52" s="3" t="inlineStr">
-        <is>
-          <t>FILE NAME VALIDATION COMPLETED</t>
-        </is>
-      </c>
-    </row>
-    <row r="53">
-      <c r="A53" s="3" t="n">
-        <v>52</v>
-      </c>
-      <c r="B53" s="3" t="inlineStr">
-        <is>
-          <t>2024-10-01</t>
-        </is>
-      </c>
-      <c r="C53" s="3" t="inlineStr">
-        <is>
-          <t>wafer_29012024_050617.csv</t>
-        </is>
-      </c>
-      <c r="D53" s="3" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
-      </c>
-      <c r="E53" s="3" t="inlineStr">
-        <is>
-          <t>NUMBER OF COLUMNS VALIDATION</t>
-        </is>
-      </c>
-      <c r="F53" s="3" t="inlineStr">
-        <is>
-          <t>NUMBER OF COLUMNS VALIDATION COMPLETED</t>
-        </is>
-      </c>
-    </row>
-    <row r="54">
-      <c r="A54" s="3" t="n">
-        <v>53</v>
-      </c>
-      <c r="B54" s="3" t="inlineStr">
-        <is>
-          <t>2024-10-01</t>
-        </is>
-      </c>
-      <c r="C54" s="3" t="inlineStr">
-        <is>
-          <t>wafer_29012024_050617.csv</t>
-        </is>
-      </c>
-      <c r="D54" s="3" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
-      </c>
-      <c r="E54" s="3" t="inlineStr">
-        <is>
-          <t>COLUMNDATA_WHOLE_MISSING_VALIDATION</t>
-        </is>
-      </c>
-      <c r="F54" s="3" t="inlineStr">
-        <is>
-          <t>COLUMN DATA WHOLE MISSING VALIDATION COMPLETED</t>
-        </is>
-      </c>
-    </row>
-    <row r="55">
-      <c r="A55" s="3" t="n">
-        <v>54</v>
-      </c>
-      <c r="B55" s="3" t="inlineStr">
-        <is>
-          <t>2024-10-01</t>
-        </is>
-      </c>
-      <c r="C55" s="3" t="inlineStr">
-        <is>
-          <t>wafer_29012024_050617.csv</t>
-        </is>
-      </c>
-      <c r="D55" s="3" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
-      </c>
-      <c r="E55" s="3" t="inlineStr">
-        <is>
-          <t>COLUMN DATA VALIDATION</t>
-        </is>
-      </c>
-      <c r="F55" s="3" t="inlineStr">
-        <is>
-          <t>COLUMN DATA VALIDATION COMPLETED</t>
-        </is>
-      </c>
-    </row>
-    <row r="56">
-      <c r="A56" s="3" t="n">
-        <v>55</v>
-      </c>
-      <c r="B56" s="3" t="inlineStr">
-        <is>
-          <t>2024-10-01</t>
-        </is>
-      </c>
-      <c r="C56" s="3" t="inlineStr">
-        <is>
-          <t>wafer_29012024_060756.csv</t>
-        </is>
-      </c>
-      <c r="D56" s="3" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
-      </c>
-      <c r="E56" s="3" t="inlineStr">
-        <is>
-          <t>FILE NAME VALIDATION</t>
-        </is>
-      </c>
-      <c r="F56" s="3" t="inlineStr">
-        <is>
-          <t>FILE NAME VALIDATION COMPLETED</t>
-        </is>
-      </c>
-    </row>
-    <row r="57">
-      <c r="A57" s="3" t="n">
-        <v>56</v>
-      </c>
-      <c r="B57" s="3" t="inlineStr">
-        <is>
-          <t>2024-10-01</t>
-        </is>
-      </c>
-      <c r="C57" s="3" t="inlineStr">
-        <is>
-          <t>wafer_29012024_060756.csv</t>
-        </is>
-      </c>
-      <c r="D57" s="3" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
-      </c>
-      <c r="E57" s="3" t="inlineStr">
-        <is>
-          <t>NUMBER OF COLUMNS VALIDATION</t>
-        </is>
-      </c>
-      <c r="F57" s="3" t="inlineStr">
-        <is>
-          <t>NUMBER OF COLUMNS VALIDATION COMPLETED</t>
-        </is>
-      </c>
-    </row>
-    <row r="58">
-      <c r="A58" s="3" t="n">
-        <v>57</v>
-      </c>
-      <c r="B58" s="3" t="inlineStr">
-        <is>
-          <t>2024-10-01</t>
-        </is>
-      </c>
-      <c r="C58" s="3" t="inlineStr">
-        <is>
-          <t>wafer_29012024_060756.csv</t>
-        </is>
-      </c>
-      <c r="D58" s="3" t="inlineStr">
-        <is>
-          <t>Failed</t>
-        </is>
-      </c>
-      <c r="E58" s="3" t="inlineStr">
-        <is>
-          <t>COLUMNDATA_WHOLE_MISSING_VALIDATION</t>
-        </is>
-      </c>
-      <c r="F58" s="3" t="inlineStr">
-        <is>
-          <t>COLUMN DATA WHOLE MISSING VALIDATION FAILED, MISMATCH COLUMN LIST:[{'Sensor_Name': 'Sensor-86', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-110', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-111', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-112', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-221', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-245', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-246', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-247', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-359', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-383', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-384', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-385', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-493', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-517', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-518', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-519', 'Column_Data': [100, 0]}]</t>
-        </is>
-      </c>
-    </row>
-    <row r="59">
-      <c r="A59" s="3" t="n">
-        <v>58</v>
-      </c>
-      <c r="B59" s="3" t="inlineStr">
-        <is>
-          <t>2024-10-01</t>
-        </is>
-      </c>
-      <c r="C59" s="3" t="inlineStr">
-        <is>
-          <t>wafer_31012024_090811.csv</t>
-        </is>
-      </c>
-      <c r="D59" s="3" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
-      </c>
-      <c r="E59" s="3" t="inlineStr">
-        <is>
-          <t>FILE NAME VALIDATION</t>
-        </is>
-      </c>
-      <c r="F59" s="3" t="inlineStr">
-        <is>
-          <t>FILE NAME VALIDATION COMPLETED</t>
-        </is>
-      </c>
-    </row>
-    <row r="60">
-      <c r="A60" s="3" t="n">
-        <v>59</v>
-      </c>
-      <c r="B60" s="3" t="inlineStr">
-        <is>
-          <t>2024-10-01</t>
-        </is>
-      </c>
-      <c r="C60" s="3" t="inlineStr">
-        <is>
-          <t>wafer_31012024_090811.csv</t>
-        </is>
-      </c>
-      <c r="D60" s="3" t="inlineStr">
-        <is>
-          <t>Passed</t>
-        </is>
-      </c>
-      <c r="E60" s="3" t="inlineStr">
-        <is>
-          <t>NUMBER OF COLUMNS VALIDATION</t>
-        </is>
-      </c>
-      <c r="F60" s="3" t="inlineStr">
-        <is>
-          <t>NUMBER OF COLUMNS VALIDATION COMPLETED</t>
-        </is>
-      </c>
-    </row>
-    <row r="61">
-      <c r="A61" s="3" t="n">
-        <v>60</v>
-      </c>
-      <c r="B61" s="3" t="inlineStr">
-        <is>
-          <t>2024-10-01</t>
-        </is>
-      </c>
-      <c r="C61" s="3" t="inlineStr">
-        <is>
-          <t>wafer_31012024_090811.csv</t>
-        </is>
-      </c>
-      <c r="D61" s="3" t="inlineStr">
-        <is>
-          <t>Failed</t>
-        </is>
-      </c>
-      <c r="E61" s="3" t="inlineStr">
-        <is>
-          <t>COLUMNDATA_WHOLE_MISSING_VALIDATION</t>
-        </is>
-      </c>
-      <c r="F61" s="3" t="inlineStr">
-        <is>
-          <t>COLUMN DATA WHOLE MISSING VALIDATION FAILED, MISMATCH COLUMN LIST:[{'Sensor_Name': 'Sensor-86', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-110', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-111', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-112', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-221', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-245', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-246', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-247', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-359', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-383', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-384', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-385', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-493', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-517', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-518', 'Column_Data': [100, 0]}, {'Sensor_Name': 'Sensor-519', 'Column_Data': [100, 0]}]</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
clean the code and testing completed
</commit_message>
<xml_diff>
--- a/data/dashboard_data/prediction_validation_logs.xlsx
+++ b/data/dashboard_data/prediction_validation_logs.xlsx
@@ -493,7 +493,7 @@
       </c>
       <c r="B2" s="3" t="inlineStr">
         <is>
-          <t>2024-10-29</t>
+          <t>2024-11-02</t>
         </is>
       </c>
       <c r="C2" s="3" t="inlineStr">
@@ -523,7 +523,7 @@
       </c>
       <c r="B3" s="3" t="inlineStr">
         <is>
-          <t>2024-10-29</t>
+          <t>2024-11-02</t>
         </is>
       </c>
       <c r="C3" s="3" t="inlineStr">
@@ -553,7 +553,7 @@
       </c>
       <c r="B4" s="3" t="inlineStr">
         <is>
-          <t>2024-10-29</t>
+          <t>2024-11-02</t>
         </is>
       </c>
       <c r="C4" s="3" t="inlineStr">
@@ -583,7 +583,7 @@
       </c>
       <c r="B5" s="3" t="inlineStr">
         <is>
-          <t>2024-10-29</t>
+          <t>2024-11-02</t>
         </is>
       </c>
       <c r="C5" s="3" t="inlineStr">
@@ -613,7 +613,7 @@
       </c>
       <c r="B6" s="3" t="inlineStr">
         <is>
-          <t>2024-10-29</t>
+          <t>2024-11-02</t>
         </is>
       </c>
       <c r="C6" s="3" t="inlineStr">
@@ -643,7 +643,7 @@
       </c>
       <c r="B7" s="3" t="inlineStr">
         <is>
-          <t>2024-10-29</t>
+          <t>2024-11-02</t>
         </is>
       </c>
       <c r="C7" s="3" t="inlineStr">
@@ -673,7 +673,7 @@
       </c>
       <c r="B8" s="3" t="inlineStr">
         <is>
-          <t>2024-10-29</t>
+          <t>2024-11-02</t>
         </is>
       </c>
       <c r="C8" s="3" t="inlineStr">
@@ -703,7 +703,7 @@
       </c>
       <c r="B9" s="3" t="inlineStr">
         <is>
-          <t>2024-10-29</t>
+          <t>2024-11-02</t>
         </is>
       </c>
       <c r="C9" s="3" t="inlineStr">
@@ -733,7 +733,7 @@
       </c>
       <c r="B10" s="3" t="inlineStr">
         <is>
-          <t>2024-10-29</t>
+          <t>2024-11-02</t>
         </is>
       </c>
       <c r="C10" s="3" t="inlineStr">
@@ -763,7 +763,7 @@
       </c>
       <c r="B11" s="3" t="inlineStr">
         <is>
-          <t>2024-10-29</t>
+          <t>2024-11-02</t>
         </is>
       </c>
       <c r="C11" s="3" t="inlineStr">
@@ -793,7 +793,7 @@
       </c>
       <c r="B12" s="3" t="inlineStr">
         <is>
-          <t>2024-10-29</t>
+          <t>2024-11-02</t>
         </is>
       </c>
       <c r="C12" s="3" t="inlineStr">
@@ -823,7 +823,7 @@
       </c>
       <c r="B13" s="3" t="inlineStr">
         <is>
-          <t>2024-10-29</t>
+          <t>2024-11-02</t>
         </is>
       </c>
       <c r="C13" s="3" t="inlineStr">
@@ -853,7 +853,7 @@
       </c>
       <c r="B14" s="3" t="inlineStr">
         <is>
-          <t>2024-10-29</t>
+          <t>2024-11-02</t>
         </is>
       </c>
       <c r="C14" s="3" t="inlineStr">
@@ -883,7 +883,7 @@
       </c>
       <c r="B15" s="3" t="inlineStr">
         <is>
-          <t>2024-10-29</t>
+          <t>2024-11-02</t>
         </is>
       </c>
       <c r="C15" s="3" t="inlineStr">
@@ -913,7 +913,7 @@
       </c>
       <c r="B16" s="3" t="inlineStr">
         <is>
-          <t>2024-10-29</t>
+          <t>2024-11-02</t>
         </is>
       </c>
       <c r="C16" s="3" t="inlineStr">
@@ -943,7 +943,7 @@
       </c>
       <c r="B17" s="3" t="inlineStr">
         <is>
-          <t>2024-10-29</t>
+          <t>2024-11-02</t>
         </is>
       </c>
       <c r="C17" s="3" t="inlineStr">
@@ -973,7 +973,7 @@
       </c>
       <c r="B18" s="3" t="inlineStr">
         <is>
-          <t>2024-10-29</t>
+          <t>2024-11-02</t>
         </is>
       </c>
       <c r="C18" s="3" t="inlineStr">
@@ -1003,7 +1003,7 @@
       </c>
       <c r="B19" s="3" t="inlineStr">
         <is>
-          <t>2024-10-29</t>
+          <t>2024-11-02</t>
         </is>
       </c>
       <c r="C19" s="3" t="inlineStr">
@@ -1033,7 +1033,7 @@
       </c>
       <c r="B20" s="3" t="inlineStr">
         <is>
-          <t>2024-10-29</t>
+          <t>2024-11-02</t>
         </is>
       </c>
       <c r="C20" s="3" t="inlineStr">
@@ -1063,7 +1063,7 @@
       </c>
       <c r="B21" s="3" t="inlineStr">
         <is>
-          <t>2024-10-29</t>
+          <t>2024-11-02</t>
         </is>
       </c>
       <c r="C21" s="3" t="inlineStr">
@@ -1093,7 +1093,7 @@
       </c>
       <c r="B22" s="3" t="inlineStr">
         <is>
-          <t>2024-10-29</t>
+          <t>2024-11-02</t>
         </is>
       </c>
       <c r="C22" s="3" t="inlineStr">
@@ -1123,7 +1123,7 @@
       </c>
       <c r="B23" s="3" t="inlineStr">
         <is>
-          <t>2024-10-29</t>
+          <t>2024-11-02</t>
         </is>
       </c>
       <c r="C23" s="3" t="inlineStr">
@@ -1153,7 +1153,7 @@
       </c>
       <c r="B24" s="3" t="inlineStr">
         <is>
-          <t>2024-10-29</t>
+          <t>2024-11-02</t>
         </is>
       </c>
       <c r="C24" s="3" t="inlineStr">
@@ -1183,7 +1183,7 @@
       </c>
       <c r="B25" s="3" t="inlineStr">
         <is>
-          <t>2024-10-29</t>
+          <t>2024-11-02</t>
         </is>
       </c>
       <c r="C25" s="3" t="inlineStr">
@@ -1213,7 +1213,7 @@
       </c>
       <c r="B26" s="3" t="inlineStr">
         <is>
-          <t>2024-10-29</t>
+          <t>2024-11-02</t>
         </is>
       </c>
       <c r="C26" s="3" t="inlineStr">
@@ -1243,7 +1243,7 @@
       </c>
       <c r="B27" s="3" t="inlineStr">
         <is>
-          <t>2024-10-29</t>
+          <t>2024-11-02</t>
         </is>
       </c>
       <c r="C27" s="3" t="inlineStr">
@@ -1273,7 +1273,7 @@
       </c>
       <c r="B28" s="3" t="inlineStr">
         <is>
-          <t>2024-10-29</t>
+          <t>2024-11-02</t>
         </is>
       </c>
       <c r="C28" s="3" t="inlineStr">
@@ -1303,7 +1303,7 @@
       </c>
       <c r="B29" s="3" t="inlineStr">
         <is>
-          <t>2024-10-29</t>
+          <t>2024-11-02</t>
         </is>
       </c>
       <c r="C29" s="3" t="inlineStr">
@@ -1333,7 +1333,7 @@
       </c>
       <c r="B30" s="3" t="inlineStr">
         <is>
-          <t>2024-10-29</t>
+          <t>2024-11-02</t>
         </is>
       </c>
       <c r="C30" s="3" t="inlineStr">
@@ -1363,7 +1363,7 @@
       </c>
       <c r="B31" s="3" t="inlineStr">
         <is>
-          <t>2024-10-29</t>
+          <t>2024-11-02</t>
         </is>
       </c>
       <c r="C31" s="3" t="inlineStr">
@@ -1393,7 +1393,7 @@
       </c>
       <c r="B32" s="3" t="inlineStr">
         <is>
-          <t>2024-10-29</t>
+          <t>2024-11-02</t>
         </is>
       </c>
       <c r="C32" s="3" t="inlineStr">
@@ -1423,7 +1423,7 @@
       </c>
       <c r="B33" s="3" t="inlineStr">
         <is>
-          <t>2024-10-29</t>
+          <t>2024-11-02</t>
         </is>
       </c>
       <c r="C33" s="3" t="inlineStr">
@@ -1453,7 +1453,7 @@
       </c>
       <c r="B34" s="3" t="inlineStr">
         <is>
-          <t>2024-10-29</t>
+          <t>2024-11-02</t>
         </is>
       </c>
       <c r="C34" s="3" t="inlineStr">
@@ -1483,7 +1483,7 @@
       </c>
       <c r="B35" s="3" t="inlineStr">
         <is>
-          <t>2024-10-29</t>
+          <t>2024-11-02</t>
         </is>
       </c>
       <c r="C35" s="3" t="inlineStr">
@@ -1513,7 +1513,7 @@
       </c>
       <c r="B36" s="3" t="inlineStr">
         <is>
-          <t>2024-10-29</t>
+          <t>2024-11-02</t>
         </is>
       </c>
       <c r="C36" s="3" t="inlineStr">
@@ -1543,7 +1543,7 @@
       </c>
       <c r="B37" s="3" t="inlineStr">
         <is>
-          <t>2024-10-29</t>
+          <t>2024-11-02</t>
         </is>
       </c>
       <c r="C37" s="3" t="inlineStr">
@@ -1573,7 +1573,7 @@
       </c>
       <c r="B38" s="3" t="inlineStr">
         <is>
-          <t>2024-10-29</t>
+          <t>2024-11-02</t>
         </is>
       </c>
       <c r="C38" s="3" t="inlineStr">
@@ -1603,7 +1603,7 @@
       </c>
       <c r="B39" s="3" t="inlineStr">
         <is>
-          <t>2024-10-29</t>
+          <t>2024-11-02</t>
         </is>
       </c>
       <c r="C39" s="3" t="inlineStr">
@@ -1633,7 +1633,7 @@
       </c>
       <c r="B40" s="3" t="inlineStr">
         <is>
-          <t>2024-10-29</t>
+          <t>2024-11-02</t>
         </is>
       </c>
       <c r="C40" s="3" t="inlineStr">
@@ -1663,7 +1663,7 @@
       </c>
       <c r="B41" s="3" t="inlineStr">
         <is>
-          <t>2024-10-29</t>
+          <t>2024-11-02</t>
         </is>
       </c>
       <c r="C41" s="3" t="inlineStr">
@@ -1693,7 +1693,7 @@
       </c>
       <c r="B42" s="3" t="inlineStr">
         <is>
-          <t>2024-10-29</t>
+          <t>2024-11-02</t>
         </is>
       </c>
       <c r="C42" s="3" t="inlineStr">
@@ -1723,7 +1723,7 @@
       </c>
       <c r="B43" s="3" t="inlineStr">
         <is>
-          <t>2024-10-29</t>
+          <t>2024-11-02</t>
         </is>
       </c>
       <c r="C43" s="3" t="inlineStr">

</xml_diff>

<commit_message>
aws cloudwatch added and tested
</commit_message>
<xml_diff>
--- a/data/dashboard_data/prediction_validation_logs.xlsx
+++ b/data/dashboard_data/prediction_validation_logs.xlsx
@@ -493,7 +493,7 @@
       </c>
       <c r="B2" s="3" t="inlineStr">
         <is>
-          <t>2024-11-02</t>
+          <t>2024-11-09</t>
         </is>
       </c>
       <c r="C2" s="3" t="inlineStr">
@@ -523,7 +523,7 @@
       </c>
       <c r="B3" s="3" t="inlineStr">
         <is>
-          <t>2024-11-02</t>
+          <t>2024-11-09</t>
         </is>
       </c>
       <c r="C3" s="3" t="inlineStr">
@@ -553,7 +553,7 @@
       </c>
       <c r="B4" s="3" t="inlineStr">
         <is>
-          <t>2024-11-02</t>
+          <t>2024-11-09</t>
         </is>
       </c>
       <c r="C4" s="3" t="inlineStr">
@@ -583,7 +583,7 @@
       </c>
       <c r="B5" s="3" t="inlineStr">
         <is>
-          <t>2024-11-02</t>
+          <t>2024-11-09</t>
         </is>
       </c>
       <c r="C5" s="3" t="inlineStr">
@@ -613,7 +613,7 @@
       </c>
       <c r="B6" s="3" t="inlineStr">
         <is>
-          <t>2024-11-02</t>
+          <t>2024-11-09</t>
         </is>
       </c>
       <c r="C6" s="3" t="inlineStr">
@@ -643,7 +643,7 @@
       </c>
       <c r="B7" s="3" t="inlineStr">
         <is>
-          <t>2024-11-02</t>
+          <t>2024-11-09</t>
         </is>
       </c>
       <c r="C7" s="3" t="inlineStr">
@@ -673,7 +673,7 @@
       </c>
       <c r="B8" s="3" t="inlineStr">
         <is>
-          <t>2024-11-02</t>
+          <t>2024-11-09</t>
         </is>
       </c>
       <c r="C8" s="3" t="inlineStr">
@@ -703,7 +703,7 @@
       </c>
       <c r="B9" s="3" t="inlineStr">
         <is>
-          <t>2024-11-02</t>
+          <t>2024-11-09</t>
         </is>
       </c>
       <c r="C9" s="3" t="inlineStr">
@@ -733,7 +733,7 @@
       </c>
       <c r="B10" s="3" t="inlineStr">
         <is>
-          <t>2024-11-02</t>
+          <t>2024-11-09</t>
         </is>
       </c>
       <c r="C10" s="3" t="inlineStr">
@@ -763,7 +763,7 @@
       </c>
       <c r="B11" s="3" t="inlineStr">
         <is>
-          <t>2024-11-02</t>
+          <t>2024-11-09</t>
         </is>
       </c>
       <c r="C11" s="3" t="inlineStr">
@@ -793,7 +793,7 @@
       </c>
       <c r="B12" s="3" t="inlineStr">
         <is>
-          <t>2024-11-02</t>
+          <t>2024-11-09</t>
         </is>
       </c>
       <c r="C12" s="3" t="inlineStr">
@@ -823,7 +823,7 @@
       </c>
       <c r="B13" s="3" t="inlineStr">
         <is>
-          <t>2024-11-02</t>
+          <t>2024-11-09</t>
         </is>
       </c>
       <c r="C13" s="3" t="inlineStr">
@@ -853,7 +853,7 @@
       </c>
       <c r="B14" s="3" t="inlineStr">
         <is>
-          <t>2024-11-02</t>
+          <t>2024-11-09</t>
         </is>
       </c>
       <c r="C14" s="3" t="inlineStr">
@@ -883,7 +883,7 @@
       </c>
       <c r="B15" s="3" t="inlineStr">
         <is>
-          <t>2024-11-02</t>
+          <t>2024-11-09</t>
         </is>
       </c>
       <c r="C15" s="3" t="inlineStr">
@@ -913,7 +913,7 @@
       </c>
       <c r="B16" s="3" t="inlineStr">
         <is>
-          <t>2024-11-02</t>
+          <t>2024-11-09</t>
         </is>
       </c>
       <c r="C16" s="3" t="inlineStr">
@@ -943,7 +943,7 @@
       </c>
       <c r="B17" s="3" t="inlineStr">
         <is>
-          <t>2024-11-02</t>
+          <t>2024-11-09</t>
         </is>
       </c>
       <c r="C17" s="3" t="inlineStr">
@@ -973,7 +973,7 @@
       </c>
       <c r="B18" s="3" t="inlineStr">
         <is>
-          <t>2024-11-02</t>
+          <t>2024-11-09</t>
         </is>
       </c>
       <c r="C18" s="3" t="inlineStr">
@@ -1003,7 +1003,7 @@
       </c>
       <c r="B19" s="3" t="inlineStr">
         <is>
-          <t>2024-11-02</t>
+          <t>2024-11-09</t>
         </is>
       </c>
       <c r="C19" s="3" t="inlineStr">
@@ -1033,7 +1033,7 @@
       </c>
       <c r="B20" s="3" t="inlineStr">
         <is>
-          <t>2024-11-02</t>
+          <t>2024-11-09</t>
         </is>
       </c>
       <c r="C20" s="3" t="inlineStr">
@@ -1063,7 +1063,7 @@
       </c>
       <c r="B21" s="3" t="inlineStr">
         <is>
-          <t>2024-11-02</t>
+          <t>2024-11-09</t>
         </is>
       </c>
       <c r="C21" s="3" t="inlineStr">
@@ -1093,7 +1093,7 @@
       </c>
       <c r="B22" s="3" t="inlineStr">
         <is>
-          <t>2024-11-02</t>
+          <t>2024-11-09</t>
         </is>
       </c>
       <c r="C22" s="3" t="inlineStr">
@@ -1123,7 +1123,7 @@
       </c>
       <c r="B23" s="3" t="inlineStr">
         <is>
-          <t>2024-11-02</t>
+          <t>2024-11-09</t>
         </is>
       </c>
       <c r="C23" s="3" t="inlineStr">
@@ -1153,7 +1153,7 @@
       </c>
       <c r="B24" s="3" t="inlineStr">
         <is>
-          <t>2024-11-02</t>
+          <t>2024-11-09</t>
         </is>
       </c>
       <c r="C24" s="3" t="inlineStr">
@@ -1183,7 +1183,7 @@
       </c>
       <c r="B25" s="3" t="inlineStr">
         <is>
-          <t>2024-11-02</t>
+          <t>2024-11-09</t>
         </is>
       </c>
       <c r="C25" s="3" t="inlineStr">
@@ -1213,7 +1213,7 @@
       </c>
       <c r="B26" s="3" t="inlineStr">
         <is>
-          <t>2024-11-02</t>
+          <t>2024-11-09</t>
         </is>
       </c>
       <c r="C26" s="3" t="inlineStr">
@@ -1243,7 +1243,7 @@
       </c>
       <c r="B27" s="3" t="inlineStr">
         <is>
-          <t>2024-11-02</t>
+          <t>2024-11-09</t>
         </is>
       </c>
       <c r="C27" s="3" t="inlineStr">
@@ -1273,7 +1273,7 @@
       </c>
       <c r="B28" s="3" t="inlineStr">
         <is>
-          <t>2024-11-02</t>
+          <t>2024-11-09</t>
         </is>
       </c>
       <c r="C28" s="3" t="inlineStr">
@@ -1303,7 +1303,7 @@
       </c>
       <c r="B29" s="3" t="inlineStr">
         <is>
-          <t>2024-11-02</t>
+          <t>2024-11-09</t>
         </is>
       </c>
       <c r="C29" s="3" t="inlineStr">
@@ -1333,7 +1333,7 @@
       </c>
       <c r="B30" s="3" t="inlineStr">
         <is>
-          <t>2024-11-02</t>
+          <t>2024-11-09</t>
         </is>
       </c>
       <c r="C30" s="3" t="inlineStr">
@@ -1363,7 +1363,7 @@
       </c>
       <c r="B31" s="3" t="inlineStr">
         <is>
-          <t>2024-11-02</t>
+          <t>2024-11-09</t>
         </is>
       </c>
       <c r="C31" s="3" t="inlineStr">
@@ -1393,7 +1393,7 @@
       </c>
       <c r="B32" s="3" t="inlineStr">
         <is>
-          <t>2024-11-02</t>
+          <t>2024-11-09</t>
         </is>
       </c>
       <c r="C32" s="3" t="inlineStr">
@@ -1423,7 +1423,7 @@
       </c>
       <c r="B33" s="3" t="inlineStr">
         <is>
-          <t>2024-11-02</t>
+          <t>2024-11-09</t>
         </is>
       </c>
       <c r="C33" s="3" t="inlineStr">
@@ -1453,7 +1453,7 @@
       </c>
       <c r="B34" s="3" t="inlineStr">
         <is>
-          <t>2024-11-02</t>
+          <t>2024-11-09</t>
         </is>
       </c>
       <c r="C34" s="3" t="inlineStr">
@@ -1483,7 +1483,7 @@
       </c>
       <c r="B35" s="3" t="inlineStr">
         <is>
-          <t>2024-11-02</t>
+          <t>2024-11-09</t>
         </is>
       </c>
       <c r="C35" s="3" t="inlineStr">
@@ -1513,7 +1513,7 @@
       </c>
       <c r="B36" s="3" t="inlineStr">
         <is>
-          <t>2024-11-02</t>
+          <t>2024-11-09</t>
         </is>
       </c>
       <c r="C36" s="3" t="inlineStr">
@@ -1543,7 +1543,7 @@
       </c>
       <c r="B37" s="3" t="inlineStr">
         <is>
-          <t>2024-11-02</t>
+          <t>2024-11-09</t>
         </is>
       </c>
       <c r="C37" s="3" t="inlineStr">
@@ -1573,7 +1573,7 @@
       </c>
       <c r="B38" s="3" t="inlineStr">
         <is>
-          <t>2024-11-02</t>
+          <t>2024-11-09</t>
         </is>
       </c>
       <c r="C38" s="3" t="inlineStr">
@@ -1603,7 +1603,7 @@
       </c>
       <c r="B39" s="3" t="inlineStr">
         <is>
-          <t>2024-11-02</t>
+          <t>2024-11-09</t>
         </is>
       </c>
       <c r="C39" s="3" t="inlineStr">
@@ -1633,7 +1633,7 @@
       </c>
       <c r="B40" s="3" t="inlineStr">
         <is>
-          <t>2024-11-02</t>
+          <t>2024-11-09</t>
         </is>
       </c>
       <c r="C40" s="3" t="inlineStr">
@@ -1663,7 +1663,7 @@
       </c>
       <c r="B41" s="3" t="inlineStr">
         <is>
-          <t>2024-11-02</t>
+          <t>2024-11-09</t>
         </is>
       </c>
       <c r="C41" s="3" t="inlineStr">
@@ -1693,7 +1693,7 @@
       </c>
       <c r="B42" s="3" t="inlineStr">
         <is>
-          <t>2024-11-02</t>
+          <t>2024-11-09</t>
         </is>
       </c>
       <c r="C42" s="3" t="inlineStr">
@@ -1723,7 +1723,7 @@
       </c>
       <c r="B43" s="3" t="inlineStr">
         <is>
-          <t>2024-11-02</t>
+          <t>2024-11-09</t>
         </is>
       </c>
       <c r="C43" s="3" t="inlineStr">

</xml_diff>

<commit_message>
demo training for video creation
</commit_message>
<xml_diff>
--- a/data/dashboard_data/prediction_validation_logs.xlsx
+++ b/data/dashboard_data/prediction_validation_logs.xlsx
@@ -493,7 +493,7 @@
       </c>
       <c r="B2" s="3" t="inlineStr">
         <is>
-          <t>2024-11-09</t>
+          <t>2024-11-18</t>
         </is>
       </c>
       <c r="C2" s="3" t="inlineStr">
@@ -523,7 +523,7 @@
       </c>
       <c r="B3" s="3" t="inlineStr">
         <is>
-          <t>2024-11-09</t>
+          <t>2024-11-18</t>
         </is>
       </c>
       <c r="C3" s="3" t="inlineStr">
@@ -553,7 +553,7 @@
       </c>
       <c r="B4" s="3" t="inlineStr">
         <is>
-          <t>2024-11-09</t>
+          <t>2024-11-18</t>
         </is>
       </c>
       <c r="C4" s="3" t="inlineStr">
@@ -583,7 +583,7 @@
       </c>
       <c r="B5" s="3" t="inlineStr">
         <is>
-          <t>2024-11-09</t>
+          <t>2024-11-18</t>
         </is>
       </c>
       <c r="C5" s="3" t="inlineStr">
@@ -613,7 +613,7 @@
       </c>
       <c r="B6" s="3" t="inlineStr">
         <is>
-          <t>2024-11-09</t>
+          <t>2024-11-18</t>
         </is>
       </c>
       <c r="C6" s="3" t="inlineStr">
@@ -643,7 +643,7 @@
       </c>
       <c r="B7" s="3" t="inlineStr">
         <is>
-          <t>2024-11-09</t>
+          <t>2024-11-18</t>
         </is>
       </c>
       <c r="C7" s="3" t="inlineStr">
@@ -673,7 +673,7 @@
       </c>
       <c r="B8" s="3" t="inlineStr">
         <is>
-          <t>2024-11-09</t>
+          <t>2024-11-18</t>
         </is>
       </c>
       <c r="C8" s="3" t="inlineStr">
@@ -703,7 +703,7 @@
       </c>
       <c r="B9" s="3" t="inlineStr">
         <is>
-          <t>2024-11-09</t>
+          <t>2024-11-18</t>
         </is>
       </c>
       <c r="C9" s="3" t="inlineStr">
@@ -733,7 +733,7 @@
       </c>
       <c r="B10" s="3" t="inlineStr">
         <is>
-          <t>2024-11-09</t>
+          <t>2024-11-18</t>
         </is>
       </c>
       <c r="C10" s="3" t="inlineStr">
@@ -763,7 +763,7 @@
       </c>
       <c r="B11" s="3" t="inlineStr">
         <is>
-          <t>2024-11-09</t>
+          <t>2024-11-18</t>
         </is>
       </c>
       <c r="C11" s="3" t="inlineStr">
@@ -793,7 +793,7 @@
       </c>
       <c r="B12" s="3" t="inlineStr">
         <is>
-          <t>2024-11-09</t>
+          <t>2024-11-18</t>
         </is>
       </c>
       <c r="C12" s="3" t="inlineStr">
@@ -823,7 +823,7 @@
       </c>
       <c r="B13" s="3" t="inlineStr">
         <is>
-          <t>2024-11-09</t>
+          <t>2024-11-18</t>
         </is>
       </c>
       <c r="C13" s="3" t="inlineStr">
@@ -853,7 +853,7 @@
       </c>
       <c r="B14" s="3" t="inlineStr">
         <is>
-          <t>2024-11-09</t>
+          <t>2024-11-18</t>
         </is>
       </c>
       <c r="C14" s="3" t="inlineStr">
@@ -883,7 +883,7 @@
       </c>
       <c r="B15" s="3" t="inlineStr">
         <is>
-          <t>2024-11-09</t>
+          <t>2024-11-18</t>
         </is>
       </c>
       <c r="C15" s="3" t="inlineStr">
@@ -913,7 +913,7 @@
       </c>
       <c r="B16" s="3" t="inlineStr">
         <is>
-          <t>2024-11-09</t>
+          <t>2024-11-18</t>
         </is>
       </c>
       <c r="C16" s="3" t="inlineStr">
@@ -943,7 +943,7 @@
       </c>
       <c r="B17" s="3" t="inlineStr">
         <is>
-          <t>2024-11-09</t>
+          <t>2024-11-18</t>
         </is>
       </c>
       <c r="C17" s="3" t="inlineStr">
@@ -973,7 +973,7 @@
       </c>
       <c r="B18" s="3" t="inlineStr">
         <is>
-          <t>2024-11-09</t>
+          <t>2024-11-18</t>
         </is>
       </c>
       <c r="C18" s="3" t="inlineStr">
@@ -1003,7 +1003,7 @@
       </c>
       <c r="B19" s="3" t="inlineStr">
         <is>
-          <t>2024-11-09</t>
+          <t>2024-11-18</t>
         </is>
       </c>
       <c r="C19" s="3" t="inlineStr">
@@ -1033,7 +1033,7 @@
       </c>
       <c r="B20" s="3" t="inlineStr">
         <is>
-          <t>2024-11-09</t>
+          <t>2024-11-18</t>
         </is>
       </c>
       <c r="C20" s="3" t="inlineStr">
@@ -1063,7 +1063,7 @@
       </c>
       <c r="B21" s="3" t="inlineStr">
         <is>
-          <t>2024-11-09</t>
+          <t>2024-11-18</t>
         </is>
       </c>
       <c r="C21" s="3" t="inlineStr">
@@ -1093,7 +1093,7 @@
       </c>
       <c r="B22" s="3" t="inlineStr">
         <is>
-          <t>2024-11-09</t>
+          <t>2024-11-18</t>
         </is>
       </c>
       <c r="C22" s="3" t="inlineStr">
@@ -1123,7 +1123,7 @@
       </c>
       <c r="B23" s="3" t="inlineStr">
         <is>
-          <t>2024-11-09</t>
+          <t>2024-11-18</t>
         </is>
       </c>
       <c r="C23" s="3" t="inlineStr">
@@ -1153,7 +1153,7 @@
       </c>
       <c r="B24" s="3" t="inlineStr">
         <is>
-          <t>2024-11-09</t>
+          <t>2024-11-18</t>
         </is>
       </c>
       <c r="C24" s="3" t="inlineStr">
@@ -1183,7 +1183,7 @@
       </c>
       <c r="B25" s="3" t="inlineStr">
         <is>
-          <t>2024-11-09</t>
+          <t>2024-11-18</t>
         </is>
       </c>
       <c r="C25" s="3" t="inlineStr">
@@ -1213,7 +1213,7 @@
       </c>
       <c r="B26" s="3" t="inlineStr">
         <is>
-          <t>2024-11-09</t>
+          <t>2024-11-18</t>
         </is>
       </c>
       <c r="C26" s="3" t="inlineStr">
@@ -1243,7 +1243,7 @@
       </c>
       <c r="B27" s="3" t="inlineStr">
         <is>
-          <t>2024-11-09</t>
+          <t>2024-11-18</t>
         </is>
       </c>
       <c r="C27" s="3" t="inlineStr">
@@ -1273,7 +1273,7 @@
       </c>
       <c r="B28" s="3" t="inlineStr">
         <is>
-          <t>2024-11-09</t>
+          <t>2024-11-18</t>
         </is>
       </c>
       <c r="C28" s="3" t="inlineStr">
@@ -1303,7 +1303,7 @@
       </c>
       <c r="B29" s="3" t="inlineStr">
         <is>
-          <t>2024-11-09</t>
+          <t>2024-11-18</t>
         </is>
       </c>
       <c r="C29" s="3" t="inlineStr">
@@ -1333,7 +1333,7 @@
       </c>
       <c r="B30" s="3" t="inlineStr">
         <is>
-          <t>2024-11-09</t>
+          <t>2024-11-18</t>
         </is>
       </c>
       <c r="C30" s="3" t="inlineStr">
@@ -1363,7 +1363,7 @@
       </c>
       <c r="B31" s="3" t="inlineStr">
         <is>
-          <t>2024-11-09</t>
+          <t>2024-11-18</t>
         </is>
       </c>
       <c r="C31" s="3" t="inlineStr">
@@ -1393,7 +1393,7 @@
       </c>
       <c r="B32" s="3" t="inlineStr">
         <is>
-          <t>2024-11-09</t>
+          <t>2024-11-18</t>
         </is>
       </c>
       <c r="C32" s="3" t="inlineStr">
@@ -1423,7 +1423,7 @@
       </c>
       <c r="B33" s="3" t="inlineStr">
         <is>
-          <t>2024-11-09</t>
+          <t>2024-11-18</t>
         </is>
       </c>
       <c r="C33" s="3" t="inlineStr">
@@ -1453,7 +1453,7 @@
       </c>
       <c r="B34" s="3" t="inlineStr">
         <is>
-          <t>2024-11-09</t>
+          <t>2024-11-18</t>
         </is>
       </c>
       <c r="C34" s="3" t="inlineStr">
@@ -1483,7 +1483,7 @@
       </c>
       <c r="B35" s="3" t="inlineStr">
         <is>
-          <t>2024-11-09</t>
+          <t>2024-11-18</t>
         </is>
       </c>
       <c r="C35" s="3" t="inlineStr">
@@ -1513,7 +1513,7 @@
       </c>
       <c r="B36" s="3" t="inlineStr">
         <is>
-          <t>2024-11-09</t>
+          <t>2024-11-18</t>
         </is>
       </c>
       <c r="C36" s="3" t="inlineStr">
@@ -1543,7 +1543,7 @@
       </c>
       <c r="B37" s="3" t="inlineStr">
         <is>
-          <t>2024-11-09</t>
+          <t>2024-11-18</t>
         </is>
       </c>
       <c r="C37" s="3" t="inlineStr">
@@ -1573,7 +1573,7 @@
       </c>
       <c r="B38" s="3" t="inlineStr">
         <is>
-          <t>2024-11-09</t>
+          <t>2024-11-18</t>
         </is>
       </c>
       <c r="C38" s="3" t="inlineStr">
@@ -1603,7 +1603,7 @@
       </c>
       <c r="B39" s="3" t="inlineStr">
         <is>
-          <t>2024-11-09</t>
+          <t>2024-11-18</t>
         </is>
       </c>
       <c r="C39" s="3" t="inlineStr">
@@ -1633,7 +1633,7 @@
       </c>
       <c r="B40" s="3" t="inlineStr">
         <is>
-          <t>2024-11-09</t>
+          <t>2024-11-18</t>
         </is>
       </c>
       <c r="C40" s="3" t="inlineStr">
@@ -1663,7 +1663,7 @@
       </c>
       <c r="B41" s="3" t="inlineStr">
         <is>
-          <t>2024-11-09</t>
+          <t>2024-11-18</t>
         </is>
       </c>
       <c r="C41" s="3" t="inlineStr">
@@ -1693,7 +1693,7 @@
       </c>
       <c r="B42" s="3" t="inlineStr">
         <is>
-          <t>2024-11-09</t>
+          <t>2024-11-18</t>
         </is>
       </c>
       <c r="C42" s="3" t="inlineStr">
@@ -1723,7 +1723,7 @@
       </c>
       <c r="B43" s="3" t="inlineStr">
         <is>
-          <t>2024-11-09</t>
+          <t>2024-11-18</t>
         </is>
       </c>
       <c r="C43" s="3" t="inlineStr">

</xml_diff>